<commit_message>
Begin entering Annual Reports
</commit_message>
<xml_diff>
--- a/£HLMA.xlsx
+++ b/£HLMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2522E6-1932-4531-9E05-15CFD186AF44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCEC658-60C6-4427-8114-C84A3E5A4D1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28470" windowHeight="11790" activeTab="1" xr2:uid="{1821E3F4-C005-474E-95BC-C5AE66A060FF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="109">
   <si>
     <t>£HLMA</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -358,9 +361,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="175" formatCode="0.0\x"/>
+    <numFmt numFmtId="165" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,6 +425,29 @@
       <i/>
       <sz val="10"/>
       <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -563,21 +589,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -604,18 +621,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -639,12 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -665,33 +664,69 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="11" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="11" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="175" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -793,8 +828,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -809,8 +844,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7639050" y="19050"/>
-          <a:ext cx="0" cy="11544300"/>
+          <a:off x="9096375" y="19050"/>
+          <a:ext cx="0" cy="17259300"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -843,8 +878,8 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -859,8 +894,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13115925" y="0"/>
-          <a:ext cx="0" cy="11544300"/>
+          <a:off x="14573250" y="0"/>
+          <a:ext cx="0" cy="17878425"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1186,7 +1221,7 @@
   <dimension ref="B2:S38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="C29" sqref="C29:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1215,699 +1250,699 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="G5" s="5" t="s">
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="G5" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="7"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="63"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="4">
         <v>22.55</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="16"/>
+      <c r="D6" s="7"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="13"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <f>'Financial Model'!M16</f>
         <v>378.2</v>
       </c>
-      <c r="D7" s="10" t="str">
+      <c r="D7" s="7" t="str">
         <f>$C$28</f>
         <v>H122</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="16"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="13"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="9">
         <f>C6*C7</f>
         <v>8528.41</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="16"/>
+      <c r="D8" s="7"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="13"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="9">
         <f>'Financial Model'!M64</f>
         <v>234.4</v>
       </c>
-      <c r="D9" s="10" t="str">
+      <c r="D9" s="7" t="str">
         <f t="shared" ref="D9:D11" si="0">$C$28</f>
         <v>H122</v>
       </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="16"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="13"/>
     </row>
     <row r="10" spans="2:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="9">
         <f>'Financial Model'!M65</f>
         <v>802</v>
       </c>
-      <c r="D10" s="10" t="str">
+      <c r="D10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>H122</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="16"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="13"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="9">
         <f>C9-C10</f>
         <v>-567.6</v>
       </c>
-      <c r="D11" s="10" t="str">
+      <c r="D11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>H122</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="16"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="13"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="10">
         <f>C8-C11</f>
         <v>9096.01</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="16"/>
+      <c r="D12" s="8"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="13"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="G13" s="26"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="16"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="13"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="G14" s="26"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="16"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="13"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="16"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="63"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="13"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="16"/>
+      <c r="D16" s="58"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="13"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="16"/>
+      <c r="D17" s="58"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="13"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="16"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="58"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="13"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="16"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="60"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="13"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="G20" s="26"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="16"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="13"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="G21" s="26"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="16"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="13"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="16"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="63"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="16"/>
+      <c r="D23" s="58"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="13"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="57">
         <v>1894</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="16"/>
+      <c r="D24" s="58"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="13"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B25" s="20"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="23"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="13"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="20"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="58"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="13"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B27" s="20"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="23"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="16"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="13"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="54">
+      <c r="D28" s="45">
         <v>44882</v>
       </c>
-      <c r="G28" s="26"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="16"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="13"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="38"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="16"/>
+      <c r="D29" s="65"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="13"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="G30" s="26"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="16"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="13"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="G31" s="26"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="16"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="13"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="7"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="16"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="63"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="13"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="57">
+      <c r="C33" s="66">
         <f>C6/'Financial Model'!M62</f>
         <v>5.24180086047941</v>
       </c>
-      <c r="D33" s="58"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="16"/>
+      <c r="D33" s="67"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="13"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="23"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="16"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="58"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="13"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="23"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="16"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="58"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="13"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="23"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="16"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="58"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="13"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="23"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="16"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="58"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12"/>
+      <c r="S37" s="13"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="25"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="19"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="60"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -1950,7 +1985,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomRight" activeCell="M19" sqref="L19:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1958,739 +1993,939 @@
     <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="9.140625" style="36"/>
+    <col min="4" max="4" width="9.140625" style="29"/>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9.140625" style="36"/>
+    <col min="6" max="6" width="9.140625" style="29"/>
     <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="36"/>
+    <col min="8" max="8" width="9.140625" style="29"/>
     <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.140625" style="36"/>
+    <col min="10" max="10" width="9.140625" style="29"/>
     <col min="11" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="9.140625" style="36"/>
+    <col min="12" max="12" width="9.140625" style="29"/>
     <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="9.140625" style="65"/>
+    <col min="14" max="14" width="9.140625" style="55"/>
     <col min="15" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="9.140625" style="36"/>
+    <col min="16" max="16" width="9.140625" style="29"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:36" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="29" t="s">
+    <row r="1" spans="2:36" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="59" t="s">
+      <c r="N1" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="R1" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="S1" s="29" t="s">
+      <c r="S1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="T1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="29" t="s">
+      <c r="U1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="29" t="s">
+      <c r="V1" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="29" t="s">
+      <c r="W1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="X1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="29" t="s">
+      <c r="Y1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="Z1" s="29" t="s">
+      <c r="Z1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AA1" s="29" t="s">
+      <c r="AA1" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="29" t="s">
+      <c r="AB1" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="AC1" s="29" t="s">
+      <c r="AC1" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="29" t="s">
+      <c r="AD1" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="AE1" s="29" t="s">
+      <c r="AE1" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="29" t="s">
+      <c r="AF1" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="AG1" s="29" t="s">
+      <c r="AG1" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AH1" s="29" t="s">
+      <c r="AH1" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AI1" s="29" t="s">
+      <c r="AI1" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AJ1" s="29" t="s">
+      <c r="AJ1" s="22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:36" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="30"/>
-      <c r="C2" s="41">
+    <row r="2" spans="2:36" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="23"/>
+      <c r="C2" s="32">
         <v>43008</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="41">
+      <c r="D2" s="27"/>
+      <c r="E2" s="32">
         <v>43373</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="41">
+      <c r="F2" s="27"/>
+      <c r="G2" s="32">
         <v>43738</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="41">
+      <c r="H2" s="27"/>
+      <c r="I2" s="32">
         <v>44104</v>
       </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="41">
+      <c r="J2" s="27"/>
+      <c r="K2" s="32">
         <v>44469</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="41">
+      <c r="L2" s="69">
+        <f>V2</f>
+        <v>44651</v>
+      </c>
+      <c r="M2" s="32">
         <v>44834</v>
       </c>
-      <c r="N2" s="60"/>
-      <c r="P2" s="34"/>
-    </row>
-    <row r="3" spans="2:36" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="30"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="40">
+      <c r="N2" s="49"/>
+      <c r="P2" s="27"/>
+      <c r="U2" s="32">
+        <v>44286</v>
+      </c>
+      <c r="V2" s="32">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="3" spans="2:36" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="23"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="31">
         <v>44885</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="40">
+      <c r="F3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="31">
         <v>44884</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="40">
+      <c r="J3" s="27"/>
+      <c r="L3" s="70">
+        <f>V3</f>
+        <v>44728</v>
+      </c>
+      <c r="M3" s="31">
         <v>44882</v>
       </c>
-      <c r="N3" s="60"/>
-      <c r="P3" s="34"/>
-    </row>
-    <row r="4" spans="2:36" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="42" t="s">
+      <c r="N3" s="49"/>
+      <c r="P3" s="27"/>
+      <c r="V3" s="31">
+        <v>44728</v>
+      </c>
+    </row>
+    <row r="4" spans="2:36" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="33">
         <v>506.3</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="42">
+      <c r="D4" s="34"/>
+      <c r="E4" s="33">
         <v>585.5</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="42">
+      <c r="F4" s="34"/>
+      <c r="G4" s="33">
         <v>653.70000000000005</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="42">
+      <c r="H4" s="34"/>
+      <c r="I4" s="33">
         <v>618.4</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="42">
+      <c r="J4" s="34"/>
+      <c r="K4" s="33">
         <v>737.2</v>
       </c>
-      <c r="L4" s="43"/>
-      <c r="M4" s="42">
+      <c r="L4" s="34">
+        <f>V4-K4</f>
+        <v>788.09999999999991</v>
+      </c>
+      <c r="M4" s="33">
         <v>875.5</v>
       </c>
-      <c r="N4" s="61"/>
-      <c r="P4" s="43"/>
-    </row>
-    <row r="5" spans="2:36" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="42" t="s">
+      <c r="N4" s="50"/>
+      <c r="P4" s="34"/>
+      <c r="U4" s="33">
+        <v>1318.2</v>
+      </c>
+      <c r="V4" s="33">
+        <v>1525.3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:36" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="33">
         <v>81.8</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="42">
+      <c r="D5" s="34"/>
+      <c r="E5" s="33">
         <v>100.4</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="42">
+      <c r="F5" s="34"/>
+      <c r="G5" s="33">
         <v>111.6</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="42">
+      <c r="H5" s="34"/>
+      <c r="I5" s="33">
         <v>102.1</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="42">
+      <c r="J5" s="34"/>
+      <c r="K5" s="33">
         <v>137.6</v>
       </c>
-      <c r="L5" s="43"/>
-      <c r="M5" s="42">
+      <c r="L5" s="34">
+        <f>V5-K5</f>
+        <v>141.29999999999998</v>
+      </c>
+      <c r="M5" s="33">
         <v>151.69999999999999</v>
       </c>
-      <c r="N5" s="61"/>
-      <c r="P5" s="43"/>
-    </row>
-    <row r="6" spans="2:36" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="44" t="s">
+      <c r="N5" s="50"/>
+      <c r="P5" s="34"/>
+      <c r="U5" s="33">
+        <v>240.8</v>
+      </c>
+      <c r="V5" s="33">
+        <v>278.89999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="35">
         <v>-0.1</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="44">
+      <c r="D6" s="36"/>
+      <c r="E6" s="35">
         <v>-0.1</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="44">
+      <c r="F6" s="36"/>
+      <c r="G6" s="35">
         <v>-0.1</v>
       </c>
-      <c r="H6" s="45"/>
-      <c r="I6" s="44">
+      <c r="H6" s="36"/>
+      <c r="I6" s="35">
         <v>0</v>
       </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="44">
+      <c r="J6" s="36"/>
+      <c r="K6" s="35">
         <v>-0.1</v>
       </c>
-      <c r="L6" s="45"/>
-      <c r="M6" s="44">
+      <c r="L6" s="36">
+        <f>V6-K6</f>
         <v>0</v>
       </c>
-      <c r="N6" s="62"/>
-      <c r="P6" s="45"/>
-    </row>
-    <row r="7" spans="2:36" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="44" t="s">
+      <c r="M6" s="35">
+        <v>0</v>
+      </c>
+      <c r="N6" s="51"/>
+      <c r="P6" s="36"/>
+      <c r="U6" s="35">
+        <v>0</v>
+      </c>
+      <c r="V6" s="35">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="35">
         <v>0</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="44">
+      <c r="D7" s="36"/>
+      <c r="E7" s="35">
         <v>-0.9</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="44">
+      <c r="F7" s="36"/>
+      <c r="G7" s="35">
         <v>0</v>
       </c>
-      <c r="H7" s="45"/>
-      <c r="I7" s="44">
+      <c r="H7" s="36"/>
+      <c r="I7" s="35">
         <v>0</v>
       </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="44">
+      <c r="J7" s="36"/>
+      <c r="K7" s="35">
         <v>34</v>
       </c>
-      <c r="L7" s="45"/>
-      <c r="M7" s="44">
+      <c r="L7" s="36">
+        <f>V7-K7</f>
         <v>0</v>
       </c>
-      <c r="N7" s="62"/>
-      <c r="P7" s="45"/>
-    </row>
-    <row r="8" spans="2:36" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="44" t="s">
+      <c r="M7" s="35">
+        <v>0</v>
+      </c>
+      <c r="N7" s="51"/>
+      <c r="P7" s="36"/>
+      <c r="U7" s="35">
+        <v>22.1</v>
+      </c>
+      <c r="V7" s="35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="35">
         <v>0.1</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="44">
+      <c r="D8" s="36"/>
+      <c r="E8" s="35">
         <v>0.1</v>
       </c>
-      <c r="F8" s="45"/>
-      <c r="G8" s="44">
+      <c r="F8" s="36"/>
+      <c r="G8" s="35">
         <v>0.4</v>
       </c>
-      <c r="H8" s="45"/>
-      <c r="I8" s="44">
+      <c r="H8" s="36"/>
+      <c r="I8" s="35">
         <v>1</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="44">
+      <c r="J8" s="36"/>
+      <c r="K8" s="35">
         <v>0.6</v>
       </c>
-      <c r="L8" s="45"/>
-      <c r="M8" s="44">
+      <c r="L8" s="36">
+        <f>V8-K8</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="35">
         <v>0.8</v>
       </c>
-      <c r="N8" s="62"/>
-      <c r="P8" s="45"/>
-    </row>
-    <row r="9" spans="2:36" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="44" t="s">
+      <c r="N8" s="51"/>
+      <c r="P8" s="36"/>
+      <c r="U8" s="35">
+        <v>1</v>
+      </c>
+      <c r="V8" s="35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="35">
         <v>5</v>
       </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="44">
+      <c r="D9" s="36"/>
+      <c r="E9" s="35">
         <v>5</v>
       </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="44">
+      <c r="F9" s="36"/>
+      <c r="G9" s="35">
         <v>6.1</v>
       </c>
-      <c r="H9" s="45"/>
-      <c r="I9" s="44">
+      <c r="H9" s="36"/>
+      <c r="I9" s="35">
         <v>6.8</v>
       </c>
-      <c r="J9" s="45"/>
-      <c r="K9" s="44">
+      <c r="J9" s="36"/>
+      <c r="K9" s="35">
         <v>4.5999999999999996</v>
       </c>
-      <c r="L9" s="45"/>
-      <c r="M9" s="44">
+      <c r="L9" s="36">
+        <f>V9-K9</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M9" s="35">
         <v>7</v>
       </c>
-      <c r="N9" s="62"/>
-      <c r="P9" s="45"/>
-    </row>
-    <row r="10" spans="2:36" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="44" t="s">
+      <c r="N9" s="51"/>
+      <c r="P9" s="36"/>
+      <c r="U9" s="35">
+        <v>11</v>
+      </c>
+      <c r="V9" s="35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="35">
         <f>C5+C6+C7+C8-C9</f>
         <v>76.8</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="44">
+      <c r="D10" s="36"/>
+      <c r="E10" s="35">
         <f>E5+E6+E7+E8-E9</f>
         <v>94.5</v>
       </c>
-      <c r="F10" s="45"/>
-      <c r="G10" s="44">
+      <c r="F10" s="36"/>
+      <c r="G10" s="35">
         <f>G5+G6+G7+G8-G9</f>
         <v>105.80000000000001</v>
       </c>
-      <c r="H10" s="45"/>
-      <c r="I10" s="44">
+      <c r="H10" s="36"/>
+      <c r="I10" s="35">
         <f>I5+I6+I7+I8-I9</f>
         <v>96.3</v>
       </c>
-      <c r="J10" s="45"/>
-      <c r="K10" s="44">
+      <c r="J10" s="36"/>
+      <c r="K10" s="35">
         <f>K5+K6+K7+K8-K9</f>
         <v>167.5</v>
       </c>
-      <c r="L10" s="45"/>
-      <c r="M10" s="44">
+      <c r="L10" s="36">
+        <f>L5+L6+L7+L8-L9</f>
+        <v>136.89999999999998</v>
+      </c>
+      <c r="M10" s="35">
         <f>M5+M6+M7+M8-M9</f>
         <v>145.5</v>
       </c>
-      <c r="N10" s="62"/>
-      <c r="P10" s="45"/>
-    </row>
-    <row r="11" spans="2:36" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="44" t="s">
+      <c r="N10" s="51"/>
+      <c r="P10" s="36"/>
+      <c r="U10" s="35">
+        <f>U5+U6+U7+U8-U9</f>
+        <v>252.90000000000003</v>
+      </c>
+      <c r="V10" s="35">
+        <f>V5+V6+V7+V8-V9</f>
+        <v>304.39999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="35">
         <v>15.1</v>
       </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="44">
+      <c r="D11" s="36"/>
+      <c r="E11" s="35">
         <v>19.899999999999999</v>
       </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="44">
+      <c r="F11" s="36"/>
+      <c r="G11" s="35">
         <v>20.8</v>
       </c>
-      <c r="H11" s="45"/>
-      <c r="I11" s="44">
+      <c r="H11" s="36"/>
+      <c r="I11" s="35">
         <v>19</v>
       </c>
-      <c r="J11" s="45"/>
-      <c r="K11" s="44">
+      <c r="J11" s="36"/>
+      <c r="K11" s="35">
         <v>31.8</v>
       </c>
-      <c r="L11" s="45"/>
-      <c r="M11" s="44">
+      <c r="L11" s="36">
+        <f>V11-K11</f>
+        <v>28.400000000000002</v>
+      </c>
+      <c r="M11" s="35">
         <v>30.7</v>
       </c>
-      <c r="N11" s="62"/>
-      <c r="P11" s="45"/>
-    </row>
-    <row r="12" spans="2:36" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="42" t="s">
+      <c r="N11" s="51"/>
+      <c r="P11" s="36"/>
+      <c r="U11" s="35">
+        <v>49.6</v>
+      </c>
+      <c r="V11" s="35">
+        <v>60.2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:36" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="33">
         <f>C10-C11</f>
         <v>61.699999999999996</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="42">
+      <c r="D12" s="34"/>
+      <c r="E12" s="33">
         <f>E10-E11</f>
         <v>74.599999999999994</v>
       </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="42">
+      <c r="F12" s="34"/>
+      <c r="G12" s="33">
         <f>G10-G11</f>
         <v>85.000000000000014</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="42">
+      <c r="H12" s="34"/>
+      <c r="I12" s="33">
         <f>I10-I11</f>
         <v>77.3</v>
       </c>
-      <c r="J12" s="43"/>
-      <c r="K12" s="42">
+      <c r="J12" s="34"/>
+      <c r="K12" s="33">
         <f>K10-K11</f>
         <v>135.69999999999999</v>
       </c>
-      <c r="L12" s="43"/>
-      <c r="M12" s="42">
+      <c r="L12" s="34">
+        <f>L10-L11</f>
+        <v>108.49999999999997</v>
+      </c>
+      <c r="M12" s="33">
         <f>M10-M11</f>
         <v>114.8</v>
       </c>
-      <c r="N12" s="61"/>
-      <c r="P12" s="43"/>
-    </row>
-    <row r="13" spans="2:36" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="N12" s="50"/>
+      <c r="P12" s="34"/>
+      <c r="U12" s="33">
+        <f>U10-U11</f>
+        <v>203.30000000000004</v>
+      </c>
+      <c r="V12" s="33">
+        <f>V10-V11</f>
+        <v>244.2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:36" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="33">
         <f>C12+C14</f>
         <v>61.699999999999996</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="42">
+      <c r="D13" s="34"/>
+      <c r="E13" s="33">
         <f>E12+E14</f>
         <v>74.599999999999994</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="42">
+      <c r="F13" s="34"/>
+      <c r="G13" s="33">
         <f>G12+G14</f>
         <v>85.000000000000014</v>
       </c>
-      <c r="H13" s="43"/>
-      <c r="I13" s="42">
+      <c r="H13" s="34"/>
+      <c r="I13" s="33">
         <f>I12+I14</f>
         <v>77.3</v>
       </c>
-      <c r="J13" s="43"/>
-      <c r="K13" s="42">
+      <c r="J13" s="34"/>
+      <c r="K13" s="33">
         <f>K12+K14</f>
         <v>135.79999999999998</v>
       </c>
-      <c r="L13" s="43"/>
-      <c r="M13" s="42">
+      <c r="L13" s="34">
+        <f>L12+L14</f>
+        <v>108.19999999999997</v>
+      </c>
+      <c r="M13" s="33">
         <f>M12+M14</f>
         <v>115</v>
       </c>
-      <c r="N13" s="61"/>
-      <c r="P13" s="43"/>
-    </row>
-    <row r="14" spans="2:36" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="44" t="s">
+      <c r="N13" s="50"/>
+      <c r="P13" s="34"/>
+      <c r="U13" s="33">
+        <f>U12+U14</f>
+        <v>203.20000000000005</v>
+      </c>
+      <c r="V13" s="33">
+        <f>V12+V14</f>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="55">
+      <c r="C14" s="46">
         <v>0</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="55">
+      <c r="D14" s="36"/>
+      <c r="E14" s="46">
         <v>0</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="55">
+      <c r="F14" s="36"/>
+      <c r="G14" s="46">
         <v>0</v>
       </c>
-      <c r="H14" s="45"/>
-      <c r="I14" s="55">
+      <c r="H14" s="36"/>
+      <c r="I14" s="46">
         <v>0</v>
       </c>
-      <c r="J14" s="45"/>
-      <c r="K14" s="44">
+      <c r="J14" s="36"/>
+      <c r="K14" s="35">
         <v>0.1</v>
       </c>
-      <c r="L14" s="45"/>
-      <c r="M14" s="44">
+      <c r="L14" s="36">
+        <f>V14-K14</f>
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="M14" s="35">
         <v>0.2</v>
       </c>
-      <c r="N14" s="62"/>
-      <c r="P14" s="45"/>
-    </row>
-    <row r="15" spans="2:36" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="46" t="s">
+      <c r="N14" s="51"/>
+      <c r="P14" s="36"/>
+      <c r="U14" s="35">
+        <v>-0.1</v>
+      </c>
+      <c r="V14" s="35">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:36" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="46">
+      <c r="C15" s="37">
         <f>C12/C16</f>
         <v>0.16270266756508422</v>
       </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="46">
+      <c r="D15" s="38"/>
+      <c r="E15" s="37">
         <f>E12/E16</f>
         <v>0.19681108372907286</v>
       </c>
-      <c r="F15" s="47"/>
-      <c r="G15" s="46">
+      <c r="F15" s="38"/>
+      <c r="G15" s="37">
         <f>G12/G16</f>
         <v>0.22419479233636896</v>
       </c>
-      <c r="H15" s="47"/>
-      <c r="I15" s="46">
+      <c r="H15" s="38"/>
+      <c r="I15" s="37">
         <f>I12/I16</f>
         <v>0.20390802308932054</v>
       </c>
-      <c r="J15" s="47"/>
-      <c r="K15" s="46">
+      <c r="J15" s="38"/>
+      <c r="K15" s="37">
         <f>K12/K16</f>
         <v>0.35795304668952777</v>
       </c>
-      <c r="L15" s="47"/>
-      <c r="M15" s="46">
+      <c r="L15" s="38">
+        <f>L12/L16</f>
+        <v>0.28650646950092412</v>
+      </c>
+      <c r="M15" s="37">
         <f>M12/M16</f>
         <v>0.30354309888947645</v>
       </c>
-      <c r="N15" s="63"/>
-      <c r="P15" s="47"/>
-    </row>
-    <row r="16" spans="2:36" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="44" t="s">
+      <c r="N15" s="52"/>
+      <c r="P15" s="38"/>
+      <c r="U15" s="37">
+        <f>U12/U16</f>
+        <v>0.53612869198312252</v>
+      </c>
+      <c r="V15" s="37">
+        <f>V12/V16</f>
+        <v>0.6448376023237391</v>
+      </c>
+    </row>
+    <row r="16" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="35">
         <v>379.21935100000002</v>
       </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="44">
+      <c r="D16" s="36"/>
+      <c r="E16" s="35">
         <v>379.04369300000002</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="44">
+      <c r="F16" s="36"/>
+      <c r="G16" s="35">
         <v>379.13458700000001</v>
       </c>
-      <c r="H16" s="45"/>
-      <c r="I16" s="44">
+      <c r="H16" s="36"/>
+      <c r="I16" s="35">
         <v>379.092489</v>
       </c>
-      <c r="J16" s="45"/>
-      <c r="K16" s="44">
+      <c r="J16" s="36"/>
+      <c r="K16" s="35">
         <v>379.1</v>
       </c>
-      <c r="L16" s="45"/>
-      <c r="M16" s="44">
+      <c r="L16" s="36">
+        <f>V16</f>
+        <v>378.7</v>
+      </c>
+      <c r="M16" s="35">
         <v>378.2</v>
       </c>
-      <c r="N16" s="62"/>
-      <c r="P16" s="45"/>
-    </row>
-    <row r="18" spans="2:16" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="50" t="s">
+      <c r="N16" s="51"/>
+      <c r="P16" s="36"/>
+      <c r="U16" s="35">
+        <v>379.2</v>
+      </c>
+      <c r="V16" s="35">
+        <v>378.7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="50">
+      <c r="D18" s="42"/>
+      <c r="E18" s="41">
         <f>E4/C4-1</f>
         <v>0.15642899466719329</v>
       </c>
-      <c r="F18" s="51"/>
-      <c r="G18" s="50">
+      <c r="F18" s="42"/>
+      <c r="G18" s="41">
         <f>G4/E4-1</f>
         <v>0.11648163962425295</v>
       </c>
-      <c r="H18" s="51"/>
-      <c r="I18" s="50">
+      <c r="H18" s="42"/>
+      <c r="I18" s="41">
         <f>I4/G4-1</f>
         <v>-5.4000305950742011E-2</v>
       </c>
-      <c r="J18" s="51"/>
-      <c r="K18" s="50">
+      <c r="J18" s="42"/>
+      <c r="K18" s="41">
         <f>K4/I4-1</f>
         <v>0.19210866752910749</v>
       </c>
-      <c r="L18" s="51"/>
-      <c r="M18" s="50">
+      <c r="L18" s="42"/>
+      <c r="M18" s="41">
         <f>M4/K4-1</f>
         <v>0.18760173629951149</v>
       </c>
-      <c r="N18" s="64"/>
-      <c r="P18" s="51"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N18" s="53"/>
+      <c r="P18" s="42"/>
+      <c r="V18" s="41">
+        <f>V4/U4-1</f>
+        <v>0.15710817781823683</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N19" s="66">
+      <c r="L19" s="40">
+        <f>L4/K4-1</f>
+        <v>6.9045035268583632E-2</v>
+      </c>
+      <c r="M19" s="39">
+        <f>M4/L4-1</f>
+        <v>0.11089963202639264</v>
+      </c>
+      <c r="N19" s="54">
         <f>N4/M4-1</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="21" spans="2:16" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="48" t="s">
+      <c r="R19" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="S19" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="T19" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="U19" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="V19" s="68" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C21" s="39">
         <f>C5/C4</f>
         <v>0.16156428994667194</v>
       </c>
-      <c r="D21" s="49"/>
-      <c r="E21" s="48">
+      <c r="D21" s="40"/>
+      <c r="E21" s="39">
         <f>E5/E4</f>
         <v>0.17147736976942785</v>
       </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="48">
+      <c r="F21" s="40"/>
+      <c r="G21" s="39">
         <f>G5/G4</f>
         <v>0.17072051399724641</v>
       </c>
-      <c r="H21" s="49"/>
-      <c r="I21" s="48">
+      <c r="H21" s="40"/>
+      <c r="I21" s="39">
         <f>I5/I4</f>
         <v>0.16510349288486417</v>
       </c>
-      <c r="J21" s="49"/>
-      <c r="K21" s="48">
+      <c r="J21" s="40"/>
+      <c r="K21" s="39">
         <f>K5/K4</f>
         <v>0.18665219750406944</v>
       </c>
-      <c r="L21" s="49"/>
-      <c r="M21" s="48">
+      <c r="L21" s="40">
+        <f>L5/L4</f>
+        <v>0.1792919680243624</v>
+      </c>
+      <c r="M21" s="39">
         <f>M5/M4</f>
         <v>0.17327241576242147</v>
       </c>
-      <c r="N21" s="66"/>
-      <c r="P21" s="49"/>
-    </row>
-    <row r="22" spans="2:16" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="48" t="s">
+      <c r="N21" s="54"/>
+      <c r="P21" s="40"/>
+      <c r="U21" s="39">
+        <f t="shared" ref="U21:V21" si="0">U5/U4</f>
+        <v>0.18267334243665606</v>
+      </c>
+      <c r="V21" s="39">
+        <f t="shared" si="0"/>
+        <v>0.18284927555235034</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="39">
         <f>C12/C4</f>
         <v>0.12186450720916452</v>
       </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="48">
+      <c r="D22" s="40"/>
+      <c r="E22" s="39">
         <f>E12/E4</f>
         <v>0.12741246797608879</v>
       </c>
-      <c r="F22" s="49"/>
-      <c r="G22" s="48">
+      <c r="F22" s="40"/>
+      <c r="G22" s="39">
         <f>G12/G4</f>
         <v>0.13002906532048342</v>
       </c>
-      <c r="H22" s="49"/>
-      <c r="I22" s="48">
+      <c r="H22" s="40"/>
+      <c r="I22" s="39">
         <f>I12/I4</f>
         <v>0.125</v>
       </c>
-      <c r="J22" s="49"/>
-      <c r="K22" s="48">
+      <c r="J22" s="40"/>
+      <c r="K22" s="39">
         <f>K12/K4</f>
         <v>0.18407487791644056</v>
       </c>
-      <c r="L22" s="49"/>
-      <c r="M22" s="48">
+      <c r="L22" s="40">
+        <f>L12/L4</f>
+        <v>0.13767288415175738</v>
+      </c>
+      <c r="M22" s="39">
         <f>M12/M4</f>
         <v>0.1311250713877784</v>
       </c>
-      <c r="N22" s="66"/>
-      <c r="P22" s="49"/>
-    </row>
-    <row r="23" spans="2:16" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="48" t="s">
+      <c r="N22" s="54"/>
+      <c r="P22" s="40"/>
+      <c r="U22" s="39">
+        <f t="shared" ref="U22:V22" si="1">U12/U4</f>
+        <v>0.1542254589591868</v>
+      </c>
+      <c r="V22" s="39">
+        <f t="shared" si="1"/>
+        <v>0.16009965252737166</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="48">
+      <c r="C23" s="39">
         <f>C11/C10</f>
         <v>0.19661458333333334</v>
       </c>
-      <c r="D23" s="49"/>
-      <c r="E23" s="48">
+      <c r="D23" s="40"/>
+      <c r="E23" s="39">
         <f>E11/E10</f>
         <v>0.21058201058201056</v>
       </c>
-      <c r="F23" s="49"/>
-      <c r="G23" s="48">
+      <c r="F23" s="40"/>
+      <c r="G23" s="39">
         <f>G11/G10</f>
         <v>0.19659735349716445</v>
       </c>
-      <c r="H23" s="49"/>
-      <c r="I23" s="48">
+      <c r="H23" s="40"/>
+      <c r="I23" s="39">
         <f>I11/I10</f>
         <v>0.19730010384215993</v>
       </c>
-      <c r="J23" s="49"/>
-      <c r="K23" s="48">
+      <c r="J23" s="40"/>
+      <c r="K23" s="39">
         <f>K11/K10</f>
         <v>0.18985074626865672</v>
       </c>
-      <c r="L23" s="49"/>
-      <c r="M23" s="48">
+      <c r="L23" s="40">
+        <f>L11/L10</f>
+        <v>0.20745069393718046</v>
+      </c>
+      <c r="M23" s="39">
         <f>M11/M10</f>
         <v>0.21099656357388316</v>
       </c>
-      <c r="N23" s="66"/>
-      <c r="P23" s="49"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B27" s="52" t="s">
+      <c r="N23" s="54"/>
+      <c r="P23" s="40"/>
+      <c r="U23" s="39">
+        <f t="shared" ref="U23:V23" si="2">U11/U10</f>
+        <v>0.19612495057334914</v>
+      </c>
+      <c r="V23" s="39">
+        <f t="shared" si="2"/>
+        <v>0.19776609724047309</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B27" s="43" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>80</v>
       </c>
@@ -2702,25 +2937,25 @@
         <f>655.6+229.9</f>
         <v>885.5</v>
       </c>
-      <c r="G28" s="44">
+      <c r="G28" s="35">
         <f>765.5+272.4</f>
         <v>1037.9000000000001</v>
       </c>
-      <c r="H28" s="45"/>
-      <c r="I28" s="44">
+      <c r="H28" s="36"/>
+      <c r="I28" s="35">
         <f>829.8+303.8</f>
         <v>1133.5999999999999</v>
       </c>
-      <c r="K28" s="44">
+      <c r="K28" s="35">
         <f>867.4+319.3</f>
         <v>1186.7</v>
       </c>
-      <c r="M28" s="44">
+      <c r="M28" s="35">
         <f>1101.8+418.6</f>
         <v>1520.4</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>81</v>
       </c>
@@ -2730,51 +2965,51 @@
       <c r="E29" s="1">
         <v>109.6</v>
       </c>
-      <c r="G29" s="44">
+      <c r="G29" s="35">
         <v>171.7</v>
       </c>
-      <c r="H29" s="45"/>
-      <c r="I29" s="44">
+      <c r="H29" s="36"/>
+      <c r="I29" s="35">
         <v>184.7</v>
       </c>
-      <c r="K29" s="44">
+      <c r="K29" s="35">
         <v>186.7</v>
       </c>
-      <c r="M29" s="44">
+      <c r="M29" s="35">
         <v>224.5</v>
       </c>
     </row>
-    <row r="30" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C30" s="2">
         <v>3.4</v>
       </c>
-      <c r="D30" s="35"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="2">
         <v>3.9</v>
       </c>
-      <c r="F30" s="35"/>
-      <c r="G30" s="42">
+      <c r="F30" s="28"/>
+      <c r="G30" s="33">
         <v>5.5</v>
       </c>
-      <c r="H30" s="43"/>
-      <c r="I30" s="42">
+      <c r="H30" s="34"/>
+      <c r="I30" s="33">
         <v>4.8</v>
       </c>
-      <c r="J30" s="35"/>
-      <c r="K30" s="42">
+      <c r="J30" s="28"/>
+      <c r="K30" s="33">
         <v>9.9</v>
       </c>
-      <c r="L30" s="35"/>
-      <c r="M30" s="42">
+      <c r="L30" s="28"/>
+      <c r="M30" s="33">
         <v>19.8</v>
       </c>
-      <c r="N30" s="67"/>
-      <c r="P30" s="35"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N30" s="56"/>
+      <c r="P30" s="28"/>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>83</v>
       </c>
@@ -2784,21 +3019,21 @@
       <c r="E31" s="1">
         <v>0</v>
       </c>
-      <c r="G31" s="44">
+      <c r="G31" s="35">
         <v>0</v>
       </c>
-      <c r="H31" s="45"/>
-      <c r="I31" s="44">
+      <c r="H31" s="36"/>
+      <c r="I31" s="35">
         <v>0</v>
       </c>
-      <c r="K31" s="44">
+      <c r="K31" s="35">
         <v>4.8</v>
       </c>
-      <c r="M31" s="44">
+      <c r="M31" s="35">
         <v>43.9</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>84</v>
       </c>
@@ -2808,17 +3043,17 @@
       <c r="E32" s="1">
         <v>0</v>
       </c>
-      <c r="G32" s="44">
+      <c r="G32" s="35">
         <v>0</v>
       </c>
-      <c r="H32" s="45"/>
-      <c r="I32" s="44">
+      <c r="H32" s="36"/>
+      <c r="I32" s="35">
         <v>0</v>
       </c>
-      <c r="K32" s="44">
+      <c r="K32" s="35">
         <v>14.7</v>
       </c>
-      <c r="M32" s="44">
+      <c r="M32" s="35">
         <v>14.7</v>
       </c>
     </row>
@@ -2832,17 +3067,17 @@
       <c r="E33" s="1">
         <v>30.9</v>
       </c>
-      <c r="G33" s="44">
+      <c r="G33" s="35">
         <v>1.4</v>
       </c>
-      <c r="H33" s="45"/>
-      <c r="I33" s="44">
+      <c r="H33" s="36"/>
+      <c r="I33" s="35">
         <v>5.6</v>
       </c>
-      <c r="K33" s="44">
+      <c r="K33" s="35">
         <v>1.9</v>
       </c>
-      <c r="M33" s="44">
+      <c r="M33" s="35">
         <v>2.8</v>
       </c>
     </row>
@@ -2850,28 +3085,28 @@
       <c r="B34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="44">
+      <c r="C34" s="35">
         <f>SUM(C28:C33)</f>
         <v>964.49999999999989</v>
       </c>
-      <c r="E34" s="44">
+      <c r="E34" s="35">
         <f>SUM(E28:E33)</f>
         <v>1029.9000000000001</v>
       </c>
-      <c r="G34" s="44">
+      <c r="G34" s="35">
         <f>SUM(G28:G33)</f>
         <v>1216.5000000000002</v>
       </c>
-      <c r="H34" s="45"/>
-      <c r="I34" s="44">
+      <c r="H34" s="36"/>
+      <c r="I34" s="35">
         <f>SUM(I28:I33)</f>
         <v>1328.6999999999998</v>
       </c>
-      <c r="K34" s="44">
+      <c r="K34" s="35">
         <f>SUM(K28:K33)</f>
         <v>1404.7000000000003</v>
       </c>
-      <c r="M34" s="44">
+      <c r="M34" s="35">
         <f>SUM(M28:M33)</f>
         <v>1826.1000000000001</v>
       </c>
@@ -2886,17 +3121,17 @@
       <c r="E35" s="1">
         <v>141.19999999999999</v>
       </c>
-      <c r="G35" s="44">
+      <c r="G35" s="35">
         <v>162.9</v>
       </c>
-      <c r="H35" s="45"/>
-      <c r="I35" s="44">
+      <c r="H35" s="36"/>
+      <c r="I35" s="35">
         <v>175.8</v>
       </c>
-      <c r="K35" s="44">
+      <c r="K35" s="35">
         <v>193.2</v>
       </c>
-      <c r="M35" s="44">
+      <c r="M35" s="35">
         <v>308.8</v>
       </c>
     </row>
@@ -2910,17 +3145,17 @@
       <c r="E36" s="1">
         <v>241.8</v>
       </c>
-      <c r="G36" s="44">
+      <c r="G36" s="35">
         <v>275.2</v>
       </c>
-      <c r="H36" s="45"/>
-      <c r="I36" s="44">
+      <c r="H36" s="36"/>
+      <c r="I36" s="35">
         <v>245.3</v>
       </c>
-      <c r="K36" s="44">
+      <c r="K36" s="35">
         <v>279.2</v>
       </c>
-      <c r="M36" s="44">
+      <c r="M36" s="35">
         <v>389.9</v>
       </c>
     </row>
@@ -2934,17 +3169,17 @@
       <c r="E37" s="1">
         <v>0.7</v>
       </c>
-      <c r="G37" s="44">
+      <c r="G37" s="35">
         <v>4.8</v>
       </c>
-      <c r="H37" s="45"/>
-      <c r="I37" s="44">
+      <c r="H37" s="36"/>
+      <c r="I37" s="35">
         <v>6.5</v>
       </c>
-      <c r="K37" s="44">
+      <c r="K37" s="35">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M37" s="44">
+      <c r="M37" s="35">
         <v>1.9</v>
       </c>
     </row>
@@ -2955,28 +3190,28 @@
       <c r="C38" s="2">
         <v>71.7</v>
       </c>
-      <c r="D38" s="35"/>
+      <c r="D38" s="28"/>
       <c r="E38" s="2">
         <v>66.400000000000006</v>
       </c>
-      <c r="F38" s="35"/>
-      <c r="G38" s="44">
+      <c r="F38" s="28"/>
+      <c r="G38" s="35">
         <v>83.2</v>
       </c>
-      <c r="H38" s="43"/>
-      <c r="I38" s="42">
+      <c r="H38" s="34"/>
+      <c r="I38" s="33">
         <v>125.5</v>
       </c>
-      <c r="J38" s="35"/>
-      <c r="K38" s="42">
+      <c r="J38" s="28"/>
+      <c r="K38" s="33">
         <v>131.1</v>
       </c>
-      <c r="L38" s="35"/>
-      <c r="M38" s="42">
+      <c r="L38" s="28"/>
+      <c r="M38" s="33">
         <v>213.4</v>
       </c>
-      <c r="N38" s="67"/>
-      <c r="P38" s="35"/>
+      <c r="N38" s="56"/>
+      <c r="P38" s="28"/>
     </row>
     <row r="39" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
@@ -2985,120 +3220,120 @@
       <c r="C39" s="2">
         <v>0.6</v>
       </c>
-      <c r="D39" s="35"/>
+      <c r="D39" s="28"/>
       <c r="E39" s="2">
         <v>0.3</v>
       </c>
-      <c r="F39" s="35"/>
-      <c r="G39" s="42">
+      <c r="F39" s="28"/>
+      <c r="G39" s="33">
         <v>0.9</v>
       </c>
-      <c r="H39" s="43"/>
-      <c r="I39" s="42">
+      <c r="H39" s="34"/>
+      <c r="I39" s="33">
         <v>0.4</v>
       </c>
-      <c r="J39" s="35"/>
-      <c r="K39" s="42">
+      <c r="J39" s="28"/>
+      <c r="K39" s="33">
         <v>0.6</v>
       </c>
-      <c r="L39" s="35"/>
-      <c r="M39" s="42">
+      <c r="L39" s="28"/>
+      <c r="M39" s="33">
         <v>1.2</v>
       </c>
-      <c r="N39" s="67"/>
-      <c r="P39" s="35"/>
+      <c r="N39" s="56"/>
+      <c r="P39" s="28"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="44">
+      <c r="C40" s="35">
         <f>SUM(C35:C39)+C34</f>
         <v>1364.8</v>
       </c>
-      <c r="E40" s="44">
+      <c r="E40" s="35">
         <f>SUM(E35:E39)+E34</f>
         <v>1480.3000000000002</v>
       </c>
-      <c r="G40" s="44">
+      <c r="G40" s="35">
         <f>SUM(G35:G39)+G34</f>
         <v>1743.5000000000002</v>
       </c>
-      <c r="H40" s="45"/>
-      <c r="I40" s="44">
+      <c r="H40" s="36"/>
+      <c r="I40" s="35">
         <f>SUM(I35:I39)+I34</f>
         <v>1882.1999999999998</v>
       </c>
-      <c r="K40" s="44">
+      <c r="K40" s="35">
         <f>SUM(K35:K39)+K34</f>
         <v>2013.2000000000003</v>
       </c>
-      <c r="M40" s="44">
+      <c r="M40" s="35">
         <f>SUM(M35:M39)+M34</f>
         <v>2741.3</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="G41" s="44"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="44"/>
-      <c r="M41" s="44"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="35"/>
+      <c r="M41" s="35"/>
     </row>
     <row r="42" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="42">
+      <c r="C42" s="33">
         <v>0.2</v>
       </c>
-      <c r="D42" s="43"/>
-      <c r="E42" s="42">
+      <c r="D42" s="34"/>
+      <c r="E42" s="33">
         <v>3</v>
       </c>
-      <c r="F42" s="43"/>
-      <c r="G42" s="42">
+      <c r="F42" s="34"/>
+      <c r="G42" s="33">
         <v>1.7</v>
       </c>
-      <c r="H42" s="43"/>
-      <c r="I42" s="42">
+      <c r="H42" s="34"/>
+      <c r="I42" s="33">
         <v>76.099999999999994</v>
       </c>
-      <c r="J42" s="43"/>
-      <c r="K42" s="42">
+      <c r="J42" s="34"/>
+      <c r="K42" s="33">
         <v>206.1</v>
       </c>
-      <c r="L42" s="43"/>
-      <c r="M42" s="42">
+      <c r="L42" s="34"/>
+      <c r="M42" s="33">
         <v>256.39999999999998</v>
       </c>
-      <c r="N42" s="67"/>
-      <c r="P42" s="35"/>
+      <c r="N42" s="56"/>
+      <c r="P42" s="28"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="44">
+      <c r="C43" s="35">
         <v>0</v>
       </c>
-      <c r="D43" s="45"/>
-      <c r="E43" s="44">
+      <c r="D43" s="36"/>
+      <c r="E43" s="35">
         <v>0</v>
       </c>
-      <c r="F43" s="45"/>
-      <c r="G43" s="44">
+      <c r="F43" s="36"/>
+      <c r="G43" s="35">
         <v>12.3</v>
       </c>
-      <c r="H43" s="45"/>
-      <c r="I43" s="44">
+      <c r="H43" s="36"/>
+      <c r="I43" s="35">
         <v>13</v>
       </c>
-      <c r="J43" s="45"/>
-      <c r="K43" s="44">
+      <c r="J43" s="36"/>
+      <c r="K43" s="35">
         <v>3</v>
       </c>
-      <c r="L43" s="45"/>
-      <c r="M43" s="44">
+      <c r="L43" s="36"/>
+      <c r="M43" s="35">
         <v>78.8</v>
       </c>
     </row>
@@ -3106,27 +3341,27 @@
       <c r="B44" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="44">
+      <c r="C44" s="35">
         <v>0</v>
       </c>
-      <c r="D44" s="45"/>
-      <c r="E44" s="44">
+      <c r="D44" s="36"/>
+      <c r="E44" s="35">
         <v>0</v>
       </c>
-      <c r="F44" s="45"/>
-      <c r="G44" s="44">
+      <c r="F44" s="36"/>
+      <c r="G44" s="35">
         <v>0</v>
       </c>
-      <c r="H44" s="45"/>
-      <c r="I44" s="44">
+      <c r="H44" s="36"/>
+      <c r="I44" s="35">
         <v>0</v>
       </c>
-      <c r="J44" s="45"/>
-      <c r="K44" s="44">
+      <c r="J44" s="36"/>
+      <c r="K44" s="35">
         <v>14.2</v>
       </c>
-      <c r="L44" s="45"/>
-      <c r="M44" s="44">
+      <c r="L44" s="36"/>
+      <c r="M44" s="35">
         <v>19.399999999999999</v>
       </c>
     </row>
@@ -3134,27 +3369,27 @@
       <c r="B45" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="44">
+      <c r="C45" s="35">
         <v>125.7</v>
       </c>
-      <c r="D45" s="45"/>
-      <c r="E45" s="44">
+      <c r="D45" s="36"/>
+      <c r="E45" s="35">
         <v>154.5</v>
       </c>
-      <c r="F45" s="45"/>
-      <c r="G45" s="44">
+      <c r="F45" s="36"/>
+      <c r="G45" s="35">
         <v>157.9</v>
       </c>
-      <c r="H45" s="45"/>
-      <c r="I45" s="44">
+      <c r="H45" s="36"/>
+      <c r="I45" s="35">
         <v>158.69999999999999</v>
       </c>
-      <c r="J45" s="45"/>
-      <c r="K45" s="44">
+      <c r="J45" s="36"/>
+      <c r="K45" s="35">
         <v>22</v>
       </c>
-      <c r="L45" s="45"/>
-      <c r="M45" s="44">
+      <c r="L45" s="36"/>
+      <c r="M45" s="35">
         <v>26.5</v>
       </c>
     </row>
@@ -3162,27 +3397,27 @@
       <c r="B46" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="44">
+      <c r="C46" s="35">
         <v>4.7</v>
       </c>
-      <c r="D46" s="45"/>
-      <c r="E46" s="44">
+      <c r="D46" s="36"/>
+      <c r="E46" s="35">
         <v>18.2</v>
       </c>
-      <c r="F46" s="45"/>
-      <c r="G46" s="44">
+      <c r="F46" s="36"/>
+      <c r="G46" s="35">
         <v>20.5</v>
       </c>
-      <c r="H46" s="45"/>
-      <c r="I46" s="44">
+      <c r="H46" s="36"/>
+      <c r="I46" s="35">
         <v>30.5</v>
       </c>
-      <c r="J46" s="45"/>
-      <c r="K46" s="44">
+      <c r="J46" s="36"/>
+      <c r="K46" s="35">
         <v>13.8</v>
       </c>
-      <c r="L46" s="45"/>
-      <c r="M46" s="44">
+      <c r="L46" s="36"/>
+      <c r="M46" s="35">
         <v>15.8</v>
       </c>
     </row>
@@ -3190,27 +3425,27 @@
       <c r="B47" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="44">
+      <c r="C47" s="35">
         <v>14.9</v>
       </c>
-      <c r="D47" s="45"/>
-      <c r="E47" s="44">
+      <c r="D47" s="36"/>
+      <c r="E47" s="35">
         <v>13.3</v>
       </c>
-      <c r="F47" s="45"/>
-      <c r="G47" s="44">
+      <c r="F47" s="36"/>
+      <c r="G47" s="35">
         <v>13.4</v>
       </c>
-      <c r="H47" s="45"/>
-      <c r="I47" s="44">
+      <c r="H47" s="36"/>
+      <c r="I47" s="35">
         <v>11.3</v>
       </c>
-      <c r="J47" s="45"/>
-      <c r="K47" s="44">
+      <c r="J47" s="36"/>
+      <c r="K47" s="35">
         <v>0.2</v>
       </c>
-      <c r="L47" s="45"/>
-      <c r="M47" s="44">
+      <c r="L47" s="36"/>
+      <c r="M47" s="35">
         <v>3.4</v>
       </c>
     </row>
@@ -3218,62 +3453,62 @@
       <c r="B48" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="42">
+      <c r="C48" s="33">
         <v>0.4</v>
       </c>
-      <c r="D48" s="43"/>
-      <c r="E48" s="42">
+      <c r="D48" s="34"/>
+      <c r="E48" s="33">
         <v>0.5</v>
       </c>
-      <c r="F48" s="43"/>
-      <c r="G48" s="42">
+      <c r="F48" s="34"/>
+      <c r="G48" s="33">
         <v>0.7</v>
       </c>
-      <c r="H48" s="43"/>
-      <c r="I48" s="42">
+      <c r="H48" s="34"/>
+      <c r="I48" s="33">
         <v>0.9</v>
       </c>
-      <c r="J48" s="43"/>
-      <c r="K48" s="42">
+      <c r="J48" s="34"/>
+      <c r="K48" s="33">
         <v>0</v>
       </c>
-      <c r="L48" s="43"/>
-      <c r="M48" s="42">
+      <c r="L48" s="34"/>
+      <c r="M48" s="33">
         <v>0</v>
       </c>
-      <c r="N48" s="67"/>
-      <c r="P48" s="35"/>
+      <c r="N48" s="56"/>
+      <c r="P48" s="28"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="44">
+      <c r="C49" s="35">
         <f>SUM(C42:C48)</f>
         <v>145.9</v>
       </c>
-      <c r="D49" s="45"/>
-      <c r="E49" s="44">
+      <c r="D49" s="36"/>
+      <c r="E49" s="35">
         <f>SUM(E42:E48)</f>
         <v>189.5</v>
       </c>
-      <c r="F49" s="45"/>
-      <c r="G49" s="44">
+      <c r="F49" s="36"/>
+      <c r="G49" s="35">
         <f>SUM(G42:G48)</f>
         <v>206.5</v>
       </c>
-      <c r="H49" s="45"/>
-      <c r="I49" s="44">
+      <c r="H49" s="36"/>
+      <c r="I49" s="35">
         <f>SUM(I42:I48)</f>
         <v>290.49999999999994</v>
       </c>
-      <c r="J49" s="45"/>
-      <c r="K49" s="44">
+      <c r="J49" s="36"/>
+      <c r="K49" s="35">
         <f>SUM(K42:K48)</f>
         <v>259.29999999999995</v>
       </c>
-      <c r="L49" s="45"/>
-      <c r="M49" s="44">
+      <c r="L49" s="36"/>
+      <c r="M49" s="35">
         <f>SUM(M42:M48)</f>
         <v>400.29999999999995</v>
       </c>
@@ -3282,57 +3517,57 @@
       <c r="B50" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C50" s="42">
+      <c r="C50" s="33">
         <v>252.5</v>
       </c>
-      <c r="D50" s="43"/>
-      <c r="E50" s="42">
+      <c r="D50" s="34"/>
+      <c r="E50" s="33">
         <v>258</v>
       </c>
-      <c r="F50" s="43"/>
-      <c r="G50" s="42">
+      <c r="F50" s="34"/>
+      <c r="G50" s="33">
         <v>334.9</v>
       </c>
-      <c r="H50" s="43"/>
-      <c r="I50" s="42">
+      <c r="H50" s="34"/>
+      <c r="I50" s="33">
         <v>300</v>
       </c>
-      <c r="J50" s="43"/>
-      <c r="K50" s="42">
+      <c r="J50" s="34"/>
+      <c r="K50" s="33">
         <v>340.7</v>
       </c>
-      <c r="L50" s="43"/>
-      <c r="M50" s="42">
+      <c r="L50" s="34"/>
+      <c r="M50" s="33">
         <v>545.6</v>
       </c>
-      <c r="N50" s="67"/>
-      <c r="P50" s="35"/>
+      <c r="N50" s="56"/>
+      <c r="P50" s="28"/>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C51" s="44">
+      <c r="C51" s="35">
         <v>0</v>
       </c>
-      <c r="D51" s="45"/>
-      <c r="E51" s="44">
+      <c r="D51" s="36"/>
+      <c r="E51" s="35">
         <v>0</v>
       </c>
-      <c r="F51" s="45"/>
-      <c r="G51" s="44">
+      <c r="F51" s="36"/>
+      <c r="G51" s="35">
         <v>44.7</v>
       </c>
-      <c r="H51" s="45"/>
-      <c r="I51" s="44">
+      <c r="H51" s="36"/>
+      <c r="I51" s="35">
         <v>51.4</v>
       </c>
-      <c r="J51" s="45"/>
-      <c r="K51" s="44">
+      <c r="J51" s="36"/>
+      <c r="K51" s="35">
         <v>53.4</v>
       </c>
-      <c r="L51" s="45"/>
-      <c r="M51" s="44">
+      <c r="L51" s="36"/>
+      <c r="M51" s="35">
         <v>69.2</v>
       </c>
     </row>
@@ -3340,27 +3575,27 @@
       <c r="B52" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C52" s="44">
+      <c r="C52" s="35">
         <v>66.8</v>
       </c>
-      <c r="D52" s="45"/>
-      <c r="E52" s="44">
+      <c r="D52" s="36"/>
+      <c r="E52" s="35">
         <v>20.7</v>
       </c>
-      <c r="F52" s="45"/>
-      <c r="G52" s="44">
+      <c r="F52" s="36"/>
+      <c r="G52" s="35">
         <v>27.6</v>
       </c>
-      <c r="H52" s="45"/>
-      <c r="I52" s="44">
+      <c r="H52" s="36"/>
+      <c r="I52" s="35">
         <v>45</v>
       </c>
-      <c r="J52" s="45"/>
-      <c r="K52" s="44">
+      <c r="J52" s="36"/>
+      <c r="K52" s="35">
         <v>10.1</v>
       </c>
-      <c r="L52" s="45"/>
-      <c r="M52" s="44">
+      <c r="L52" s="36"/>
+      <c r="M52" s="35">
         <v>0.7</v>
       </c>
     </row>
@@ -3368,27 +3603,27 @@
       <c r="B53" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="44">
+      <c r="C53" s="35">
         <v>11.4</v>
       </c>
-      <c r="D53" s="45"/>
-      <c r="E53" s="44">
+      <c r="D53" s="36"/>
+      <c r="E53" s="35">
         <v>9.6999999999999993</v>
       </c>
-      <c r="F53" s="45"/>
-      <c r="G53" s="44">
+      <c r="F53" s="36"/>
+      <c r="G53" s="35">
         <v>13.3</v>
       </c>
-      <c r="H53" s="45"/>
-      <c r="I53" s="44">
+      <c r="H53" s="36"/>
+      <c r="I53" s="35">
         <v>16.3</v>
       </c>
-      <c r="J53" s="45"/>
-      <c r="K53" s="44">
+      <c r="J53" s="36"/>
+      <c r="K53" s="35">
         <v>15.2</v>
       </c>
-      <c r="L53" s="45"/>
-      <c r="M53" s="44">
+      <c r="L53" s="36"/>
+      <c r="M53" s="35">
         <v>21.4</v>
       </c>
     </row>
@@ -3396,27 +3631,27 @@
       <c r="B54" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C54" s="44">
+      <c r="C54" s="35">
         <v>16.899999999999999</v>
       </c>
-      <c r="D54" s="45"/>
-      <c r="E54" s="44">
+      <c r="D54" s="36"/>
+      <c r="E54" s="35">
         <v>4.7</v>
       </c>
-      <c r="F54" s="45"/>
-      <c r="G54" s="44">
+      <c r="F54" s="36"/>
+      <c r="G54" s="35">
         <v>7.9</v>
       </c>
-      <c r="H54" s="45"/>
-      <c r="I54" s="44">
+      <c r="H54" s="36"/>
+      <c r="I54" s="35">
         <v>14.3</v>
       </c>
-      <c r="J54" s="45"/>
-      <c r="K54" s="44">
+      <c r="J54" s="36"/>
+      <c r="K54" s="35">
         <v>6.3</v>
       </c>
-      <c r="L54" s="45"/>
-      <c r="M54" s="44">
+      <c r="L54" s="36"/>
+      <c r="M54" s="35">
         <v>7.9</v>
       </c>
     </row>
@@ -3424,27 +3659,27 @@
       <c r="B55" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="44">
+      <c r="C55" s="35">
         <v>96</v>
       </c>
-      <c r="D55" s="45"/>
-      <c r="E55" s="44">
+      <c r="D55" s="36"/>
+      <c r="E55" s="35">
         <v>70.400000000000006</v>
       </c>
-      <c r="F55" s="45"/>
-      <c r="G55" s="44">
+      <c r="F55" s="36"/>
+      <c r="G55" s="35">
         <v>41.1</v>
       </c>
-      <c r="H55" s="45"/>
-      <c r="I55" s="44">
+      <c r="H55" s="36"/>
+      <c r="I55" s="35">
         <v>41.7</v>
       </c>
-      <c r="J55" s="45"/>
-      <c r="K55" s="44">
+      <c r="J55" s="36"/>
+      <c r="K55" s="35">
         <v>51.1</v>
       </c>
-      <c r="L55" s="45"/>
-      <c r="M55" s="44">
+      <c r="L55" s="36"/>
+      <c r="M55" s="35">
         <v>69.2</v>
       </c>
     </row>
@@ -3452,94 +3687,94 @@
       <c r="B56" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="44">
+      <c r="C56" s="35">
         <f>C49+SUM(C50:C55)</f>
         <v>589.5</v>
       </c>
-      <c r="D56" s="45"/>
-      <c r="E56" s="44">
+      <c r="D56" s="36"/>
+      <c r="E56" s="35">
         <f>E49+SUM(E50:E55)</f>
         <v>553</v>
       </c>
-      <c r="F56" s="45"/>
-      <c r="G56" s="44">
+      <c r="F56" s="36"/>
+      <c r="G56" s="35">
         <f>G49+SUM(G50:G55)</f>
         <v>676</v>
       </c>
-      <c r="H56" s="45"/>
-      <c r="I56" s="44">
+      <c r="H56" s="36"/>
+      <c r="I56" s="35">
         <f>I49+SUM(I50:I55)</f>
         <v>759.19999999999993</v>
       </c>
-      <c r="J56" s="45"/>
-      <c r="K56" s="44">
+      <c r="J56" s="36"/>
+      <c r="K56" s="35">
         <f>K49+SUM(K50:K55)</f>
         <v>736.09999999999991</v>
       </c>
-      <c r="L56" s="45"/>
-      <c r="M56" s="44">
+      <c r="L56" s="36"/>
+      <c r="M56" s="35">
         <f>M49+SUM(M50:M55)</f>
         <v>1114.3000000000002</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="M57" s="44"/>
-    </row>
-    <row r="58" spans="2:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="44" t="s">
+      <c r="M57" s="35"/>
+    </row>
+    <row r="58" spans="2:16" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="C58" s="44">
+      <c r="C58" s="35">
         <v>775.3</v>
       </c>
-      <c r="D58" s="45"/>
-      <c r="E58" s="44">
+      <c r="D58" s="36"/>
+      <c r="E58" s="35">
         <v>927.3</v>
       </c>
-      <c r="F58" s="45"/>
-      <c r="G58" s="44">
+      <c r="F58" s="36"/>
+      <c r="G58" s="35">
         <v>1067.5</v>
       </c>
-      <c r="H58" s="45"/>
-      <c r="I58" s="44">
+      <c r="H58" s="36"/>
+      <c r="I58" s="35">
         <v>1123</v>
       </c>
-      <c r="J58" s="45"/>
-      <c r="K58" s="44">
+      <c r="J58" s="36"/>
+      <c r="K58" s="35">
         <v>1277.0999999999999</v>
       </c>
-      <c r="L58" s="45"/>
-      <c r="M58" s="44">
+      <c r="L58" s="36"/>
+      <c r="M58" s="35">
         <v>1627</v>
       </c>
-      <c r="N58" s="62"/>
-      <c r="P58" s="45"/>
+      <c r="N58" s="51"/>
+      <c r="P58" s="36"/>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C59" s="44">
+      <c r="C59" s="35">
         <f>C58+C56</f>
         <v>1364.8</v>
       </c>
-      <c r="E59" s="44">
+      <c r="E59" s="35">
         <f>E58+E56</f>
         <v>1480.3</v>
       </c>
-      <c r="G59" s="44">
+      <c r="G59" s="35">
         <f>G58+G56</f>
         <v>1743.5</v>
       </c>
-      <c r="I59" s="44">
+      <c r="I59" s="35">
         <f>I58+I56</f>
         <v>1882.1999999999998</v>
       </c>
-      <c r="K59" s="44">
+      <c r="K59" s="35">
         <f>K58+K56</f>
         <v>2013.1999999999998</v>
       </c>
-      <c r="M59" s="44">
+      <c r="M59" s="35">
         <f>M58+M56</f>
         <v>2741.3</v>
       </c>
@@ -3548,27 +3783,27 @@
       <c r="B61" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C61" s="44">
+      <c r="C61" s="35">
         <f>C40-C56</f>
         <v>775.3</v>
       </c>
-      <c r="E61" s="44">
+      <c r="E61" s="35">
         <f>E40-E56</f>
         <v>927.30000000000018</v>
       </c>
-      <c r="G61" s="44">
+      <c r="G61" s="35">
         <f>G40-G56</f>
         <v>1067.5000000000002</v>
       </c>
-      <c r="I61" s="44">
+      <c r="I61" s="35">
         <f>I40-I56</f>
         <v>1123</v>
       </c>
-      <c r="K61" s="44">
+      <c r="K61" s="35">
         <f>K40-K56</f>
         <v>1277.1000000000004</v>
       </c>
-      <c r="M61" s="44">
+      <c r="M61" s="35">
         <f>M40-M56</f>
         <v>1627</v>
       </c>
@@ -3606,27 +3841,27 @@
       <c r="B64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="44">
+      <c r="C64" s="35">
         <f>C38+C39+C30</f>
         <v>75.7</v>
       </c>
-      <c r="E64" s="44">
+      <c r="E64" s="35">
         <f>E38+E39+E30</f>
         <v>70.600000000000009</v>
       </c>
-      <c r="G64" s="44">
+      <c r="G64" s="35">
         <f>G38+G39+G30</f>
         <v>89.600000000000009</v>
       </c>
-      <c r="I64" s="44">
+      <c r="I64" s="35">
         <f>I38+I39+I30</f>
         <v>130.70000000000002</v>
       </c>
-      <c r="K64" s="44">
+      <c r="K64" s="35">
         <f>K38+K39+K30</f>
         <v>141.6</v>
       </c>
-      <c r="M64" s="44">
+      <c r="M64" s="35">
         <f>M38+M39+M30</f>
         <v>234.4</v>
       </c>
@@ -3635,27 +3870,27 @@
       <c r="B65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C65" s="44">
+      <c r="C65" s="35">
         <f>C50+C42+C48</f>
         <v>253.1</v>
       </c>
-      <c r="E65" s="44">
+      <c r="E65" s="35">
         <f>E50+E42+E48</f>
         <v>261.5</v>
       </c>
-      <c r="G65" s="44">
+      <c r="G65" s="35">
         <f>G50+G42+G48</f>
         <v>337.29999999999995</v>
       </c>
-      <c r="I65" s="44">
+      <c r="I65" s="35">
         <f>I50+I42+I48</f>
         <v>377</v>
       </c>
-      <c r="K65" s="44">
+      <c r="K65" s="35">
         <f>K50+K42+K48</f>
         <v>546.79999999999995</v>
       </c>
-      <c r="M65" s="44">
+      <c r="M65" s="35">
         <f>M50+M42+M48</f>
         <v>802</v>
       </c>
@@ -3664,86 +3899,86 @@
       <c r="B66" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C66" s="44">
+      <c r="C66" s="35">
         <f>C64-C65</f>
         <v>-177.39999999999998</v>
       </c>
-      <c r="E66" s="44">
+      <c r="E66" s="35">
         <f>E64-E65</f>
         <v>-190.89999999999998</v>
       </c>
-      <c r="G66" s="44">
+      <c r="G66" s="35">
         <f>G64-G65</f>
         <v>-247.69999999999993</v>
       </c>
-      <c r="I66" s="44">
+      <c r="I66" s="35">
         <f>I64-I65</f>
         <v>-246.29999999999998</v>
       </c>
-      <c r="K66" s="44">
+      <c r="K66" s="35">
         <f>K64-K65</f>
         <v>-405.19999999999993</v>
       </c>
-      <c r="M66" s="44">
+      <c r="M66" s="35">
         <f>M64-M65</f>
         <v>-567.6</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="46" t="s">
+    <row r="68" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="46">
+      <c r="C68" s="37">
         <v>10.8497</v>
       </c>
-      <c r="D68" s="47"/>
-      <c r="E68" s="46">
+      <c r="D68" s="38"/>
+      <c r="E68" s="37">
         <v>14.0044</v>
       </c>
-      <c r="F68" s="47"/>
-      <c r="G68" s="46">
+      <c r="F68" s="38"/>
+      <c r="G68" s="37">
         <v>19.282</v>
       </c>
-      <c r="H68" s="47"/>
-      <c r="I68" s="46">
+      <c r="H68" s="38"/>
+      <c r="I68" s="37">
         <v>23.1129</v>
       </c>
-      <c r="J68" s="47"/>
-      <c r="K68" s="46">
+      <c r="J68" s="38"/>
+      <c r="K68" s="37">
         <v>28.1996</v>
       </c>
-      <c r="L68" s="47"/>
-      <c r="M68" s="46">
+      <c r="L68" s="38"/>
+      <c r="M68" s="37">
         <v>20.45</v>
       </c>
-      <c r="N68" s="63"/>
-      <c r="P68" s="47"/>
+      <c r="N68" s="52"/>
+      <c r="P68" s="38"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C69" s="44">
+      <c r="C69" s="35">
         <f>C68*C16</f>
         <v>4114.4161925447006</v>
       </c>
-      <c r="E69" s="44">
+      <c r="E69" s="35">
         <f>E68*E16</f>
         <v>5308.2794942492001</v>
       </c>
-      <c r="G69" s="44">
+      <c r="G69" s="35">
         <f>G68*G16</f>
         <v>7310.4731065340002</v>
       </c>
-      <c r="I69" s="44">
+      <c r="I69" s="35">
         <f>I68*I16</f>
         <v>8761.9267890080991</v>
       </c>
-      <c r="K69" s="44">
+      <c r="K69" s="35">
         <f>K68*K16</f>
         <v>10690.468360000001</v>
       </c>
-      <c r="M69" s="44">
+      <c r="M69" s="35">
         <f>M68*M16</f>
         <v>7734.19</v>
       </c>
@@ -3752,60 +3987,60 @@
       <c r="B70" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C70" s="44">
+      <c r="C70" s="35">
         <f>C69-C66</f>
         <v>4291.8161925447002</v>
       </c>
-      <c r="E70" s="44">
+      <c r="E70" s="35">
         <f>E69-E66</f>
         <v>5499.1794942491997</v>
       </c>
-      <c r="G70" s="44">
+      <c r="G70" s="35">
         <f>G69-G66</f>
         <v>7558.173106534</v>
       </c>
-      <c r="I70" s="44">
+      <c r="I70" s="35">
         <f>I69-I66</f>
         <v>9008.2267890080984</v>
       </c>
-      <c r="K70" s="44">
+      <c r="K70" s="35">
         <f>K69-K66</f>
         <v>11095.668360000001</v>
       </c>
-      <c r="M70" s="44">
+      <c r="M70" s="35">
         <f>M69-M66</f>
         <v>8301.7899999999991</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A72" s="56">
+      <c r="A72" s="47">
         <f>AVERAGE(C72:AZ72)</f>
         <v>6.467721604504824</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C72" s="53">
+      <c r="C72" s="44">
         <f>C68/C62</f>
         <v>5.306869847213596</v>
       </c>
-      <c r="E72" s="53">
+      <c r="E72" s="44">
         <f>E68/E62</f>
         <v>5.7244467747753687</v>
       </c>
-      <c r="G72" s="53">
+      <c r="G72" s="44">
         <f>G68/G62</f>
         <v>6.8482183667765799</v>
       </c>
-      <c r="I72" s="53">
+      <c r="I72" s="44">
         <f>I68/I62</f>
         <v>7.8022500347356187</v>
       </c>
-      <c r="K72" s="53">
+      <c r="K72" s="44">
         <f>K68/K62</f>
         <v>8.3708937123169669</v>
       </c>
-      <c r="M72" s="53">
+      <c r="M72" s="44">
         <f>M68/M62</f>
         <v>4.7536508912108166</v>
       </c>
@@ -3829,7 +4064,7 @@
       <c r="B76" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M76" s="48"/>
+      <c r="M76" s="39"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
@@ -3841,9 +4076,13 @@
     <hyperlink ref="M1" r:id="rId1" xr:uid="{64230965-EEC2-4818-9500-5E49F2C6FBF5}"/>
     <hyperlink ref="I1" r:id="rId2" xr:uid="{879E0608-9977-4013-9DB7-7908B60FAFB2}"/>
     <hyperlink ref="E1" r:id="rId3" xr:uid="{D2F2E719-2F49-4057-B46A-7E29B8F345FA}"/>
+    <hyperlink ref="V1" r:id="rId4" xr:uid="{312EC780-3433-42F0-97FF-0788993E5A29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
+  <ignoredErrors>
+    <ignoredError sqref="L10" formula="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More historical financial data & metric calcs for £HLMA
</commit_message>
<xml_diff>
--- a/£HLMA.xlsx
+++ b/£HLMA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCEC658-60C6-4427-8114-C84A3E5A4D1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43140AF5-4A44-E94B-A72A-B74F09545752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28470" windowHeight="11790" activeTab="1" xr2:uid="{1821E3F4-C005-474E-95BC-C5AE66A060FF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{1821E3F4-C005-474E-95BC-C5AE66A060FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="110">
   <si>
     <t>£HLMA</t>
   </si>
@@ -353,6 +363,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>FY16</t>
   </si>
 </sst>
 </file>
@@ -363,7 +376,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +461,13 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -589,7 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -685,12 +705,16 @@
     <xf numFmtId="9" fontId="11" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="16" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -706,6 +730,12 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,13 +748,7 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -870,13 +894,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>110</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -1224,12 +1248,12 @@
       <selection activeCell="C29" sqref="C29:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1244,34 +1268,34 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="61" t="s">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B5" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="63"/>
-      <c r="G5" s="61" t="s">
+      <c r="C5" s="64"/>
+      <c r="D5" s="65"/>
+      <c r="G5" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="63"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="64"/>
+      <c r="S5" s="65"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1293,7 +1317,7 @@
       <c r="R6" s="12"/>
       <c r="S6" s="13"/>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1319,7 +1343,7 @@
       <c r="R7" s="12"/>
       <c r="S7" s="13"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1342,7 +1366,7 @@
       <c r="R8" s="12"/>
       <c r="S8" s="13"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1368,7 +1392,7 @@
       <c r="R9" s="12"/>
       <c r="S9" s="13"/>
     </row>
-    <row r="10" spans="2:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1394,7 +1418,7 @@
       <c r="R10" s="12"/>
       <c r="S10" s="13"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1420,7 +1444,7 @@
       <c r="R11" s="12"/>
       <c r="S11" s="13"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
@@ -1443,7 +1467,7 @@
       <c r="R12" s="12"/>
       <c r="S12" s="13"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.15">
       <c r="G13" s="19"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -1458,7 +1482,7 @@
       <c r="R13" s="12"/>
       <c r="S13" s="13"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.15">
       <c r="G14" s="19"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -1473,12 +1497,12 @@
       <c r="R14" s="12"/>
       <c r="S14" s="13"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="61" t="s">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B15" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="65"/>
       <c r="G15" s="19"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -1493,14 +1517,14 @@
       <c r="R15" s="12"/>
       <c r="S15" s="13"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="58"/>
+      <c r="D16" s="67"/>
       <c r="G16" s="19"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -1515,14 +1539,14 @@
       <c r="R16" s="12"/>
       <c r="S16" s="13"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="58"/>
+      <c r="D17" s="67"/>
       <c r="G17" s="19"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -1537,12 +1561,12 @@
       <c r="R17" s="12"/>
       <c r="S17" s="13"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="67"/>
       <c r="G18" s="19"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -1557,12 +1581,12 @@
       <c r="R18" s="12"/>
       <c r="S18" s="13"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="62"/>
       <c r="G19" s="19"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -1577,7 +1601,7 @@
       <c r="R19" s="12"/>
       <c r="S19" s="13"/>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.15">
       <c r="G20" s="19"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -1592,7 +1616,7 @@
       <c r="R20" s="12"/>
       <c r="S20" s="13"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.15">
       <c r="G21" s="19"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -1607,12 +1631,12 @@
       <c r="R21" s="12"/>
       <c r="S21" s="13"/>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="61" t="s">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B22" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="63"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="65"/>
       <c r="G22" s="19"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -1627,14 +1651,14 @@
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B23" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="58"/>
+      <c r="D23" s="67"/>
       <c r="G23" s="19"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -1649,14 +1673,14 @@
       <c r="R23" s="12"/>
       <c r="S23" s="13"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="57">
+      <c r="C24" s="66">
         <v>1894</v>
       </c>
-      <c r="D24" s="58"/>
+      <c r="D24" s="67"/>
       <c r="G24" s="19"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -1671,10 +1695,10 @@
       <c r="R24" s="12"/>
       <c r="S24" s="13"/>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B25" s="17"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="67"/>
       <c r="G25" s="19"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -1689,10 +1713,10 @@
       <c r="R25" s="12"/>
       <c r="S25" s="13"/>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B26" s="17"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="67"/>
       <c r="G26" s="19"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -1707,10 +1731,10 @@
       <c r="R26" s="12"/>
       <c r="S26" s="13"/>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B27" s="17"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="67"/>
       <c r="G27" s="19"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -1725,7 +1749,7 @@
       <c r="R27" s="12"/>
       <c r="S27" s="13"/>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B28" s="17" t="s">
         <v>19</v>
       </c>
@@ -1749,14 +1773,14 @@
       <c r="R28" s="12"/>
       <c r="S28" s="13"/>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B29" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="65"/>
+      <c r="D29" s="69"/>
       <c r="G29" s="19"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -1771,7 +1795,7 @@
       <c r="R29" s="12"/>
       <c r="S29" s="13"/>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.15">
       <c r="G30" s="19"/>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -1786,7 +1810,7 @@
       <c r="R30" s="12"/>
       <c r="S30" s="13"/>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.15">
       <c r="G31" s="19"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -1801,12 +1825,12 @@
       <c r="R31" s="12"/>
       <c r="S31" s="13"/>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B32" s="61" t="s">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B32" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="63"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="65"/>
       <c r="G32" s="19"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -1821,15 +1845,15 @@
       <c r="R32" s="12"/>
       <c r="S32" s="13"/>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B33" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="66">
+      <c r="C33" s="70">
         <f>C6/'Financial Model'!M62</f>
         <v>5.24180086047941</v>
       </c>
-      <c r="D33" s="67"/>
+      <c r="D33" s="71"/>
       <c r="G33" s="19"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
@@ -1844,12 +1868,15 @@
       <c r="R33" s="12"/>
       <c r="S33" s="13"/>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B34" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="58"/>
+      <c r="C34" s="70">
+        <f>C8/SUM('Financial Model'!L4:M4)</f>
+        <v>5.1264787208463574</v>
+      </c>
+      <c r="D34" s="71"/>
       <c r="G34" s="19"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
@@ -1864,12 +1891,12 @@
       <c r="R34" s="12"/>
       <c r="S34" s="13"/>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B35" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="58"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="67"/>
       <c r="G35" s="19"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
@@ -1884,12 +1911,15 @@
       <c r="R35" s="12"/>
       <c r="S35" s="13"/>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B36" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="58"/>
+      <c r="C36" s="70">
+        <f>C6/SUM('Financial Model'!L15:M15)</f>
+        <v>38.217128200795514</v>
+      </c>
+      <c r="D36" s="71"/>
       <c r="G36" s="19"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
@@ -1904,12 +1934,12 @@
       <c r="R36" s="12"/>
       <c r="S36" s="13"/>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B37" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="58"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="67"/>
       <c r="G37" s="19"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
@@ -1924,12 +1954,12 @@
       <c r="R37" s="12"/>
       <c r="S37" s="13"/>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B38" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="60"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="62"/>
       <c r="G38" s="21"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
@@ -1946,6 +1976,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="G5:S5"/>
     <mergeCell ref="C16:D16"/>
@@ -1962,11 +1997,6 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{14EC5317-C73B-4350-A09D-C7641F7FCA8D}"/>
@@ -1979,37 +2009,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F5332D-7B2B-4D46-8BAA-4FBC91F2AA00}">
-  <dimension ref="A1:AJ77"/>
+  <dimension ref="A1:AK77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M19" sqref="L19:M19"/>
+      <selection pane="bottomRight" activeCell="W77" sqref="V77:W77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="9.140625" style="29"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9.140625" style="29"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="29"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.140625" style="29"/>
-    <col min="11" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="9.140625" style="29"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="9.140625" style="55"/>
-    <col min="15" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="9.140625" style="29"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="9.1640625" style="29"/>
+    <col min="5" max="5" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="9.1640625" style="29"/>
+    <col min="7" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="9.1640625" style="29"/>
+    <col min="9" max="9" width="9.1640625" style="1"/>
+    <col min="10" max="10" width="9.1640625" style="29"/>
+    <col min="11" max="11" width="9.1640625" style="1"/>
+    <col min="12" max="12" width="9.1640625" style="29"/>
+    <col min="13" max="13" width="9.1640625" style="1"/>
+    <col min="14" max="14" width="9.1640625" style="55"/>
+    <col min="15" max="15" width="9.1640625" style="1"/>
+    <col min="16" max="16" width="9.1640625" style="29"/>
+    <col min="17" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:36" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:37" s="22" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="C1" s="22" t="s">
         <v>105</v>
       </c>
@@ -2053,86 +2083,101 @@
         <v>45</v>
       </c>
       <c r="R1" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="S1" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="T1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="U1" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="V1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="30" t="s">
+      <c r="W1" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="22" t="s">
+      <c r="X1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="X1" s="22" t="s">
+      <c r="Y1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="22" t="s">
+      <c r="Z1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="Z1" s="22" t="s">
+      <c r="AA1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AA1" s="22" t="s">
+      <c r="AB1" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="22" t="s">
+      <c r="AC1" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="AC1" s="22" t="s">
+      <c r="AD1" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="22" t="s">
+      <c r="AE1" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="AE1" s="22" t="s">
+      <c r="AF1" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="22" t="s">
+      <c r="AG1" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="AG1" s="22" t="s">
+      <c r="AH1" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AH1" s="22" t="s">
+      <c r="AI1" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AI1" s="22" t="s">
+      <c r="AJ1" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AJ1" s="22" t="s">
+      <c r="AK1" s="22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:36" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:37" s="24" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B2" s="23"/>
       <c r="C2" s="32">
         <v>43008</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="27">
+        <f>S2</f>
+        <v>0</v>
+      </c>
       <c r="E2" s="32">
         <v>43373</v>
       </c>
-      <c r="F2" s="27"/>
+      <c r="F2" s="58">
+        <f>T2</f>
+        <v>43555</v>
+      </c>
       <c r="G2" s="32">
         <v>43738</v>
       </c>
-      <c r="H2" s="27"/>
+      <c r="H2" s="58">
+        <f>U2</f>
+        <v>43921</v>
+      </c>
       <c r="I2" s="32">
         <v>44104</v>
       </c>
-      <c r="J2" s="27"/>
+      <c r="J2" s="58">
+        <f>V2</f>
+        <v>44286</v>
+      </c>
       <c r="K2" s="32">
         <v>44469</v>
       </c>
-      <c r="L2" s="69">
-        <f>V2</f>
+      <c r="L2" s="58">
+        <f>W2</f>
         <v>44651</v>
       </c>
       <c r="M2" s="32">
@@ -2140,27 +2185,36 @@
       </c>
       <c r="N2" s="49"/>
       <c r="P2" s="27"/>
+      <c r="T2" s="32">
+        <v>43555</v>
+      </c>
       <c r="U2" s="32">
+        <v>43921</v>
+      </c>
+      <c r="V2" s="32">
         <v>44286</v>
       </c>
-      <c r="V2" s="32">
+      <c r="W2" s="32">
         <v>44651</v>
       </c>
     </row>
-    <row r="3" spans="2:36" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:37" s="24" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B3" s="23"/>
       <c r="D3" s="27"/>
       <c r="E3" s="31">
         <v>44885</v>
       </c>
       <c r="F3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="H3" s="59">
+        <f>U3</f>
+        <v>44756</v>
+      </c>
       <c r="I3" s="31">
         <v>44884</v>
       </c>
       <c r="J3" s="27"/>
-      <c r="L3" s="70">
-        <f>V3</f>
+      <c r="L3" s="59">
+        <f>W3</f>
         <v>44728</v>
       </c>
       <c r="M3" s="31">
@@ -2168,35 +2222,50 @@
       </c>
       <c r="N3" s="49"/>
       <c r="P3" s="27"/>
-      <c r="V3" s="31">
+      <c r="U3" s="31">
+        <v>44756</v>
+      </c>
+      <c r="W3" s="31">
         <v>44728</v>
       </c>
     </row>
-    <row r="4" spans="2:36" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:37" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="33" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="33">
         <v>506.3</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="34">
+        <f>S4-C4</f>
+        <v>-506.3</v>
+      </c>
       <c r="E4" s="33">
         <v>585.5</v>
       </c>
-      <c r="F4" s="34"/>
+      <c r="F4" s="34">
+        <f>T4-E4</f>
+        <v>625.40000000000009</v>
+      </c>
       <c r="G4" s="33">
         <v>653.70000000000005</v>
       </c>
-      <c r="H4" s="34"/>
+      <c r="H4" s="34">
+        <f>U4-G4</f>
+        <v>684.7</v>
+      </c>
       <c r="I4" s="33">
         <v>618.4</v>
       </c>
-      <c r="J4" s="34"/>
+      <c r="J4" s="34">
+        <f>V4-I4</f>
+        <v>699.80000000000007</v>
+      </c>
       <c r="K4" s="33">
         <v>737.2</v>
       </c>
       <c r="L4" s="34">
-        <f>V4-K4</f>
+        <f t="shared" ref="L4:L9" si="0">W4-K4</f>
         <v>788.09999999999991</v>
       </c>
       <c r="M4" s="33">
@@ -2204,38 +2273,56 @@
       </c>
       <c r="N4" s="50"/>
       <c r="P4" s="34"/>
+      <c r="T4" s="33">
+        <v>1210.9000000000001</v>
+      </c>
       <c r="U4" s="33">
+        <v>1338.4</v>
+      </c>
+      <c r="V4" s="33">
         <v>1318.2</v>
       </c>
-      <c r="V4" s="33">
+      <c r="W4" s="33">
         <v>1525.3</v>
       </c>
     </row>
-    <row r="5" spans="2:36" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:37" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="33" t="s">
         <v>64</v>
       </c>
       <c r="C5" s="33">
         <v>81.8</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="34">
+        <f>S5-C5</f>
+        <v>-81.8</v>
+      </c>
       <c r="E5" s="33">
         <v>100.4</v>
       </c>
-      <c r="F5" s="34"/>
+      <c r="F5" s="34">
+        <f>T5-E5</f>
+        <v>117.4</v>
+      </c>
       <c r="G5" s="33">
         <v>111.6</v>
       </c>
-      <c r="H5" s="34"/>
+      <c r="H5" s="34">
+        <f>U5-G5</f>
+        <v>121.80000000000001</v>
+      </c>
       <c r="I5" s="33">
         <v>102.1</v>
       </c>
-      <c r="J5" s="34"/>
+      <c r="J5" s="34">
+        <f>V5-I5</f>
+        <v>138.70000000000002</v>
+      </c>
       <c r="K5" s="33">
         <v>137.6</v>
       </c>
       <c r="L5" s="34">
-        <f>V5-K5</f>
+        <f t="shared" si="0"/>
         <v>141.29999999999998</v>
       </c>
       <c r="M5" s="33">
@@ -2243,38 +2330,56 @@
       </c>
       <c r="N5" s="50"/>
       <c r="P5" s="34"/>
+      <c r="T5" s="33">
+        <v>217.8</v>
+      </c>
       <c r="U5" s="33">
+        <v>233.4</v>
+      </c>
+      <c r="V5" s="33">
         <v>240.8</v>
       </c>
-      <c r="V5" s="33">
+      <c r="W5" s="33">
         <v>278.89999999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="35" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="35">
         <v>-0.1</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="36">
+        <f>S6-C6</f>
+        <v>0.1</v>
+      </c>
       <c r="E6" s="35">
         <v>-0.1</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="36">
+        <f>T6-E6</f>
+        <v>0</v>
+      </c>
       <c r="G6" s="35">
         <v>-0.1</v>
       </c>
-      <c r="H6" s="36"/>
+      <c r="H6" s="36">
+        <f>U6-G6</f>
+        <v>0</v>
+      </c>
       <c r="I6" s="35">
         <v>0</v>
       </c>
-      <c r="J6" s="36"/>
+      <c r="J6" s="36">
+        <f>V6-I6</f>
+        <v>0</v>
+      </c>
       <c r="K6" s="35">
         <v>-0.1</v>
       </c>
       <c r="L6" s="36">
-        <f>V6-K6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M6" s="35">
@@ -2282,38 +2387,56 @@
       </c>
       <c r="N6" s="51"/>
       <c r="P6" s="36"/>
+      <c r="T6" s="35">
+        <v>-0.1</v>
+      </c>
       <c r="U6" s="35">
+        <v>-0.1</v>
+      </c>
+      <c r="V6" s="35">
         <v>0</v>
       </c>
-      <c r="V6" s="35">
+      <c r="W6" s="35">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="7" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B7" s="35" t="s">
         <v>66</v>
       </c>
       <c r="C7" s="35">
         <v>0</v>
       </c>
-      <c r="D7" s="36"/>
+      <c r="D7" s="36">
+        <f t="shared" ref="D7:D11" si="1">S7-C7</f>
+        <v>0</v>
+      </c>
       <c r="E7" s="35">
         <v>-0.9</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="36">
+        <f t="shared" ref="F7:F11" si="2">T7-E7</f>
+        <v>-9.9999999999999978E-2</v>
+      </c>
       <c r="G7" s="35">
         <v>0</v>
       </c>
-      <c r="H7" s="36"/>
+      <c r="H7" s="36">
+        <f t="shared" ref="H7:H11" si="3">U7-G7</f>
+        <v>2.9</v>
+      </c>
       <c r="I7" s="35">
         <v>0</v>
       </c>
-      <c r="J7" s="36"/>
+      <c r="J7" s="36">
+        <f t="shared" ref="J7:J11" si="4">V7-I7</f>
+        <v>22.1</v>
+      </c>
       <c r="K7" s="35">
         <v>34</v>
       </c>
       <c r="L7" s="36">
-        <f>V7-K7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M7" s="35">
@@ -2321,38 +2444,56 @@
       </c>
       <c r="N7" s="51"/>
       <c r="P7" s="36"/>
+      <c r="T7" s="35">
+        <v>-1</v>
+      </c>
       <c r="U7" s="35">
+        <v>2.9</v>
+      </c>
+      <c r="V7" s="35">
         <v>22.1</v>
       </c>
-      <c r="V7" s="35">
+      <c r="W7" s="35">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B8" s="35" t="s">
         <v>67</v>
       </c>
       <c r="C8" s="35">
         <v>0.1</v>
       </c>
-      <c r="D8" s="36"/>
+      <c r="D8" s="36">
+        <f t="shared" si="1"/>
+        <v>-0.1</v>
+      </c>
       <c r="E8" s="35">
         <v>0.1</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="36">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
       <c r="G8" s="35">
         <v>0.4</v>
       </c>
-      <c r="H8" s="36"/>
+      <c r="H8" s="36">
+        <f t="shared" si="3"/>
+        <v>0.19999999999999996</v>
+      </c>
       <c r="I8" s="35">
         <v>1</v>
       </c>
-      <c r="J8" s="36"/>
+      <c r="J8" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="K8" s="35">
         <v>0.6</v>
       </c>
       <c r="L8" s="36">
-        <f>V8-K8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M8" s="35">
@@ -2360,38 +2501,56 @@
       </c>
       <c r="N8" s="51"/>
       <c r="P8" s="36"/>
+      <c r="T8" s="35">
+        <v>0.5</v>
+      </c>
       <c r="U8" s="35">
+        <v>0.6</v>
+      </c>
+      <c r="V8" s="35">
         <v>1</v>
       </c>
-      <c r="V8" s="35">
+      <c r="W8" s="35">
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B9" s="35" t="s">
         <v>68</v>
       </c>
       <c r="C9" s="35">
         <v>5</v>
       </c>
-      <c r="D9" s="36"/>
+      <c r="D9" s="36">
+        <f t="shared" si="1"/>
+        <v>-5</v>
+      </c>
       <c r="E9" s="35">
         <v>5</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="36">
+        <f t="shared" si="2"/>
+        <v>5.5</v>
+      </c>
       <c r="G9" s="35">
         <v>6.1</v>
       </c>
-      <c r="H9" s="36"/>
+      <c r="H9" s="36">
+        <f t="shared" si="3"/>
+        <v>6.6</v>
+      </c>
       <c r="I9" s="35">
         <v>6.8</v>
       </c>
-      <c r="J9" s="36"/>
+      <c r="J9" s="36">
+        <f t="shared" si="4"/>
+        <v>4.2</v>
+      </c>
       <c r="K9" s="35">
         <v>4.5999999999999996</v>
       </c>
       <c r="L9" s="36">
-        <f>V9-K9</f>
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="M9" s="35">
@@ -2399,85 +2558,123 @@
       </c>
       <c r="N9" s="51"/>
       <c r="P9" s="36"/>
+      <c r="T9" s="35">
+        <v>10.5</v>
+      </c>
       <c r="U9" s="35">
+        <v>12.7</v>
+      </c>
+      <c r="V9" s="35">
         <v>11</v>
       </c>
-      <c r="V9" s="35">
+      <c r="W9" s="35">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B10" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C10" s="35">
-        <f>C5+C6+C7+C8-C9</f>
+        <f t="shared" ref="C10:M10" si="5">C5+C6+C7+C8-C9</f>
         <v>76.8</v>
       </c>
-      <c r="D10" s="36"/>
+      <c r="D10" s="36">
+        <f t="shared" si="5"/>
+        <v>-76.8</v>
+      </c>
       <c r="E10" s="35">
-        <f>E5+E6+E7+E8-E9</f>
+        <f t="shared" si="5"/>
         <v>94.5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="36">
+        <f t="shared" si="5"/>
+        <v>112.20000000000002</v>
+      </c>
       <c r="G10" s="35">
-        <f>G5+G6+G7+G8-G9</f>
+        <f t="shared" si="5"/>
         <v>105.80000000000001</v>
       </c>
-      <c r="H10" s="36"/>
+      <c r="H10" s="36">
+        <f t="shared" si="5"/>
+        <v>118.30000000000003</v>
+      </c>
       <c r="I10" s="35">
-        <f>I5+I6+I7+I8-I9</f>
+        <f t="shared" si="5"/>
         <v>96.3</v>
       </c>
-      <c r="J10" s="36"/>
+      <c r="J10" s="36">
+        <f t="shared" si="5"/>
+        <v>156.60000000000002</v>
+      </c>
       <c r="K10" s="35">
-        <f>K5+K6+K7+K8-K9</f>
+        <f t="shared" si="5"/>
         <v>167.5</v>
       </c>
       <c r="L10" s="36">
-        <f>L5+L6+L7+L8-L9</f>
+        <f t="shared" si="5"/>
         <v>136.89999999999998</v>
       </c>
       <c r="M10" s="35">
-        <f>M5+M6+M7+M8-M9</f>
+        <f t="shared" si="5"/>
         <v>145.5</v>
       </c>
       <c r="N10" s="51"/>
       <c r="P10" s="36"/>
+      <c r="T10" s="35">
+        <f>T5+T6+T7+T8-T9</f>
+        <v>206.70000000000002</v>
+      </c>
       <c r="U10" s="35">
         <f>U5+U6+U7+U8-U9</f>
-        <v>252.90000000000003</v>
+        <v>224.10000000000002</v>
       </c>
       <c r="V10" s="35">
         <f>V5+V6+V7+V8-V9</f>
+        <v>252.90000000000003</v>
+      </c>
+      <c r="W10" s="35">
+        <f>W5+W6+W7+W8-W9</f>
         <v>304.39999999999998</v>
       </c>
     </row>
-    <row r="11" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B11" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="35">
         <v>15.1</v>
       </c>
-      <c r="D11" s="36"/>
+      <c r="D11" s="36">
+        <f t="shared" si="1"/>
+        <v>-15.1</v>
+      </c>
       <c r="E11" s="35">
         <v>19.899999999999999</v>
       </c>
-      <c r="F11" s="36"/>
+      <c r="F11" s="36">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
       <c r="G11" s="35">
         <v>20.8</v>
       </c>
-      <c r="H11" s="36"/>
+      <c r="H11" s="36">
+        <f t="shared" si="3"/>
+        <v>18.900000000000002</v>
+      </c>
       <c r="I11" s="35">
         <v>19</v>
       </c>
-      <c r="J11" s="36"/>
+      <c r="J11" s="36">
+        <f t="shared" si="4"/>
+        <v>30.6</v>
+      </c>
       <c r="K11" s="35">
         <v>31.8</v>
       </c>
       <c r="L11" s="36">
-        <f>V11-K11</f>
+        <f>W11-K11</f>
         <v>28.400000000000002</v>
       </c>
       <c r="M11" s="35">
@@ -2485,132 +2682,190 @@
       </c>
       <c r="N11" s="51"/>
       <c r="P11" s="36"/>
+      <c r="T11" s="35">
+        <v>36.9</v>
+      </c>
       <c r="U11" s="35">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="V11" s="35">
         <v>49.6</v>
       </c>
-      <c r="V11" s="35">
+      <c r="W11" s="35">
         <v>60.2</v>
       </c>
     </row>
-    <row r="12" spans="2:36" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:37" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B12" s="33" t="s">
         <v>71</v>
       </c>
       <c r="C12" s="33">
-        <f>C10-C11</f>
+        <f t="shared" ref="C12:M12" si="6">C10-C11</f>
         <v>61.699999999999996</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="34">
+        <f t="shared" si="6"/>
+        <v>-61.699999999999996</v>
+      </c>
       <c r="E12" s="33">
-        <f>E10-E11</f>
+        <f t="shared" si="6"/>
         <v>74.599999999999994</v>
       </c>
-      <c r="F12" s="34"/>
+      <c r="F12" s="34">
+        <f t="shared" si="6"/>
+        <v>95.200000000000017</v>
+      </c>
       <c r="G12" s="33">
-        <f>G10-G11</f>
+        <f t="shared" si="6"/>
         <v>85.000000000000014</v>
       </c>
-      <c r="H12" s="34"/>
+      <c r="H12" s="34">
+        <f t="shared" si="6"/>
+        <v>99.40000000000002</v>
+      </c>
       <c r="I12" s="33">
-        <f>I10-I11</f>
+        <f t="shared" si="6"/>
         <v>77.3</v>
       </c>
-      <c r="J12" s="34"/>
+      <c r="J12" s="34">
+        <f t="shared" si="6"/>
+        <v>126.00000000000003</v>
+      </c>
       <c r="K12" s="33">
-        <f>K10-K11</f>
+        <f t="shared" si="6"/>
         <v>135.69999999999999</v>
       </c>
       <c r="L12" s="34">
-        <f>L10-L11</f>
+        <f t="shared" si="6"/>
         <v>108.49999999999997</v>
       </c>
       <c r="M12" s="33">
-        <f>M10-M11</f>
+        <f t="shared" si="6"/>
         <v>114.8</v>
       </c>
       <c r="N12" s="50"/>
       <c r="P12" s="34"/>
+      <c r="T12" s="33">
+        <f>T10-T11</f>
+        <v>169.8</v>
+      </c>
       <c r="U12" s="33">
         <f>U10-U11</f>
-        <v>203.30000000000004</v>
+        <v>184.40000000000003</v>
       </c>
       <c r="V12" s="33">
         <f>V10-V11</f>
+        <v>203.30000000000004</v>
+      </c>
+      <c r="W12" s="33">
+        <f>W10-W11</f>
         <v>244.2</v>
       </c>
     </row>
-    <row r="13" spans="2:36" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:37" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B13" s="35" t="s">
         <v>74</v>
       </c>
       <c r="C13" s="33">
-        <f>C12+C14</f>
+        <f t="shared" ref="C13:M13" si="7">C12+C14</f>
         <v>61.699999999999996</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="34">
+        <f t="shared" si="7"/>
+        <v>-61.699999999999996</v>
+      </c>
       <c r="E13" s="33">
-        <f>E12+E14</f>
+        <f t="shared" si="7"/>
         <v>74.599999999999994</v>
       </c>
-      <c r="F13" s="34"/>
+      <c r="F13" s="34">
+        <f t="shared" si="7"/>
+        <v>95.200000000000017</v>
+      </c>
       <c r="G13" s="33">
-        <f>G12+G14</f>
+        <f t="shared" si="7"/>
         <v>85.000000000000014</v>
       </c>
-      <c r="H13" s="34"/>
+      <c r="H13" s="34">
+        <f t="shared" si="7"/>
+        <v>99.40000000000002</v>
+      </c>
       <c r="I13" s="33">
-        <f>I12+I14</f>
+        <f t="shared" si="7"/>
         <v>77.3</v>
       </c>
-      <c r="J13" s="34"/>
+      <c r="J13" s="34">
+        <f t="shared" si="7"/>
+        <v>125.90000000000003</v>
+      </c>
       <c r="K13" s="33">
-        <f>K12+K14</f>
+        <f t="shared" si="7"/>
         <v>135.79999999999998</v>
       </c>
       <c r="L13" s="34">
-        <f>L12+L14</f>
+        <f t="shared" si="7"/>
         <v>108.19999999999997</v>
       </c>
       <c r="M13" s="33">
-        <f>M12+M14</f>
+        <f t="shared" si="7"/>
         <v>115</v>
       </c>
       <c r="N13" s="50"/>
       <c r="P13" s="34"/>
+      <c r="T13" s="33">
+        <f>T12+T14</f>
+        <v>169.8</v>
+      </c>
       <c r="U13" s="33">
         <f>U12+U14</f>
-        <v>203.20000000000005</v>
+        <v>184.40000000000003</v>
       </c>
       <c r="V13" s="33">
         <f>V12+V14</f>
+        <v>203.20000000000005</v>
+      </c>
+      <c r="W13" s="33">
+        <f>W12+W14</f>
         <v>244</v>
       </c>
     </row>
-    <row r="14" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C14" s="46">
         <v>0</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="36">
+        <f>S14-C14</f>
+        <v>0</v>
+      </c>
       <c r="E14" s="46">
         <v>0</v>
       </c>
-      <c r="F14" s="36"/>
+      <c r="F14" s="36">
+        <f>T14-E14</f>
+        <v>0</v>
+      </c>
       <c r="G14" s="46">
         <v>0</v>
       </c>
-      <c r="H14" s="36"/>
+      <c r="H14" s="36">
+        <f t="shared" ref="H14" si="8">U14-G14</f>
+        <v>0</v>
+      </c>
       <c r="I14" s="46">
         <v>0</v>
       </c>
-      <c r="J14" s="36"/>
+      <c r="J14" s="36">
+        <f>V14-I14</f>
+        <v>-0.1</v>
+      </c>
       <c r="K14" s="35">
         <v>0.1</v>
       </c>
       <c r="L14" s="36">
-        <f>V14-K14</f>
+        <f>W14-K14</f>
         <v>-0.30000000000000004</v>
       </c>
       <c r="M14" s="35">
@@ -2618,85 +2873,126 @@
       </c>
       <c r="N14" s="51"/>
       <c r="P14" s="36"/>
+      <c r="S14" s="35">
+        <v>0</v>
+      </c>
+      <c r="T14" s="35">
+        <v>0</v>
+      </c>
       <c r="U14" s="35">
+        <v>0</v>
+      </c>
+      <c r="V14" s="35">
         <v>-0.1</v>
       </c>
-      <c r="V14" s="35">
+      <c r="W14" s="35">
         <v>-0.2</v>
       </c>
     </row>
-    <row r="15" spans="2:36" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:37" s="37" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="37" t="s">
         <v>73</v>
       </c>
       <c r="C15" s="37">
-        <f>C12/C16</f>
+        <f t="shared" ref="C15:M15" si="9">C12/C16</f>
         <v>0.16270266756508422</v>
       </c>
-      <c r="D15" s="38"/>
+      <c r="D15" s="38" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E15" s="37">
-        <f>E12/E16</f>
+        <f t="shared" si="9"/>
         <v>0.19681108372907286</v>
       </c>
-      <c r="F15" s="38"/>
+      <c r="F15" s="38">
+        <f t="shared" si="9"/>
+        <v>0.25108149993397905</v>
+      </c>
       <c r="G15" s="37">
-        <f>G12/G16</f>
+        <f t="shared" si="9"/>
         <v>0.22419479233636896</v>
       </c>
-      <c r="H15" s="38"/>
+      <c r="H15" s="38">
+        <f t="shared" si="9"/>
+        <v>0.26220905435668357</v>
+      </c>
       <c r="I15" s="37">
-        <f>I12/I16</f>
+        <f t="shared" si="9"/>
         <v>0.20390802308932054</v>
       </c>
-      <c r="J15" s="38"/>
+      <c r="J15" s="38">
+        <f t="shared" si="9"/>
+        <v>0.33271719038817016</v>
+      </c>
       <c r="K15" s="37">
-        <f>K12/K16</f>
+        <f t="shared" si="9"/>
         <v>0.35795304668952777</v>
       </c>
       <c r="L15" s="38">
-        <f>L12/L16</f>
+        <f t="shared" si="9"/>
         <v>0.28650646950092412</v>
       </c>
       <c r="M15" s="37">
-        <f>M12/M16</f>
+        <f t="shared" si="9"/>
         <v>0.30354309888947645</v>
       </c>
       <c r="N15" s="52"/>
       <c r="P15" s="38"/>
+      <c r="T15" s="37">
+        <f t="shared" ref="T15:U15" si="10">T12/T16</f>
+        <v>0.44783233916795839</v>
+      </c>
       <c r="U15" s="37">
-        <f>U12/U16</f>
-        <v>0.53612869198312252</v>
+        <f t="shared" si="10"/>
+        <v>0.48643208876632238</v>
       </c>
       <c r="V15" s="37">
         <f>V12/V16</f>
+        <v>0.53612869198312252</v>
+      </c>
+      <c r="W15" s="37">
+        <f>W12/W16</f>
         <v>0.6448376023237391</v>
       </c>
     </row>
-    <row r="16" spans="2:36" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="35">
         <v>379.21935100000002</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" s="36">
+        <f>S16</f>
+        <v>0</v>
+      </c>
       <c r="E16" s="35">
         <v>379.04369300000002</v>
       </c>
-      <c r="F16" s="36"/>
+      <c r="F16" s="36">
+        <f>T16</f>
+        <v>379.15975500000002</v>
+      </c>
       <c r="G16" s="35">
         <v>379.13458700000001</v>
       </c>
-      <c r="H16" s="36"/>
+      <c r="H16" s="36">
+        <f>U16</f>
+        <v>379.08683300000001</v>
+      </c>
       <c r="I16" s="35">
         <v>379.092489</v>
       </c>
-      <c r="J16" s="36"/>
+      <c r="J16" s="36">
+        <f>W16</f>
+        <v>378.7</v>
+      </c>
       <c r="K16" s="35">
         <v>379.1</v>
       </c>
       <c r="L16" s="36">
-        <f>V16</f>
+        <f>W16</f>
         <v>378.7</v>
       </c>
       <c r="M16" s="35">
@@ -2704,14 +3000,20 @@
       </c>
       <c r="N16" s="51"/>
       <c r="P16" s="36"/>
+      <c r="T16" s="35">
+        <v>379.15975500000002</v>
+      </c>
       <c r="U16" s="35">
+        <v>379.08683300000001</v>
+      </c>
+      <c r="V16" s="35">
         <v>379.2</v>
       </c>
-      <c r="V16" s="35">
+      <c r="W16" s="35">
         <v>378.7</v>
       </c>
     </row>
-    <row r="18" spans="2:22" s="41" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:23" s="41" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="41" t="s">
         <v>75</v>
       </c>
@@ -2735,21 +3037,40 @@
         <f>K4/I4-1</f>
         <v>0.19210866752910749</v>
       </c>
-      <c r="L18" s="42"/>
+      <c r="L18" s="42">
+        <f>L4/J4-1</f>
+        <v>0.1261789082595024</v>
+      </c>
       <c r="M18" s="41">
         <f>M4/K4-1</f>
         <v>0.18760173629951149</v>
       </c>
       <c r="N18" s="53"/>
       <c r="P18" s="42"/>
+      <c r="U18" s="41">
+        <f t="shared" ref="U18:V18" si="11">U4/T4-1</f>
+        <v>0.10529358328515981</v>
+      </c>
       <c r="V18" s="41">
-        <f>V4/U4-1</f>
+        <f t="shared" si="11"/>
+        <v>-1.5092647937836268E-2</v>
+      </c>
+      <c r="W18" s="41">
+        <f>W4/V4-1</f>
         <v>0.15710817781823683</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>76</v>
+      </c>
+      <c r="J19" s="40">
+        <f>J4/I4-1</f>
+        <v>0.13163001293661081</v>
+      </c>
+      <c r="K19" s="39">
+        <f>K4/J4-1</f>
+        <v>5.3443841097456479E-2</v>
       </c>
       <c r="L19" s="40">
         <f>L4/K4-1</f>
@@ -2763,23 +3084,23 @@
         <f>N4/M4-1</f>
         <v>-1</v>
       </c>
-      <c r="R19" s="68" t="s">
+      <c r="S19" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="S19" s="68" t="s">
+      <c r="T19" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="T19" s="68" t="s">
+      <c r="U19" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="U19" s="68" t="s">
+      <c r="V19" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="V19" s="68" t="s">
+      <c r="W19" s="57" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="2:22" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:23" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B21" s="39" t="s">
         <v>77</v>
       </c>
@@ -2802,7 +3123,10 @@
         <f>I5/I4</f>
         <v>0.16510349288486417</v>
       </c>
-      <c r="J21" s="40"/>
+      <c r="J21" s="40">
+        <f>J5/J4</f>
+        <v>0.19819948556730496</v>
+      </c>
       <c r="K21" s="39">
         <f>K5/K4</f>
         <v>0.18665219750406944</v>
@@ -2817,16 +3141,24 @@
       </c>
       <c r="N21" s="54"/>
       <c r="P21" s="40"/>
+      <c r="T21" s="39">
+        <f t="shared" ref="T21" si="12">T5/T4</f>
+        <v>0.17986621521182591</v>
+      </c>
       <c r="U21" s="39">
-        <f t="shared" ref="U21:V21" si="0">U5/U4</f>
+        <f t="shared" ref="U21:V21" si="13">U5/U4</f>
+        <v>0.17438732815301852</v>
+      </c>
+      <c r="V21" s="39">
+        <f t="shared" ref="V21:W21" si="14">V5/V4</f>
         <v>0.18267334243665606</v>
       </c>
-      <c r="V21" s="39">
-        <f t="shared" si="0"/>
+      <c r="W21" s="39">
+        <f t="shared" si="14"/>
         <v>0.18284927555235034</v>
       </c>
     </row>
-    <row r="22" spans="2:22" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:23" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="39" t="s">
         <v>78</v>
       </c>
@@ -2849,7 +3181,10 @@
         <f>I12/I4</f>
         <v>0.125</v>
       </c>
-      <c r="J22" s="40"/>
+      <c r="J22" s="40">
+        <f>J12/J4</f>
+        <v>0.18005144326950559</v>
+      </c>
       <c r="K22" s="39">
         <f>K12/K4</f>
         <v>0.18407487791644056</v>
@@ -2864,16 +3199,24 @@
       </c>
       <c r="N22" s="54"/>
       <c r="P22" s="40"/>
+      <c r="T22" s="39">
+        <f t="shared" ref="T22" si="15">T12/T4</f>
+        <v>0.14022627797505988</v>
+      </c>
       <c r="U22" s="39">
-        <f t="shared" ref="U22:V22" si="1">U12/U4</f>
+        <f t="shared" ref="U22:V22" si="16">U12/U4</f>
+        <v>0.13777644949193069</v>
+      </c>
+      <c r="V22" s="39">
+        <f t="shared" ref="V22:W22" si="17">V12/V4</f>
         <v>0.1542254589591868</v>
       </c>
-      <c r="V22" s="39">
-        <f t="shared" si="1"/>
+      <c r="W22" s="39">
+        <f t="shared" si="17"/>
         <v>0.16009965252737166</v>
       </c>
     </row>
-    <row r="23" spans="2:22" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:23" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B23" s="39" t="s">
         <v>107</v>
       </c>
@@ -2896,7 +3239,10 @@
         <f>I11/I10</f>
         <v>0.19730010384215993</v>
       </c>
-      <c r="J23" s="40"/>
+      <c r="J23" s="40">
+        <f>J11/J10</f>
+        <v>0.1954022988505747</v>
+      </c>
       <c r="K23" s="39">
         <f>K11/K10</f>
         <v>0.18985074626865672</v>
@@ -2911,21 +3257,29 @@
       </c>
       <c r="N23" s="54"/>
       <c r="P23" s="40"/>
+      <c r="T23" s="39">
+        <f t="shared" ref="T23" si="18">T11/T10</f>
+        <v>0.17851959361393321</v>
+      </c>
       <c r="U23" s="39">
-        <f t="shared" ref="U23:V23" si="2">U11/U10</f>
+        <f t="shared" ref="U23:V23" si="19">U11/U10</f>
+        <v>0.17715305667112896</v>
+      </c>
+      <c r="V23" s="39">
+        <f t="shared" ref="V23:W23" si="20">V11/V10</f>
         <v>0.19612495057334914</v>
       </c>
-      <c r="V23" s="39">
-        <f t="shared" si="2"/>
+      <c r="W23" s="39">
+        <f t="shared" si="20"/>
         <v>0.19776609724047309</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B27" s="43" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
         <v>80</v>
       </c>
@@ -2946,16 +3300,32 @@
         <f>829.8+303.8</f>
         <v>1133.5999999999999</v>
       </c>
+      <c r="J28" s="36">
+        <f>V28</f>
+        <v>1098.5</v>
+      </c>
       <c r="K28" s="35">
         <f>867.4+319.3</f>
         <v>1186.7</v>
       </c>
+      <c r="L28" s="36">
+        <f>W28</f>
+        <v>1233.9000000000001</v>
+      </c>
       <c r="M28" s="35">
         <f>1101.8+418.6</f>
         <v>1520.4</v>
       </c>
-    </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V28" s="35">
+        <f>808.5+290</f>
+        <v>1098.5</v>
+      </c>
+      <c r="W28" s="35">
+        <f>908.7+325.2</f>
+        <v>1233.9000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
         <v>81</v>
       </c>
@@ -2972,14 +3342,28 @@
       <c r="I29" s="35">
         <v>184.7</v>
       </c>
+      <c r="J29" s="36">
+        <f>V29</f>
+        <v>180.8</v>
+      </c>
       <c r="K29" s="35">
         <v>186.7</v>
       </c>
+      <c r="L29" s="36">
+        <f>W29</f>
+        <v>194</v>
+      </c>
       <c r="M29" s="35">
         <v>224.5</v>
       </c>
-    </row>
-    <row r="30" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V29" s="35">
+        <v>180.8</v>
+      </c>
+      <c r="W29" s="35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B30" s="2" t="s">
         <v>82</v>
       </c>
@@ -2998,18 +3382,30 @@
       <c r="I30" s="33">
         <v>4.8</v>
       </c>
-      <c r="J30" s="28"/>
+      <c r="J30" s="34">
+        <f>V30</f>
+        <v>9.3000000000000007</v>
+      </c>
       <c r="K30" s="33">
         <v>9.9</v>
       </c>
-      <c r="L30" s="28"/>
+      <c r="L30" s="36">
+        <f t="shared" ref="L30:L37" si="21">W30</f>
+        <v>8.1999999999999993</v>
+      </c>
       <c r="M30" s="33">
         <v>19.8</v>
       </c>
       <c r="N30" s="56"/>
       <c r="P30" s="28"/>
-    </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V30" s="33">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="W30" s="33">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>83</v>
       </c>
@@ -3026,14 +3422,28 @@
       <c r="I31" s="35">
         <v>0</v>
       </c>
+      <c r="J31" s="36">
+        <f t="shared" ref="J31:J33" si="22">V31</f>
+        <v>0</v>
+      </c>
       <c r="K31" s="35">
         <v>4.8</v>
       </c>
+      <c r="L31" s="36">
+        <f t="shared" si="21"/>
+        <v>31.1</v>
+      </c>
       <c r="M31" s="35">
         <v>43.9</v>
       </c>
-    </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V31" s="35">
+        <v>0</v>
+      </c>
+      <c r="W31" s="35">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
         <v>84</v>
       </c>
@@ -3050,14 +3460,28 @@
       <c r="I32" s="35">
         <v>0</v>
       </c>
+      <c r="J32" s="36">
+        <f t="shared" si="22"/>
+        <v>13.9</v>
+      </c>
       <c r="K32" s="35">
         <v>14.7</v>
       </c>
+      <c r="L32" s="36">
+        <f t="shared" si="21"/>
+        <v>14.7</v>
+      </c>
       <c r="M32" s="35">
         <v>14.7</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V32" s="35">
+        <v>13.9</v>
+      </c>
+      <c r="W32" s="35">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
         <v>85</v>
       </c>
@@ -3074,14 +3498,28 @@
       <c r="I33" s="35">
         <v>5.6</v>
       </c>
+      <c r="J33" s="36">
+        <f t="shared" si="22"/>
+        <v>1.3</v>
+      </c>
       <c r="K33" s="35">
         <v>1.9</v>
       </c>
+      <c r="L33" s="36">
+        <f t="shared" si="21"/>
+        <v>2.4</v>
+      </c>
       <c r="M33" s="35">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V33" s="35">
+        <v>1.3</v>
+      </c>
+      <c r="W33" s="35">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
         <v>86</v>
       </c>
@@ -3102,16 +3540,32 @@
         <f>SUM(I28:I33)</f>
         <v>1328.6999999999998</v>
       </c>
+      <c r="J34" s="36">
+        <f>SUM(J28:J33)</f>
+        <v>1303.8</v>
+      </c>
       <c r="K34" s="35">
         <f>SUM(K28:K33)</f>
         <v>1404.7000000000003</v>
       </c>
+      <c r="L34" s="36">
+        <f>SUM(L28:L33)</f>
+        <v>1484.3000000000002</v>
+      </c>
       <c r="M34" s="35">
         <f>SUM(M28:M33)</f>
         <v>1826.1000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V34" s="35">
+        <f>SUM(V28:V33)</f>
+        <v>1303.8</v>
+      </c>
+      <c r="W34" s="35">
+        <f>SUM(W28:W33)</f>
+        <v>1484.3000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
         <v>87</v>
       </c>
@@ -3128,14 +3582,28 @@
       <c r="I35" s="35">
         <v>175.8</v>
       </c>
+      <c r="J35" s="36">
+        <f t="shared" ref="J35:J37" si="23">V35</f>
+        <v>167.8</v>
+      </c>
       <c r="K35" s="35">
         <v>193.2</v>
       </c>
+      <c r="L35" s="36">
+        <f t="shared" si="21"/>
+        <v>228.8</v>
+      </c>
       <c r="M35" s="35">
         <v>308.8</v>
       </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V35" s="35">
+        <v>167.8</v>
+      </c>
+      <c r="W35" s="35">
+        <v>228.8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
         <v>88</v>
       </c>
@@ -3152,14 +3620,28 @@
       <c r="I36" s="35">
         <v>245.3</v>
       </c>
+      <c r="J36" s="36">
+        <f t="shared" si="23"/>
+        <v>268</v>
+      </c>
       <c r="K36" s="35">
         <v>279.2</v>
       </c>
+      <c r="L36" s="36">
+        <f t="shared" si="21"/>
+        <v>325.10000000000002</v>
+      </c>
       <c r="M36" s="35">
         <v>389.9</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V36" s="35">
+        <v>268</v>
+      </c>
+      <c r="W36" s="35">
+        <v>325.10000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
         <v>84</v>
       </c>
@@ -3176,14 +3658,28 @@
       <c r="I37" s="35">
         <v>6.5</v>
       </c>
+      <c r="J37" s="36">
+        <f t="shared" si="23"/>
+        <v>2.5</v>
+      </c>
       <c r="K37" s="35">
         <v>4.4000000000000004</v>
       </c>
+      <c r="L37" s="36">
+        <f t="shared" si="21"/>
+        <v>0.7</v>
+      </c>
       <c r="M37" s="35">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="38" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V37" s="35">
+        <v>2.5</v>
+      </c>
+      <c r="W37" s="35">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B38" s="2" t="s">
         <v>89</v>
       </c>
@@ -3202,18 +3698,30 @@
       <c r="I38" s="33">
         <v>125.5</v>
       </c>
-      <c r="J38" s="28"/>
+      <c r="J38" s="34">
+        <f t="shared" ref="J38:J39" si="24">V38</f>
+        <v>134.1</v>
+      </c>
       <c r="K38" s="33">
         <v>131.1</v>
       </c>
-      <c r="L38" s="28"/>
+      <c r="L38" s="34">
+        <f>W38</f>
+        <v>157.4</v>
+      </c>
       <c r="M38" s="33">
         <v>213.4</v>
       </c>
       <c r="N38" s="56"/>
       <c r="P38" s="28"/>
-    </row>
-    <row r="39" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V38" s="33">
+        <v>134.1</v>
+      </c>
+      <c r="W38" s="33">
+        <v>157.4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B39" s="2" t="s">
         <v>97</v>
       </c>
@@ -3232,18 +3740,30 @@
       <c r="I39" s="33">
         <v>0.4</v>
       </c>
-      <c r="J39" s="28"/>
+      <c r="J39" s="34">
+        <f t="shared" si="24"/>
+        <v>1.7</v>
+      </c>
       <c r="K39" s="33">
         <v>0.6</v>
       </c>
-      <c r="L39" s="28"/>
+      <c r="L39" s="34">
+        <f>W39</f>
+        <v>0.7</v>
+      </c>
       <c r="M39" s="33">
         <v>1.2</v>
       </c>
       <c r="N39" s="56"/>
       <c r="P39" s="28"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V39" s="33">
+        <v>1.7</v>
+      </c>
+      <c r="W39" s="33">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>90</v>
       </c>
@@ -3264,22 +3784,41 @@
         <f>SUM(I35:I39)+I34</f>
         <v>1882.1999999999998</v>
       </c>
+      <c r="J40" s="36">
+        <f>SUM(J35:J39)+J34</f>
+        <v>1877.9</v>
+      </c>
       <c r="K40" s="35">
         <f>SUM(K35:K39)+K34</f>
         <v>2013.2000000000003</v>
       </c>
+      <c r="L40" s="36">
+        <f>SUM(L35:L39)+L34</f>
+        <v>2197.0000000000005</v>
+      </c>
       <c r="M40" s="35">
         <f>SUM(M35:M39)+M34</f>
         <v>2741.3</v>
       </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V40" s="35">
+        <f>SUM(V35:V39)+V34</f>
+        <v>1877.9</v>
+      </c>
+      <c r="W40" s="35">
+        <f>SUM(W35:W39)+W34</f>
+        <v>2197.0000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.15">
       <c r="G41" s="35"/>
       <c r="H41" s="36"/>
       <c r="I41" s="35"/>
+      <c r="L41" s="36"/>
       <c r="M41" s="35"/>
-    </row>
-    <row r="42" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V41" s="35"/>
+      <c r="W41" s="35"/>
+    </row>
+    <row r="42" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
@@ -3298,18 +3837,30 @@
       <c r="I42" s="33">
         <v>76.099999999999994</v>
       </c>
-      <c r="J42" s="34"/>
+      <c r="J42" s="34">
+        <f>V42</f>
+        <v>3</v>
+      </c>
       <c r="K42" s="33">
         <v>206.1</v>
       </c>
-      <c r="L42" s="34"/>
+      <c r="L42" s="34">
+        <f>W42</f>
+        <v>72.5</v>
+      </c>
       <c r="M42" s="33">
         <v>256.39999999999998</v>
       </c>
       <c r="N42" s="56"/>
       <c r="P42" s="28"/>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V42" s="33">
+        <v>3</v>
+      </c>
+      <c r="W42" s="33">
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>92</v>
       </c>
@@ -3328,16 +3879,28 @@
       <c r="I43" s="35">
         <v>13</v>
       </c>
-      <c r="J43" s="36"/>
+      <c r="J43" s="36">
+        <f>V43</f>
+        <v>13.3</v>
+      </c>
       <c r="K43" s="35">
         <v>3</v>
       </c>
-      <c r="L43" s="36"/>
+      <c r="L43" s="36">
+        <f t="shared" ref="L43:L47" si="25">W43</f>
+        <v>15.5</v>
+      </c>
       <c r="M43" s="35">
         <v>78.8</v>
       </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V43" s="35">
+        <v>13.3</v>
+      </c>
+      <c r="W43" s="35">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>93</v>
       </c>
@@ -3356,16 +3919,28 @@
       <c r="I44" s="35">
         <v>0</v>
       </c>
-      <c r="J44" s="36"/>
+      <c r="J44" s="36">
+        <f t="shared" ref="J44:J47" si="26">V44</f>
+        <v>0</v>
+      </c>
       <c r="K44" s="35">
         <v>14.2</v>
       </c>
-      <c r="L44" s="36"/>
+      <c r="L44" s="36">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
       <c r="M44" s="35">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V44" s="35">
+        <v>0</v>
+      </c>
+      <c r="W44" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>94</v>
       </c>
@@ -3384,16 +3959,28 @@
       <c r="I45" s="35">
         <v>158.69999999999999</v>
       </c>
-      <c r="J45" s="36"/>
+      <c r="J45" s="36">
+        <f t="shared" si="26"/>
+        <v>186.7</v>
+      </c>
       <c r="K45" s="35">
         <v>22</v>
       </c>
-      <c r="L45" s="36"/>
+      <c r="L45" s="36">
+        <f t="shared" si="25"/>
+        <v>242.7</v>
+      </c>
       <c r="M45" s="35">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V45" s="35">
+        <v>186.7</v>
+      </c>
+      <c r="W45" s="35">
+        <v>242.7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>95</v>
       </c>
@@ -3412,16 +3999,28 @@
       <c r="I46" s="35">
         <v>30.5</v>
       </c>
-      <c r="J46" s="36"/>
+      <c r="J46" s="36">
+        <f t="shared" si="26"/>
+        <v>35.4</v>
+      </c>
       <c r="K46" s="35">
         <v>13.8</v>
       </c>
-      <c r="L46" s="36"/>
+      <c r="L46" s="36">
+        <f t="shared" si="25"/>
+        <v>20.7</v>
+      </c>
       <c r="M46" s="35">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V46" s="35">
+        <v>35.4</v>
+      </c>
+      <c r="W46" s="35">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>85</v>
       </c>
@@ -3440,16 +4039,28 @@
       <c r="I47" s="35">
         <v>11.3</v>
       </c>
-      <c r="J47" s="36"/>
+      <c r="J47" s="36">
+        <f t="shared" si="26"/>
+        <v>8.9</v>
+      </c>
       <c r="K47" s="35">
         <v>0.2</v>
       </c>
-      <c r="L47" s="36"/>
+      <c r="L47" s="36">
+        <f t="shared" si="25"/>
+        <v>11.6</v>
+      </c>
       <c r="M47" s="35">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="48" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V47" s="35">
+        <v>8.9</v>
+      </c>
+      <c r="W47" s="35">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B48" s="2" t="s">
         <v>97</v>
       </c>
@@ -3468,18 +4079,30 @@
       <c r="I48" s="33">
         <v>0.9</v>
       </c>
-      <c r="J48" s="34"/>
+      <c r="J48" s="34">
+        <f>V48</f>
+        <v>0.7</v>
+      </c>
       <c r="K48" s="33">
         <v>0</v>
       </c>
-      <c r="L48" s="34"/>
+      <c r="L48" s="34">
+        <f>W48</f>
+        <v>0.9</v>
+      </c>
       <c r="M48" s="33">
         <v>0</v>
       </c>
       <c r="N48" s="56"/>
       <c r="P48" s="28"/>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V48" s="33">
+        <v>0.7</v>
+      </c>
+      <c r="W48" s="33">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="49" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>103</v>
       </c>
@@ -3502,18 +4125,32 @@
         <f>SUM(I42:I48)</f>
         <v>290.49999999999994</v>
       </c>
-      <c r="J49" s="36"/>
+      <c r="J49" s="36">
+        <f>SUM(J42:J48)</f>
+        <v>248</v>
+      </c>
       <c r="K49" s="35">
         <f>SUM(K42:K48)</f>
         <v>259.29999999999995</v>
       </c>
-      <c r="L49" s="36"/>
+      <c r="L49" s="36">
+        <f>SUM(L42:L48)</f>
+        <v>363.9</v>
+      </c>
       <c r="M49" s="35">
         <f>SUM(M42:M48)</f>
         <v>400.29999999999995</v>
       </c>
-    </row>
-    <row r="50" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V49" s="35">
+        <f t="shared" ref="V49:W49" si="27">SUM(V42:V48)</f>
+        <v>248</v>
+      </c>
+      <c r="W49" s="35">
+        <f t="shared" si="27"/>
+        <v>363.9</v>
+      </c>
+    </row>
+    <row r="50" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B50" s="2" t="s">
         <v>91</v>
       </c>
@@ -3532,18 +4169,30 @@
       <c r="I50" s="33">
         <v>300</v>
       </c>
-      <c r="J50" s="34"/>
+      <c r="J50" s="34">
+        <f>V50</f>
+        <v>322.3</v>
+      </c>
       <c r="K50" s="33">
         <v>340.7</v>
       </c>
-      <c r="L50" s="34"/>
+      <c r="L50" s="34">
+        <f>W50</f>
+        <v>287.60000000000002</v>
+      </c>
       <c r="M50" s="33">
         <v>545.6</v>
       </c>
       <c r="N50" s="56"/>
       <c r="P50" s="28"/>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V50" s="33">
+        <v>322.3</v>
+      </c>
+      <c r="W50" s="33">
+        <v>287.60000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
         <v>92</v>
       </c>
@@ -3562,16 +4211,28 @@
       <c r="I51" s="35">
         <v>51.4</v>
       </c>
-      <c r="J51" s="36"/>
+      <c r="J51" s="36">
+        <f t="shared" ref="J51:J55" si="28">V51</f>
+        <v>51.7</v>
+      </c>
       <c r="K51" s="35">
         <v>53.4</v>
       </c>
-      <c r="L51" s="36"/>
+      <c r="L51" s="36">
+        <f t="shared" ref="L51:L55" si="29">W51</f>
+        <v>56.6</v>
+      </c>
       <c r="M51" s="35">
         <v>69.2</v>
       </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V51" s="35">
+        <v>51.7</v>
+      </c>
+      <c r="W51" s="35">
+        <v>56.6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
         <v>93</v>
       </c>
@@ -3590,16 +4251,28 @@
       <c r="I52" s="35">
         <v>45</v>
       </c>
-      <c r="J52" s="36"/>
+      <c r="J52" s="36">
+        <f t="shared" si="28"/>
+        <v>22.5</v>
+      </c>
       <c r="K52" s="35">
         <v>10.1</v>
       </c>
-      <c r="L52" s="36"/>
+      <c r="L52" s="36">
+        <f t="shared" si="29"/>
+        <v>0.6</v>
+      </c>
       <c r="M52" s="35">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V52" s="35">
+        <v>22.5</v>
+      </c>
+      <c r="W52" s="35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
         <v>94</v>
       </c>
@@ -3618,16 +4291,28 @@
       <c r="I53" s="35">
         <v>16.3</v>
       </c>
-      <c r="J53" s="36"/>
+      <c r="J53" s="36">
+        <f t="shared" si="28"/>
+        <v>16.8</v>
+      </c>
       <c r="K53" s="35">
         <v>15.2</v>
       </c>
-      <c r="L53" s="36"/>
+      <c r="L53" s="36">
+        <f t="shared" si="29"/>
+        <v>19</v>
+      </c>
       <c r="M53" s="35">
         <v>21.4</v>
       </c>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V53" s="35">
+        <v>16.8</v>
+      </c>
+      <c r="W53" s="35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
         <v>95</v>
       </c>
@@ -3646,16 +4331,28 @@
       <c r="I54" s="35">
         <v>14.3</v>
       </c>
-      <c r="J54" s="36"/>
+      <c r="J54" s="36">
+        <f t="shared" si="28"/>
+        <v>8.4</v>
+      </c>
       <c r="K54" s="35">
         <v>6.3</v>
       </c>
-      <c r="L54" s="36"/>
+      <c r="L54" s="36">
+        <f t="shared" si="29"/>
+        <v>7.7</v>
+      </c>
       <c r="M54" s="35">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V54" s="35">
+        <v>8.4</v>
+      </c>
+      <c r="W54" s="35">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="55" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B55" s="1" t="s">
         <v>85</v>
       </c>
@@ -3674,16 +4371,28 @@
       <c r="I55" s="35">
         <v>41.7</v>
       </c>
-      <c r="J55" s="36"/>
+      <c r="J55" s="36">
+        <f t="shared" si="28"/>
+        <v>40.6</v>
+      </c>
       <c r="K55" s="35">
         <v>51.1</v>
       </c>
-      <c r="L55" s="36"/>
+      <c r="L55" s="36">
+        <f t="shared" si="29"/>
+        <v>58.5</v>
+      </c>
       <c r="M55" s="35">
         <v>69.2</v>
       </c>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V55" s="35">
+        <v>40.6</v>
+      </c>
+      <c r="W55" s="35">
+        <v>58.5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
         <v>96</v>
       </c>
@@ -3706,21 +4415,35 @@
         <f>I49+SUM(I50:I55)</f>
         <v>759.19999999999993</v>
       </c>
-      <c r="J56" s="36"/>
+      <c r="J56" s="36">
+        <f>J49+SUM(J50:J55)</f>
+        <v>710.3</v>
+      </c>
       <c r="K56" s="35">
         <f>K49+SUM(K50:K55)</f>
         <v>736.09999999999991</v>
       </c>
-      <c r="L56" s="36"/>
+      <c r="L56" s="36">
+        <f>L49+SUM(L50:L55)</f>
+        <v>793.90000000000009</v>
+      </c>
       <c r="M56" s="35">
         <f>M49+SUM(M50:M55)</f>
         <v>1114.3000000000002</v>
       </c>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V56" s="35">
+        <f>V49+SUM(V50:V55)</f>
+        <v>710.3</v>
+      </c>
+      <c r="W56" s="35">
+        <f>W49+SUM(W50:W55)</f>
+        <v>793.90000000000009</v>
+      </c>
+    </row>
+    <row r="57" spans="2:23" x14ac:dyDescent="0.15">
       <c r="M57" s="35"/>
     </row>
-    <row r="58" spans="2:16" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:23" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B58" s="35" t="s">
         <v>98</v>
       </c>
@@ -3739,18 +4462,30 @@
       <c r="I58" s="35">
         <v>1123</v>
       </c>
-      <c r="J58" s="36"/>
+      <c r="J58" s="36">
+        <f>V58</f>
+        <v>1167.5999999999999</v>
+      </c>
       <c r="K58" s="35">
         <v>1277.0999999999999</v>
       </c>
-      <c r="L58" s="36"/>
+      <c r="L58" s="36">
+        <f>W58</f>
+        <v>1403.1</v>
+      </c>
       <c r="M58" s="35">
         <v>1627</v>
       </c>
       <c r="N58" s="51"/>
       <c r="P58" s="36"/>
-    </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V58" s="35">
+        <v>1167.5999999999999</v>
+      </c>
+      <c r="W58" s="35">
+        <v>1403.1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
         <v>99</v>
       </c>
@@ -3770,16 +4505,32 @@
         <f>I58+I56</f>
         <v>1882.1999999999998</v>
       </c>
+      <c r="J59" s="36">
+        <f>J58+J56</f>
+        <v>1877.8999999999999</v>
+      </c>
       <c r="K59" s="35">
         <f>K58+K56</f>
         <v>2013.1999999999998</v>
       </c>
+      <c r="L59" s="36">
+        <f>L58+L56</f>
+        <v>2197</v>
+      </c>
       <c r="M59" s="35">
         <f>M58+M56</f>
         <v>2741.3</v>
       </c>
-    </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V59" s="35">
+        <f>V58+V56</f>
+        <v>1877.8999999999999</v>
+      </c>
+      <c r="W59" s="35">
+        <f>W58+W56</f>
+        <v>2197</v>
+      </c>
+    </row>
+    <row r="61" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B61" s="1" t="s">
         <v>100</v>
       </c>
@@ -3799,16 +4550,32 @@
         <f>I40-I56</f>
         <v>1123</v>
       </c>
+      <c r="J61" s="36">
+        <f>J40-J56</f>
+        <v>1167.6000000000001</v>
+      </c>
       <c r="K61" s="35">
         <f>K40-K56</f>
         <v>1277.1000000000004</v>
       </c>
+      <c r="L61" s="36">
+        <f>L40-L56</f>
+        <v>1403.1000000000004</v>
+      </c>
       <c r="M61" s="35">
         <f>M40-M56</f>
         <v>1627</v>
       </c>
-    </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V61" s="35">
+        <f t="shared" ref="V61:W61" si="30">V40-V56</f>
+        <v>1167.6000000000001</v>
+      </c>
+      <c r="W61" s="35">
+        <f t="shared" si="30"/>
+        <v>1403.1000000000004</v>
+      </c>
+    </row>
+    <row r="62" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
         <v>101</v>
       </c>
@@ -3828,16 +4595,32 @@
         <f>I61/I16</f>
         <v>2.9623377739884473</v>
       </c>
+      <c r="J62" s="36">
+        <f>J61/J16</f>
+        <v>3.0831792975970429</v>
+      </c>
       <c r="K62" s="1">
         <f>K61/K16</f>
         <v>3.368768135056714</v>
       </c>
+      <c r="L62" s="36">
+        <f>L61/L16</f>
+        <v>3.7050435701082662</v>
+      </c>
       <c r="M62" s="1">
         <f>M61/M16</f>
         <v>4.3019566367001589</v>
       </c>
-    </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="V62" s="1">
+        <f t="shared" ref="V62:W62" si="31">V61/V16</f>
+        <v>3.0791139240506333</v>
+      </c>
+      <c r="W62" s="1">
+        <f t="shared" si="31"/>
+        <v>3.7050435701082662</v>
+      </c>
+    </row>
+    <row r="64" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B64" s="1" t="s">
         <v>7</v>
       </c>
@@ -3857,16 +4640,32 @@
         <f>I38+I39+I30</f>
         <v>130.70000000000002</v>
       </c>
+      <c r="J64" s="36">
+        <f>J38+J39+J30</f>
+        <v>145.1</v>
+      </c>
       <c r="K64" s="35">
         <f>K38+K39+K30</f>
         <v>141.6</v>
       </c>
+      <c r="L64" s="36">
+        <f>L38+L39+L30</f>
+        <v>166.29999999999998</v>
+      </c>
       <c r="M64" s="35">
         <f>M38+M39+M30</f>
         <v>234.4</v>
       </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="V64" s="35">
+        <f>V38+V39+V30</f>
+        <v>145.1</v>
+      </c>
+      <c r="W64" s="35">
+        <f>W38+W39+W30</f>
+        <v>166.29999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B65" s="1" t="s">
         <v>8</v>
       </c>
@@ -3886,16 +4685,32 @@
         <f>I50+I42+I48</f>
         <v>377</v>
       </c>
+      <c r="J65" s="36">
+        <f>J50+J42+J48</f>
+        <v>326</v>
+      </c>
       <c r="K65" s="35">
         <f>K50+K42+K48</f>
         <v>546.79999999999995</v>
       </c>
+      <c r="L65" s="36">
+        <f>L50+L42+L48</f>
+        <v>361</v>
+      </c>
       <c r="M65" s="35">
         <f>M50+M42+M48</f>
         <v>802</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="V65" s="35">
+        <f>V50+V42+V48</f>
+        <v>326</v>
+      </c>
+      <c r="W65" s="35">
+        <f>W50+W42+W48</f>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B66" s="1" t="s">
         <v>9</v>
       </c>
@@ -3915,16 +4730,32 @@
         <f>I64-I65</f>
         <v>-246.29999999999998</v>
       </c>
+      <c r="J66" s="36">
+        <f>J64-J65</f>
+        <v>-180.9</v>
+      </c>
       <c r="K66" s="35">
         <f>K64-K65</f>
         <v>-405.19999999999993</v>
       </c>
+      <c r="L66" s="36">
+        <f>L64-L65</f>
+        <v>-194.70000000000002</v>
+      </c>
       <c r="M66" s="35">
         <f>M64-M65</f>
         <v>-567.6</v>
       </c>
-    </row>
-    <row r="68" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V66" s="35">
+        <f>V64-V65</f>
+        <v>-180.9</v>
+      </c>
+      <c r="W66" s="35">
+        <f>W64-W65</f>
+        <v>-194.70000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" s="37" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B68" s="37" t="s">
         <v>102</v>
       </c>
@@ -3943,18 +4774,36 @@
       <c r="I68" s="37">
         <v>23.1129</v>
       </c>
-      <c r="J68" s="38"/>
+      <c r="J68" s="38">
+        <f>V68</f>
+        <v>23.4651</v>
+      </c>
       <c r="K68" s="37">
         <v>28.1996</v>
       </c>
-      <c r="L68" s="38"/>
+      <c r="L68" s="38">
+        <f>W68</f>
+        <v>24.9636</v>
+      </c>
       <c r="M68" s="37">
         <v>20.45</v>
       </c>
       <c r="N68" s="52"/>
       <c r="P68" s="38"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T68" s="37">
+        <v>16.279199999999999</v>
+      </c>
+      <c r="U68" s="37">
+        <v>18.8504</v>
+      </c>
+      <c r="V68" s="37">
+        <v>23.4651</v>
+      </c>
+      <c r="W68" s="37">
+        <v>24.9636</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B69" s="1" t="s">
         <v>6</v>
       </c>
@@ -3974,16 +4823,40 @@
         <f>I68*I16</f>
         <v>8761.9267890080991</v>
       </c>
+      <c r="J69" s="36">
+        <f t="shared" ref="J69:L69" si="32">J68*J16</f>
+        <v>8886.2333699999999</v>
+      </c>
       <c r="K69" s="35">
         <f>K68*K16</f>
         <v>10690.468360000001</v>
       </c>
+      <c r="L69" s="36">
+        <f t="shared" si="32"/>
+        <v>9453.7153199999993</v>
+      </c>
       <c r="M69" s="35">
         <f>M68*M16</f>
         <v>7734.19</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T69" s="35">
+        <f t="shared" ref="T69:W69" si="33">T68*T16</f>
+        <v>6172.4174835960002</v>
+      </c>
+      <c r="U69" s="35">
+        <f t="shared" si="33"/>
+        <v>7145.9384367832008</v>
+      </c>
+      <c r="V69" s="35">
+        <f t="shared" si="33"/>
+        <v>8897.9659199999987</v>
+      </c>
+      <c r="W69" s="35">
+        <f t="shared" si="33"/>
+        <v>9453.7153199999993</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B70" s="1" t="s">
         <v>10</v>
       </c>
@@ -4003,19 +4876,43 @@
         <f>I69-I66</f>
         <v>9008.2267890080984</v>
       </c>
+      <c r="J70" s="36">
+        <f t="shared" ref="J70:L70" si="34">J69-J66</f>
+        <v>9067.1333699999996</v>
+      </c>
       <c r="K70" s="35">
         <f>K69-K66</f>
         <v>11095.668360000001</v>
       </c>
+      <c r="L70" s="36">
+        <f t="shared" si="34"/>
+        <v>9648.4153200000001</v>
+      </c>
       <c r="M70" s="35">
         <f>M69-M66</f>
         <v>8301.7899999999991</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T70" s="35">
+        <f t="shared" ref="T70:W70" si="35">T69-T66</f>
+        <v>6172.4174835960002</v>
+      </c>
+      <c r="U70" s="35">
+        <f t="shared" si="35"/>
+        <v>7145.9384367832008</v>
+      </c>
+      <c r="V70" s="35">
+        <f t="shared" si="35"/>
+        <v>9078.8659199999984</v>
+      </c>
+      <c r="W70" s="35">
+        <f t="shared" si="35"/>
+        <v>9648.4153200000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A72" s="47">
-        <f>AVERAGE(C72:AZ72)</f>
-        <v>6.467721604504824</v>
+        <f>AVERAGE(C72:BA72)</f>
+        <v>6.6455994380078121</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>22</v>
@@ -4044,31 +4941,148 @@
         <f>M68/M62</f>
         <v>4.7536508912108166</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="V72" s="44">
+        <f t="shared" ref="V72:W72" si="36">V68/V62</f>
+        <v>7.620731346351489</v>
+      </c>
+      <c r="W72" s="44">
+        <f>W68/W62</f>
+        <v>6.7377345306820589</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B73" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I73" s="44">
+        <f>I69/SUM(H4:I4)</f>
+        <v>6.7239097452291459</v>
+      </c>
+      <c r="J73" s="60">
+        <f>J69/SUM(I4:J4)</f>
+        <v>6.7411875056895765</v>
+      </c>
+      <c r="K73" s="44">
+        <f>K69/SUM(J4:K4)</f>
+        <v>7.4394351844119697</v>
+      </c>
+      <c r="L73" s="60">
+        <f>L69/SUM(K4:L4)</f>
+        <v>6.1979383203304268</v>
+      </c>
+      <c r="M73" s="44">
+        <f>M69/SUM(L4:M4)</f>
+        <v>4.6490682856455878</v>
+      </c>
+      <c r="T73" s="44">
+        <f t="shared" ref="T73:W73" si="37">T69/T4</f>
+        <v>5.0973800343513087</v>
+      </c>
+      <c r="U73" s="44">
+        <f t="shared" si="37"/>
+        <v>5.3391650005851767</v>
+      </c>
+      <c r="V73" s="44">
+        <f t="shared" si="37"/>
+        <v>6.7500879380974039</v>
+      </c>
+      <c r="W73" s="44">
+        <f>W69/W4</f>
+        <v>6.1979383203304268</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B74" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B75" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C75" s="44"/>
+      <c r="E75" s="44"/>
+      <c r="G75" s="44">
+        <f>G68/(G15+F15)</f>
+        <v>40.570085892338092</v>
+      </c>
+      <c r="I75" s="44">
+        <f>I68/(I15+H15)</f>
+        <v>49.58603989933718</v>
+      </c>
+      <c r="J75" s="60">
+        <f>J68/(J15+I15)</f>
+        <v>43.727166392237116</v>
+      </c>
+      <c r="K75" s="44">
+        <f>K68/(K15+J15)</f>
+        <v>40.829325611764631</v>
+      </c>
+      <c r="L75" s="60">
+        <f>L68/(L15+K15)</f>
+        <v>38.73571477005347</v>
+      </c>
+      <c r="M75" s="44">
+        <f>M68/(M15+L15)</f>
+        <v>34.65810517544427</v>
+      </c>
+      <c r="T75" s="44">
+        <f t="shared" ref="T75:W75" si="38">T68/T15</f>
+        <v>36.35110414367491</v>
+      </c>
+      <c r="U75" s="44">
+        <f t="shared" si="38"/>
+        <v>38.752377639822122</v>
+      </c>
+      <c r="V75" s="44">
+        <f t="shared" si="38"/>
+        <v>43.767663157894724</v>
+      </c>
+      <c r="W75" s="44">
+        <f>W68/W15</f>
+        <v>38.713002948402945</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B76" s="1" t="s">
         <v>26</v>
       </c>
       <c r="M76" s="39"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B77" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="C77" s="39"/>
+      <c r="E77" s="39"/>
+      <c r="G77" s="39"/>
+      <c r="I77" s="39">
+        <f>(I5+H5)/(I40-I49)</f>
+        <v>0.14066721115788153</v>
+      </c>
+      <c r="J77" s="40">
+        <f>(J5+I5)/(J40-J49)</f>
+        <v>0.14773912509969936</v>
+      </c>
+      <c r="K77" s="39">
+        <f>(K5+J5)/(K40-K49)</f>
+        <v>0.15753463709447516</v>
+      </c>
+      <c r="L77" s="40">
+        <f>(L5+K5)/(L40-L49)</f>
+        <v>0.15214663684468929</v>
+      </c>
+      <c r="M77" s="39">
+        <f>(M5+L5)/(M40-M49)</f>
+        <v>0.12516018795386588</v>
+      </c>
+      <c r="V77" s="39">
+        <f t="shared" ref="V77:W77" si="39">V5/(V40-V49)</f>
+        <v>0.14773912509969936</v>
+      </c>
+      <c r="W77" s="39">
+        <f>W5/(W40-W49)</f>
+        <v>0.15214663684468929</v>
       </c>
     </row>
   </sheetData>
@@ -4076,13 +5090,16 @@
     <hyperlink ref="M1" r:id="rId1" xr:uid="{64230965-EEC2-4818-9500-5E49F2C6FBF5}"/>
     <hyperlink ref="I1" r:id="rId2" xr:uid="{879E0608-9977-4013-9DB7-7908B60FAFB2}"/>
     <hyperlink ref="E1" r:id="rId3" xr:uid="{D2F2E719-2F49-4057-B46A-7E29B8F345FA}"/>
-    <hyperlink ref="V1" r:id="rId4" xr:uid="{312EC780-3433-42F0-97FF-0788993E5A29}"/>
+    <hyperlink ref="W1" r:id="rId4" xr:uid="{312EC780-3433-42F0-97FF-0788993E5A29}"/>
+    <hyperlink ref="U1" r:id="rId5" xr:uid="{313C0DA0-3F4A-45BC-BA9D-854CC763EEA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
   <ignoredErrors>
-    <ignoredError sqref="L10" formula="1"/>
+    <ignoredError sqref="L10 L34 L49 J10 H10:H15 J34 J49" formula="1"/>
+    <ignoredError sqref="D11:F15 E10" evalError="1"/>
+    <ignoredError sqref="F10 D10" evalError="1" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
£HLMA DCF/NPV forecast, fair valued @ 8% discount rate
</commit_message>
<xml_diff>
--- a/£HLMA.xlsx
+++ b/£HLMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43140AF5-4A44-E94B-A72A-B74F09545752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C808652-3B53-1A46-B2FC-688441716B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{1821E3F4-C005-474E-95BC-C5AE66A060FF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="115">
   <si>
     <t>£HLMA</t>
   </si>
@@ -221,15 +221,6 @@
     <t>FY32</t>
   </si>
   <si>
-    <t>FY33</t>
-  </si>
-  <si>
-    <t>FY34</t>
-  </si>
-  <si>
-    <t>FY35</t>
-  </si>
-  <si>
     <t>Operating Profit</t>
   </si>
   <si>
@@ -366,15 +357,40 @@
   </si>
   <si>
     <t>FY16</t>
+  </si>
+  <si>
+    <t>(Projected)</t>
+  </si>
+  <si>
+    <t>Maturity Rate</t>
+  </si>
+  <si>
+    <t>Discount Rate</t>
+  </si>
+  <si>
+    <t>NPV</t>
+  </si>
+  <si>
+    <t>Total Value</t>
+  </si>
+  <si>
+    <t>Per Share</t>
+  </si>
+  <si>
+    <t>S/P</t>
+  </si>
+  <si>
+    <t>Upside</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0\x"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0_);[Red]\(#,##0.0\)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -609,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -715,6 +731,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -748,9 +767,17 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1245,7 +1272,7 @@
   <dimension ref="B2:S38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1274,26 +1301,26 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="65"/>
-      <c r="G5" s="63" t="s">
+      <c r="C5" s="65"/>
+      <c r="D5" s="66"/>
+      <c r="G5" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="66"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B6" s="5" t="s">
@@ -1498,11 +1525,11 @@
       <c r="S14" s="13"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="66"/>
       <c r="G15" s="19"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -1521,10 +1548,10 @@
       <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="66" t="s">
+      <c r="C16" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="67"/>
+      <c r="D16" s="68"/>
       <c r="G16" s="19"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -1543,10 +1570,10 @@
       <c r="B17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="66" t="s">
+      <c r="C17" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="67"/>
+      <c r="D17" s="68"/>
       <c r="G17" s="19"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -1565,8 +1592,8 @@
       <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="68"/>
       <c r="G18" s="19"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -1585,8 +1612,8 @@
       <c r="B19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="63"/>
       <c r="G19" s="19"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -1632,11 +1659,11 @@
       <c r="S21" s="13"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
       <c r="G22" s="19"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -1655,10 +1682,10 @@
       <c r="B23" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="66" t="s">
+      <c r="C23" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="67"/>
+      <c r="D23" s="68"/>
       <c r="G23" s="19"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -1677,10 +1704,10 @@
       <c r="B24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="66">
+      <c r="C24" s="67">
         <v>1894</v>
       </c>
-      <c r="D24" s="67"/>
+      <c r="D24" s="68"/>
       <c r="G24" s="19"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -1697,8 +1724,8 @@
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B25" s="17"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="68"/>
       <c r="G25" s="19"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -1715,8 +1742,8 @@
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B26" s="17"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="68"/>
       <c r="G26" s="19"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -1733,8 +1760,8 @@
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B27" s="17"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="68"/>
       <c r="G27" s="19"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -1777,10 +1804,10 @@
       <c r="B29" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="68" t="s">
+      <c r="C29" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="69"/>
+      <c r="D29" s="70"/>
       <c r="G29" s="19"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -1826,11 +1853,11 @@
       <c r="S31" s="13"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="66"/>
       <c r="G32" s="19"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -1849,11 +1876,11 @@
       <c r="B33" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="70">
+      <c r="C33" s="71">
         <f>C6/'Financial Model'!M62</f>
         <v>5.24180086047941</v>
       </c>
-      <c r="D33" s="71"/>
+      <c r="D33" s="72"/>
       <c r="G33" s="19"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
@@ -1872,11 +1899,11 @@
       <c r="B34" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="70">
+      <c r="C34" s="71">
         <f>C8/SUM('Financial Model'!L4:M4)</f>
         <v>5.1264787208463574</v>
       </c>
-      <c r="D34" s="71"/>
+      <c r="D34" s="72"/>
       <c r="G34" s="19"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
@@ -1895,8 +1922,8 @@
       <c r="B35" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="66"/>
-      <c r="D35" s="67"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="68"/>
       <c r="G35" s="19"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
@@ -1915,11 +1942,11 @@
       <c r="B36" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="70">
+      <c r="C36" s="71">
         <f>C6/SUM('Financial Model'!L15:M15)</f>
         <v>38.217128200795514</v>
       </c>
-      <c r="D36" s="71"/>
+      <c r="D36" s="72"/>
       <c r="G36" s="19"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
@@ -1938,8 +1965,8 @@
       <c r="B37" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="66"/>
-      <c r="D37" s="67"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="68"/>
       <c r="G37" s="19"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
@@ -1958,8 +1985,8 @@
       <c r="B38" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="61"/>
-      <c r="D38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="63"/>
       <c r="G38" s="21"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
@@ -2009,18 +2036,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F5332D-7B2B-4D46-8BAA-4FBC91F2AA00}">
-  <dimension ref="A1:AK77"/>
+  <dimension ref="A1:BU77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="R6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W77" sqref="V77:W77"/>
+      <selection pane="bottomRight" activeCell="AJ22" sqref="AJ22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" style="1"/>
     <col min="4" max="4" width="9.1640625" style="29"/>
@@ -2036,15 +2063,20 @@
     <col min="14" max="14" width="9.1640625" style="55"/>
     <col min="15" max="15" width="9.1640625" style="1"/>
     <col min="16" max="16" width="9.1640625" style="29"/>
-    <col min="17" max="16384" width="9.1640625" style="1"/>
+    <col min="17" max="23" width="9.1640625" style="1"/>
+    <col min="24" max="24" width="9.1640625" style="55"/>
+    <col min="25" max="35" width="9.1640625" style="1"/>
+    <col min="36" max="36" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:37" s="22" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:73" s="22" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="C1" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E1" s="30" t="s">
         <v>34</v>
@@ -2083,15 +2115,15 @@
         <v>45</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="S1" s="22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="T1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="72" t="s">
+      <c r="U1" s="61" t="s">
         <v>47</v>
       </c>
       <c r="V1" s="22" t="s">
@@ -2100,7 +2132,7 @@
       <c r="W1" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="22" t="s">
+      <c r="X1" s="48" t="s">
         <v>50</v>
       </c>
       <c r="Y1" s="22" t="s">
@@ -2133,17 +2165,8 @@
       <c r="AH1" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AI1" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ1" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK1" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="2:37" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="2:73" s="24" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B2" s="23"/>
       <c r="C2" s="32">
         <v>43008</v>
@@ -2197,8 +2220,11 @@
       <c r="W2" s="32">
         <v>44651</v>
       </c>
-    </row>
-    <row r="3" spans="2:37" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X2" s="49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="2:73" s="24" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B3" s="23"/>
       <c r="D3" s="27"/>
       <c r="E3" s="31">
@@ -2228,8 +2254,9 @@
       <c r="W3" s="31">
         <v>44728</v>
       </c>
-    </row>
-    <row r="4" spans="2:37" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X3" s="49"/>
+    </row>
+    <row r="4" spans="2:73" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="33" t="s">
         <v>29</v>
       </c>
@@ -2271,7 +2298,10 @@
       <c r="M4" s="33">
         <v>875.5</v>
       </c>
-      <c r="N4" s="50"/>
+      <c r="N4" s="50">
+        <f>M4*(1+N19)</f>
+        <v>989.31499999999994</v>
+      </c>
       <c r="P4" s="34"/>
       <c r="T4" s="33">
         <v>1210.9000000000001</v>
@@ -2285,10 +2315,54 @@
       <c r="W4" s="33">
         <v>1525.3</v>
       </c>
-    </row>
-    <row r="5" spans="2:37" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X4" s="50">
+        <f>N4+M4</f>
+        <v>1864.8150000000001</v>
+      </c>
+      <c r="Y4" s="33">
+        <f>X4*(1+Y18)</f>
+        <v>2200.4816999999998</v>
+      </c>
+      <c r="Z4" s="33">
+        <f t="shared" ref="Z4:AH4" si="1">Y4*(1+Z18)</f>
+        <v>2596.5684059999999</v>
+      </c>
+      <c r="AA4" s="33">
+        <f t="shared" si="1"/>
+        <v>3063.9507190799995</v>
+      </c>
+      <c r="AB4" s="33">
+        <f t="shared" si="1"/>
+        <v>3615.4618485143992</v>
+      </c>
+      <c r="AC4" s="33">
+        <f t="shared" si="1"/>
+        <v>4266.2449812469904</v>
+      </c>
+      <c r="AD4" s="33">
+        <f t="shared" si="1"/>
+        <v>5034.1690778714483</v>
+      </c>
+      <c r="AE4" s="33">
+        <f t="shared" si="1"/>
+        <v>5940.3195118883086</v>
+      </c>
+      <c r="AF4" s="33">
+        <f t="shared" si="1"/>
+        <v>7009.5770240282036</v>
+      </c>
+      <c r="AG4" s="33">
+        <f t="shared" si="1"/>
+        <v>8271.3008883532802</v>
+      </c>
+      <c r="AH4" s="33">
+        <f t="shared" si="1"/>
+        <v>9760.1350482568705</v>
+      </c>
+    </row>
+    <row r="5" spans="2:73" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C5" s="33">
         <v>81.8</v>
@@ -2328,7 +2402,10 @@
       <c r="M5" s="33">
         <v>151.69999999999999</v>
       </c>
-      <c r="N5" s="50"/>
+      <c r="N5" s="50">
+        <f>N4*0.18</f>
+        <v>178.07669999999999</v>
+      </c>
       <c r="P5" s="34"/>
       <c r="T5" s="33">
         <v>217.8</v>
@@ -2342,10 +2419,54 @@
       <c r="W5" s="33">
         <v>278.89999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X5" s="50">
+        <f>N5+M5</f>
+        <v>329.77670000000001</v>
+      </c>
+      <c r="Y5" s="33">
+        <f>Y4*0.18</f>
+        <v>396.08670599999994</v>
+      </c>
+      <c r="Z5" s="33">
+        <f t="shared" ref="Z5:AH5" si="2">Z4*0.18</f>
+        <v>467.38231307999996</v>
+      </c>
+      <c r="AA5" s="33">
+        <f t="shared" si="2"/>
+        <v>551.51112943439989</v>
+      </c>
+      <c r="AB5" s="33">
+        <f t="shared" si="2"/>
+        <v>650.78313273259187</v>
+      </c>
+      <c r="AC5" s="33">
+        <f t="shared" si="2"/>
+        <v>767.92409662445823</v>
+      </c>
+      <c r="AD5" s="33">
+        <f t="shared" si="2"/>
+        <v>906.15043401686069</v>
+      </c>
+      <c r="AE5" s="33">
+        <f t="shared" si="2"/>
+        <v>1069.2575121398954</v>
+      </c>
+      <c r="AF5" s="33">
+        <f t="shared" si="2"/>
+        <v>1261.7238643250766</v>
+      </c>
+      <c r="AG5" s="33">
+        <f t="shared" si="2"/>
+        <v>1488.8341599035905</v>
+      </c>
+      <c r="AH5" s="33">
+        <f t="shared" si="2"/>
+        <v>1756.8243086862367</v>
+      </c>
+    </row>
+    <row r="6" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C6" s="35">
         <v>-0.1</v>
@@ -2385,7 +2506,9 @@
       <c r="M6" s="35">
         <v>0</v>
       </c>
-      <c r="N6" s="51"/>
+      <c r="N6" s="51">
+        <v>0</v>
+      </c>
       <c r="P6" s="36"/>
       <c r="T6" s="35">
         <v>-0.1</v>
@@ -2399,37 +2522,71 @@
       <c r="W6" s="35">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="7" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X6" s="51">
+        <f>N6+M6</f>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="35">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="35">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="35">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="35">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="35">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="35">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="35">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B7" s="35" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" s="35">
         <v>0</v>
       </c>
       <c r="D7" s="36">
-        <f t="shared" ref="D7:D11" si="1">S7-C7</f>
+        <f t="shared" ref="D7:D11" si="3">S7-C7</f>
         <v>0</v>
       </c>
       <c r="E7" s="35">
         <v>-0.9</v>
       </c>
       <c r="F7" s="36">
-        <f t="shared" ref="F7:F11" si="2">T7-E7</f>
+        <f t="shared" ref="F7:F11" si="4">T7-E7</f>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="G7" s="35">
         <v>0</v>
       </c>
       <c r="H7" s="36">
-        <f t="shared" ref="H7:H11" si="3">U7-G7</f>
+        <f t="shared" ref="H7:H11" si="5">U7-G7</f>
         <v>2.9</v>
       </c>
       <c r="I7" s="35">
         <v>0</v>
       </c>
       <c r="J7" s="36">
-        <f t="shared" ref="J7:J11" si="4">V7-I7</f>
+        <f t="shared" ref="J7:J11" si="6">V7-I7</f>
         <v>22.1</v>
       </c>
       <c r="K7" s="35">
@@ -2442,7 +2599,9 @@
       <c r="M7" s="35">
         <v>0</v>
       </c>
-      <c r="N7" s="51"/>
+      <c r="N7" s="51">
+        <v>0</v>
+      </c>
       <c r="P7" s="36"/>
       <c r="T7" s="35">
         <v>-1</v>
@@ -2456,37 +2615,71 @@
       <c r="W7" s="35">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X7" s="51">
+        <f t="shared" ref="X7:X9" si="7">N7+M7</f>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="35">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="35">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="35">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="35">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="35">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="35">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="35">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B8" s="35" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C8" s="35">
         <v>0.1</v>
       </c>
       <c r="D8" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-0.1</v>
       </c>
       <c r="E8" s="35">
         <v>0.1</v>
       </c>
       <c r="F8" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="G8" s="35">
         <v>0.4</v>
       </c>
       <c r="H8" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="I8" s="35">
         <v>1</v>
       </c>
       <c r="J8" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K8" s="35">
@@ -2499,7 +2692,10 @@
       <c r="M8" s="35">
         <v>0.8</v>
       </c>
-      <c r="N8" s="51"/>
+      <c r="N8" s="51">
+        <f>AVERAGE(K8:M8)</f>
+        <v>0.46666666666666662</v>
+      </c>
       <c r="P8" s="36"/>
       <c r="T8" s="35">
         <v>0.5</v>
@@ -2513,37 +2709,81 @@
       <c r="W8" s="35">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="9" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X8" s="51">
+        <f t="shared" si="7"/>
+        <v>1.2666666666666666</v>
+      </c>
+      <c r="Y8" s="35">
+        <f t="shared" ref="Y8" si="8">AVERAGE(V8:X8)</f>
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="Z8" s="35">
+        <f t="shared" ref="Z8" si="9">AVERAGE(W8:Y8)</f>
+        <v>0.94074074074074077</v>
+      </c>
+      <c r="AA8" s="35">
+        <f t="shared" ref="AA8" si="10">AVERAGE(X8:Z8)</f>
+        <v>1.0543209876543209</v>
+      </c>
+      <c r="AB8" s="35">
+        <f t="shared" ref="AB8" si="11">AVERAGE(Y8:AA8)</f>
+        <v>0.98353909465020573</v>
+      </c>
+      <c r="AC8" s="35">
+        <f t="shared" ref="AC8" si="12">AVERAGE(Z8:AB8)</f>
+        <v>0.99286694101508921</v>
+      </c>
+      <c r="AD8" s="35">
+        <f t="shared" ref="AD8" si="13">AVERAGE(AA8:AC8)</f>
+        <v>1.0102423411065387</v>
+      </c>
+      <c r="AE8" s="35">
+        <f t="shared" ref="AE8" si="14">AVERAGE(AB8:AD8)</f>
+        <v>0.99554945892394464</v>
+      </c>
+      <c r="AF8" s="35">
+        <f t="shared" ref="AF8" si="15">AVERAGE(AC8:AE8)</f>
+        <v>0.99955291368185739</v>
+      </c>
+      <c r="AG8" s="35">
+        <f t="shared" ref="AG8" si="16">AVERAGE(AD8:AF8)</f>
+        <v>1.0017815712374467</v>
+      </c>
+      <c r="AH8" s="35">
+        <f t="shared" ref="AH8" si="17">AVERAGE(AE8:AG8)</f>
+        <v>0.99896131461441617</v>
+      </c>
+    </row>
+    <row r="9" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B9" s="35" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C9" s="35">
         <v>5</v>
       </c>
       <c r="D9" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="E9" s="35">
         <v>5</v>
       </c>
       <c r="F9" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.5</v>
       </c>
       <c r="G9" s="35">
         <v>6.1</v>
       </c>
       <c r="H9" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.6</v>
       </c>
       <c r="I9" s="35">
         <v>6.8</v>
       </c>
       <c r="J9" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.2</v>
       </c>
       <c r="K9" s="35">
@@ -2556,7 +2796,10 @@
       <c r="M9" s="35">
         <v>7</v>
       </c>
-      <c r="N9" s="51"/>
+      <c r="N9" s="51">
+        <f>AVERAGE(K9:M9)</f>
+        <v>5.333333333333333</v>
+      </c>
       <c r="P9" s="36"/>
       <c r="T9" s="35">
         <v>10.5</v>
@@ -2570,56 +2813,103 @@
       <c r="W9" s="35">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X9" s="51">
+        <f t="shared" si="7"/>
+        <v>12.333333333333332</v>
+      </c>
+      <c r="Y9" s="35">
+        <f>AVERAGE(V9:X9)</f>
+        <v>10.777777777777777</v>
+      </c>
+      <c r="Z9" s="35">
+        <f t="shared" ref="Z9:AH9" si="18">AVERAGE(W9:Y9)</f>
+        <v>10.703703703703702</v>
+      </c>
+      <c r="AA9" s="35">
+        <f t="shared" si="18"/>
+        <v>11.271604938271603</v>
+      </c>
+      <c r="AB9" s="35">
+        <f t="shared" si="18"/>
+        <v>10.917695473251028</v>
+      </c>
+      <c r="AC9" s="35">
+        <f t="shared" si="18"/>
+        <v>10.964334705075444</v>
+      </c>
+      <c r="AD9" s="35">
+        <f t="shared" si="18"/>
+        <v>11.051211705532692</v>
+      </c>
+      <c r="AE9" s="35">
+        <f t="shared" si="18"/>
+        <v>10.977747294619723</v>
+      </c>
+      <c r="AF9" s="35">
+        <f t="shared" si="18"/>
+        <v>10.997764568409288</v>
+      </c>
+      <c r="AG9" s="35">
+        <f t="shared" si="18"/>
+        <v>11.008907856187236</v>
+      </c>
+      <c r="AH9" s="35">
+        <f t="shared" si="18"/>
+        <v>10.994806573072083</v>
+      </c>
+    </row>
+    <row r="10" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B10" s="35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C10" s="35">
-        <f t="shared" ref="C10:M10" si="5">C5+C6+C7+C8-C9</f>
+        <f t="shared" ref="C10:N10" si="19">C5+C6+C7+C8-C9</f>
         <v>76.8</v>
       </c>
       <c r="D10" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="19"/>
         <v>-76.8</v>
       </c>
       <c r="E10" s="35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="19"/>
         <v>94.5</v>
       </c>
       <c r="F10" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="19"/>
         <v>112.20000000000002</v>
       </c>
       <c r="G10" s="35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="19"/>
         <v>105.80000000000001</v>
       </c>
       <c r="H10" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="19"/>
         <v>118.30000000000003</v>
       </c>
       <c r="I10" s="35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="19"/>
         <v>96.3</v>
       </c>
       <c r="J10" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="19"/>
         <v>156.60000000000002</v>
       </c>
       <c r="K10" s="35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="19"/>
         <v>167.5</v>
       </c>
       <c r="L10" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="19"/>
         <v>136.89999999999998</v>
       </c>
       <c r="M10" s="35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="19"/>
         <v>145.5</v>
       </c>
-      <c r="N10" s="51"/>
+      <c r="N10" s="51">
+        <f t="shared" si="19"/>
+        <v>173.21003333333331</v>
+      </c>
       <c r="P10" s="36"/>
       <c r="T10" s="35">
         <f>T5+T6+T7+T8-T9</f>
@@ -2637,37 +2927,81 @@
         <f>W5+W6+W7+W8-W9</f>
         <v>304.39999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X10" s="51">
+        <f>X5+X6+X7+X8-X9</f>
+        <v>318.71003333333334</v>
+      </c>
+      <c r="Y10" s="35">
+        <f t="shared" ref="Y10:AH10" si="20">Y5+Y6+Y7+Y8-Y9</f>
+        <v>386.26448377777774</v>
+      </c>
+      <c r="Z10" s="35">
+        <f t="shared" si="20"/>
+        <v>457.61935011703702</v>
+      </c>
+      <c r="AA10" s="35">
+        <f t="shared" si="20"/>
+        <v>541.29384548378266</v>
+      </c>
+      <c r="AB10" s="35">
+        <f t="shared" si="20"/>
+        <v>640.84897635399102</v>
+      </c>
+      <c r="AC10" s="35">
+        <f t="shared" si="20"/>
+        <v>757.95262886039791</v>
+      </c>
+      <c r="AD10" s="35">
+        <f t="shared" si="20"/>
+        <v>896.10946465243455</v>
+      </c>
+      <c r="AE10" s="35">
+        <f t="shared" si="20"/>
+        <v>1059.2753143041996</v>
+      </c>
+      <c r="AF10" s="35">
+        <f t="shared" si="20"/>
+        <v>1251.7256526703491</v>
+      </c>
+      <c r="AG10" s="35">
+        <f t="shared" si="20"/>
+        <v>1478.8270336186406</v>
+      </c>
+      <c r="AH10" s="35">
+        <f t="shared" si="20"/>
+        <v>1746.8284634277791</v>
+      </c>
+    </row>
+    <row r="11" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B11" s="35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C11" s="35">
         <v>15.1</v>
       </c>
       <c r="D11" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-15.1</v>
       </c>
       <c r="E11" s="35">
         <v>19.899999999999999</v>
       </c>
       <c r="F11" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G11" s="35">
         <v>20.8</v>
       </c>
       <c r="H11" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.900000000000002</v>
       </c>
       <c r="I11" s="35">
         <v>19</v>
       </c>
       <c r="J11" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>30.6</v>
       </c>
       <c r="K11" s="35">
@@ -2680,7 +3014,10 @@
       <c r="M11" s="35">
         <v>30.7</v>
       </c>
-      <c r="N11" s="51"/>
+      <c r="N11" s="51">
+        <f>N10*N23</f>
+        <v>36.374106999999995</v>
+      </c>
       <c r="P11" s="36"/>
       <c r="T11" s="35">
         <v>36.9</v>
@@ -2694,56 +3031,103 @@
       <c r="W11" s="35">
         <v>60.2</v>
       </c>
-    </row>
-    <row r="12" spans="2:37" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X11" s="51">
+        <f>N11+M11</f>
+        <v>67.074106999999998</v>
+      </c>
+      <c r="Y11" s="35">
+        <f>Y10*Y23</f>
+        <v>81.115541593333319</v>
+      </c>
+      <c r="Z11" s="35">
+        <f t="shared" ref="Z11:AH11" si="21">Z10*Z23</f>
+        <v>96.100063524577763</v>
+      </c>
+      <c r="AA11" s="35">
+        <f t="shared" si="21"/>
+        <v>113.67170755159435</v>
+      </c>
+      <c r="AB11" s="35">
+        <f t="shared" si="21"/>
+        <v>134.57828503433811</v>
+      </c>
+      <c r="AC11" s="35">
+        <f t="shared" si="21"/>
+        <v>159.17005206068356</v>
+      </c>
+      <c r="AD11" s="35">
+        <f t="shared" si="21"/>
+        <v>188.18298757701126</v>
+      </c>
+      <c r="AE11" s="35">
+        <f t="shared" si="21"/>
+        <v>222.44781600388191</v>
+      </c>
+      <c r="AF11" s="35">
+        <f t="shared" si="21"/>
+        <v>262.8623870607733</v>
+      </c>
+      <c r="AG11" s="35">
+        <f t="shared" si="21"/>
+        <v>310.55367705991449</v>
+      </c>
+      <c r="AH11" s="35">
+        <f t="shared" si="21"/>
+        <v>366.83397731983359</v>
+      </c>
+    </row>
+    <row r="12" spans="2:73" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B12" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C12" s="33">
-        <f t="shared" ref="C12:M12" si="6">C10-C11</f>
+        <f t="shared" ref="C12:M12" si="22">C10-C11</f>
         <v>61.699999999999996</v>
       </c>
       <c r="D12" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>-61.699999999999996</v>
       </c>
       <c r="E12" s="33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>74.599999999999994</v>
       </c>
       <c r="F12" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>95.200000000000017</v>
       </c>
       <c r="G12" s="33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>85.000000000000014</v>
       </c>
       <c r="H12" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>99.40000000000002</v>
       </c>
       <c r="I12" s="33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>77.3</v>
       </c>
       <c r="J12" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>126.00000000000003</v>
       </c>
       <c r="K12" s="33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>135.69999999999999</v>
       </c>
       <c r="L12" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>108.49999999999997</v>
       </c>
       <c r="M12" s="33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="22"/>
         <v>114.8</v>
       </c>
-      <c r="N12" s="50"/>
+      <c r="N12" s="50">
+        <f>N10-N11</f>
+        <v>136.8359263333333</v>
+      </c>
       <c r="P12" s="34"/>
       <c r="T12" s="33">
         <f>T10-T11</f>
@@ -2761,56 +3145,259 @@
         <f>W10-W11</f>
         <v>244.2</v>
       </c>
-    </row>
-    <row r="13" spans="2:37" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X12" s="50">
+        <f t="shared" ref="X12:AH12" si="23">X10-X11</f>
+        <v>251.63592633333334</v>
+      </c>
+      <c r="Y12" s="33">
+        <f t="shared" si="23"/>
+        <v>305.14894218444442</v>
+      </c>
+      <c r="Z12" s="33">
+        <f t="shared" si="23"/>
+        <v>361.51928659245925</v>
+      </c>
+      <c r="AA12" s="33">
+        <f t="shared" si="23"/>
+        <v>427.62213793218831</v>
+      </c>
+      <c r="AB12" s="33">
+        <f t="shared" si="23"/>
+        <v>506.27069131965288</v>
+      </c>
+      <c r="AC12" s="33">
+        <f t="shared" si="23"/>
+        <v>598.78257679971432</v>
+      </c>
+      <c r="AD12" s="33">
+        <f t="shared" si="23"/>
+        <v>707.92647707542324</v>
+      </c>
+      <c r="AE12" s="33">
+        <f t="shared" si="23"/>
+        <v>836.82749830031764</v>
+      </c>
+      <c r="AF12" s="33">
+        <f t="shared" si="23"/>
+        <v>988.86326560957582</v>
+      </c>
+      <c r="AG12" s="33">
+        <f t="shared" si="23"/>
+        <v>1168.2733565587262</v>
+      </c>
+      <c r="AH12" s="33">
+        <f t="shared" si="23"/>
+        <v>1379.9944861079455</v>
+      </c>
+      <c r="AI12" s="33">
+        <f>AH12*(1+$AK$21)</f>
+        <v>1366.194541246866</v>
+      </c>
+      <c r="AJ12" s="33">
+        <f t="shared" ref="AJ12:BU12" si="24">AI12*(1+$AK$21)</f>
+        <v>1352.5325958343974</v>
+      </c>
+      <c r="AK12" s="33">
+        <f t="shared" si="24"/>
+        <v>1339.0072698760534</v>
+      </c>
+      <c r="AL12" s="33">
+        <f t="shared" si="24"/>
+        <v>1325.6171971772928</v>
+      </c>
+      <c r="AM12" s="33">
+        <f t="shared" si="24"/>
+        <v>1312.3610252055198</v>
+      </c>
+      <c r="AN12" s="33">
+        <f t="shared" si="24"/>
+        <v>1299.2374149534646</v>
+      </c>
+      <c r="AO12" s="33">
+        <f t="shared" si="24"/>
+        <v>1286.2450408039299</v>
+      </c>
+      <c r="AP12" s="33">
+        <f t="shared" si="24"/>
+        <v>1273.3825903958905</v>
+      </c>
+      <c r="AQ12" s="33">
+        <f t="shared" si="24"/>
+        <v>1260.6487644919316</v>
+      </c>
+      <c r="AR12" s="33">
+        <f t="shared" si="24"/>
+        <v>1248.0422768470123</v>
+      </c>
+      <c r="AS12" s="33">
+        <f t="shared" si="24"/>
+        <v>1235.5618540785422</v>
+      </c>
+      <c r="AT12" s="33">
+        <f t="shared" si="24"/>
+        <v>1223.2062355377568</v>
+      </c>
+      <c r="AU12" s="33">
+        <f t="shared" si="24"/>
+        <v>1210.9741731823792</v>
+      </c>
+      <c r="AV12" s="33">
+        <f t="shared" si="24"/>
+        <v>1198.8644314505555</v>
+      </c>
+      <c r="AW12" s="33">
+        <f t="shared" si="24"/>
+        <v>1186.8757871360499</v>
+      </c>
+      <c r="AX12" s="33">
+        <f t="shared" si="24"/>
+        <v>1175.0070292646894</v>
+      </c>
+      <c r="AY12" s="33">
+        <f t="shared" si="24"/>
+        <v>1163.2569589720426</v>
+      </c>
+      <c r="AZ12" s="33">
+        <f t="shared" si="24"/>
+        <v>1151.6243893823223</v>
+      </c>
+      <c r="BA12" s="33">
+        <f t="shared" si="24"/>
+        <v>1140.1081454884991</v>
+      </c>
+      <c r="BB12" s="33">
+        <f t="shared" si="24"/>
+        <v>1128.7070640336142</v>
+      </c>
+      <c r="BC12" s="33">
+        <f t="shared" si="24"/>
+        <v>1117.419993393278</v>
+      </c>
+      <c r="BD12" s="33">
+        <f t="shared" si="24"/>
+        <v>1106.2457934593451</v>
+      </c>
+      <c r="BE12" s="33">
+        <f t="shared" si="24"/>
+        <v>1095.1833355247516</v>
+      </c>
+      <c r="BF12" s="33">
+        <f t="shared" si="24"/>
+        <v>1084.231502169504</v>
+      </c>
+      <c r="BG12" s="33">
+        <f t="shared" si="24"/>
+        <v>1073.389187147809</v>
+      </c>
+      <c r="BH12" s="33">
+        <f t="shared" si="24"/>
+        <v>1062.6552952763309</v>
+      </c>
+      <c r="BI12" s="33">
+        <f t="shared" si="24"/>
+        <v>1052.0287423235675</v>
+      </c>
+      <c r="BJ12" s="33">
+        <f t="shared" si="24"/>
+        <v>1041.5084549003318</v>
+      </c>
+      <c r="BK12" s="33">
+        <f t="shared" si="24"/>
+        <v>1031.0933703513285</v>
+      </c>
+      <c r="BL12" s="33">
+        <f t="shared" si="24"/>
+        <v>1020.7824366478152</v>
+      </c>
+      <c r="BM12" s="33">
+        <f t="shared" si="24"/>
+        <v>1010.5746122813371</v>
+      </c>
+      <c r="BN12" s="33">
+        <f t="shared" si="24"/>
+        <v>1000.4688661585237</v>
+      </c>
+      <c r="BO12" s="33">
+        <f t="shared" si="24"/>
+        <v>990.46417749693853</v>
+      </c>
+      <c r="BP12" s="33">
+        <f t="shared" si="24"/>
+        <v>980.55953572196916</v>
+      </c>
+      <c r="BQ12" s="33">
+        <f t="shared" si="24"/>
+        <v>970.7539403647495</v>
+      </c>
+      <c r="BR12" s="33">
+        <f t="shared" si="24"/>
+        <v>961.04640096110199</v>
+      </c>
+      <c r="BS12" s="33">
+        <f t="shared" si="24"/>
+        <v>951.43593695149093</v>
+      </c>
+      <c r="BT12" s="33">
+        <f t="shared" si="24"/>
+        <v>941.92157758197607</v>
+      </c>
+      <c r="BU12" s="33">
+        <f t="shared" si="24"/>
+        <v>932.50236180615627</v>
+      </c>
+    </row>
+    <row r="13" spans="2:73" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B13" s="35" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C13" s="33">
-        <f t="shared" ref="C13:M13" si="7">C12+C14</f>
+        <f t="shared" ref="C13:N13" si="25">C12+C14</f>
         <v>61.699999999999996</v>
       </c>
       <c r="D13" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>-61.699999999999996</v>
       </c>
       <c r="E13" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>74.599999999999994</v>
       </c>
       <c r="F13" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>95.200000000000017</v>
       </c>
       <c r="G13" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>85.000000000000014</v>
       </c>
       <c r="H13" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>99.40000000000002</v>
       </c>
       <c r="I13" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>77.3</v>
       </c>
       <c r="J13" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>125.90000000000003</v>
       </c>
       <c r="K13" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>135.79999999999998</v>
       </c>
       <c r="L13" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>108.19999999999997</v>
       </c>
       <c r="M13" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>115</v>
       </c>
-      <c r="N13" s="50"/>
+      <c r="N13" s="50">
+        <f t="shared" si="25"/>
+        <v>136.97276225966664</v>
+      </c>
       <c r="P13" s="34"/>
       <c r="T13" s="33">
         <f>T12+T14</f>
@@ -2828,10 +3415,54 @@
         <f>W12+W14</f>
         <v>244</v>
       </c>
-    </row>
-    <row r="14" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X13" s="50">
+        <f t="shared" ref="X13" si="26">X12+X14</f>
+        <v>251.97276225966667</v>
+      </c>
+      <c r="Y13" s="33">
+        <f>Y12+Y14</f>
+        <v>305.18861154692843</v>
+      </c>
+      <c r="Z13" s="33">
+        <f t="shared" ref="Z13:AH13" si="27">Z12+Z14</f>
+        <v>361.56628409971626</v>
+      </c>
+      <c r="AA13" s="33">
+        <f t="shared" si="27"/>
+        <v>427.6777288101195</v>
+      </c>
+      <c r="AB13" s="33">
+        <f t="shared" si="27"/>
+        <v>506.33650650952444</v>
+      </c>
+      <c r="AC13" s="33">
+        <f t="shared" si="27"/>
+        <v>598.86041853469828</v>
+      </c>
+      <c r="AD13" s="33">
+        <f t="shared" si="27"/>
+        <v>708.01850751744303</v>
+      </c>
+      <c r="AE13" s="33">
+        <f t="shared" si="27"/>
+        <v>836.9362858750967</v>
+      </c>
+      <c r="AF13" s="33">
+        <f t="shared" si="27"/>
+        <v>988.99181783410506</v>
+      </c>
+      <c r="AG13" s="33">
+        <f t="shared" si="27"/>
+        <v>1168.4252320950789</v>
+      </c>
+      <c r="AH13" s="33">
+        <f t="shared" si="27"/>
+        <v>1380.1738853911395</v>
+      </c>
+    </row>
+    <row r="14" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="35" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C14" s="46">
         <v>0</v>
@@ -2851,7 +3482,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="36">
-        <f t="shared" ref="H14" si="8">U14-G14</f>
+        <f t="shared" ref="H14" si="28">U14-G14</f>
         <v>0</v>
       </c>
       <c r="I14" s="46">
@@ -2871,7 +3502,10 @@
       <c r="M14" s="35">
         <v>0.2</v>
       </c>
-      <c r="N14" s="51"/>
+      <c r="N14" s="51">
+        <f>N12*0.001</f>
+        <v>0.1368359263333333</v>
+      </c>
       <c r="P14" s="36"/>
       <c r="S14" s="35">
         <v>0</v>
@@ -2888,63 +3522,110 @@
       <c r="W14" s="35">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="15" spans="2:37" s="37" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X14" s="51">
+        <f>N14+M14</f>
+        <v>0.33683592633333331</v>
+      </c>
+      <c r="Y14" s="35">
+        <f>Y12*0.00013</f>
+        <v>3.9669362483977774E-2</v>
+      </c>
+      <c r="Z14" s="35">
+        <f t="shared" ref="Z14:AH14" si="29">Z12*0.00013</f>
+        <v>4.6997507257019698E-2</v>
+      </c>
+      <c r="AA14" s="35">
+        <f t="shared" si="29"/>
+        <v>5.5590877931184474E-2</v>
+      </c>
+      <c r="AB14" s="35">
+        <f t="shared" si="29"/>
+        <v>6.5815189871554866E-2</v>
+      </c>
+      <c r="AC14" s="35">
+        <f t="shared" si="29"/>
+        <v>7.7841734983962851E-2</v>
+      </c>
+      <c r="AD14" s="35">
+        <f t="shared" si="29"/>
+        <v>9.2030442019805009E-2</v>
+      </c>
+      <c r="AE14" s="35">
+        <f t="shared" si="29"/>
+        <v>0.10878757477904129</v>
+      </c>
+      <c r="AF14" s="35">
+        <f t="shared" si="29"/>
+        <v>0.12855222452924484</v>
+      </c>
+      <c r="AG14" s="35">
+        <f t="shared" si="29"/>
+        <v>0.1518755363526344</v>
+      </c>
+      <c r="AH14" s="35">
+        <f t="shared" si="29"/>
+        <v>0.17939928319403289</v>
+      </c>
+    </row>
+    <row r="15" spans="2:73" s="37" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C15" s="37">
-        <f t="shared" ref="C15:M15" si="9">C12/C16</f>
+        <f t="shared" ref="C15:N15" si="30">C12/C16</f>
         <v>0.16270266756508422</v>
       </c>
       <c r="D15" s="38" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E15" s="37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0.19681108372907286</v>
       </c>
       <c r="F15" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0.25108149993397905</v>
       </c>
       <c r="G15" s="37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0.22419479233636896</v>
       </c>
       <c r="H15" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0.26220905435668357</v>
       </c>
       <c r="I15" s="37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0.20390802308932054</v>
       </c>
       <c r="J15" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0.33271719038817016</v>
       </c>
       <c r="K15" s="37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0.35795304668952777</v>
       </c>
       <c r="L15" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0.28650646950092412</v>
       </c>
       <c r="M15" s="37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0.30354309888947645</v>
       </c>
-      <c r="N15" s="52"/>
+      <c r="N15" s="52">
+        <f t="shared" si="30"/>
+        <v>0.36180837211352013</v>
+      </c>
       <c r="P15" s="38"/>
       <c r="T15" s="37">
-        <f t="shared" ref="T15:U15" si="10">T12/T16</f>
+        <f t="shared" ref="T15:U15" si="31">T12/T16</f>
         <v>0.44783233916795839</v>
       </c>
       <c r="U15" s="37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="31"/>
         <v>0.48643208876632238</v>
       </c>
       <c r="V15" s="37">
@@ -2955,8 +3636,52 @@
         <f>W12/W16</f>
         <v>0.6448376023237391</v>
       </c>
-    </row>
-    <row r="16" spans="2:37" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X15" s="52">
+        <f>X13/X16</f>
+        <v>0.66624210010488283</v>
+      </c>
+      <c r="Y15" s="37">
+        <f>Y13/Y16</f>
+        <v>0.80695032138267697</v>
+      </c>
+      <c r="Z15" s="37">
+        <f t="shared" ref="Z15:AH15" si="32">Z13/Z16</f>
+        <v>0.95601873109390867</v>
+      </c>
+      <c r="AA15" s="37">
+        <f t="shared" si="32"/>
+        <v>1.1308242432842928</v>
+      </c>
+      <c r="AB15" s="37">
+        <f t="shared" si="32"/>
+        <v>1.3388062044143958</v>
+      </c>
+      <c r="AC15" s="37">
+        <f t="shared" si="32"/>
+        <v>1.5834490178072405</v>
+      </c>
+      <c r="AD15" s="37">
+        <f t="shared" si="32"/>
+        <v>1.8720743191894316</v>
+      </c>
+      <c r="AE15" s="37">
+        <f t="shared" si="32"/>
+        <v>2.21294628734822</v>
+      </c>
+      <c r="AF15" s="37">
+        <f t="shared" si="32"/>
+        <v>2.6149968742308438</v>
+      </c>
+      <c r="AG15" s="37">
+        <f t="shared" si="32"/>
+        <v>3.0894374196062371</v>
+      </c>
+      <c r="AH15" s="37">
+        <f t="shared" si="32"/>
+        <v>3.6493228064281849</v>
+      </c>
+    </row>
+    <row r="16" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="35" t="s">
         <v>5</v>
       </c>
@@ -2998,7 +3723,10 @@
       <c r="M16" s="35">
         <v>378.2</v>
       </c>
-      <c r="N16" s="51"/>
+      <c r="N16" s="51">
+        <f>M16</f>
+        <v>378.2</v>
+      </c>
       <c r="P16" s="36"/>
       <c r="T16" s="35">
         <v>379.15975500000002</v>
@@ -3012,10 +3740,54 @@
       <c r="W16" s="35">
         <v>378.7</v>
       </c>
-    </row>
-    <row r="18" spans="2:23" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X16" s="51">
+        <f>N16</f>
+        <v>378.2</v>
+      </c>
+      <c r="Y16" s="35">
+        <f>X16</f>
+        <v>378.2</v>
+      </c>
+      <c r="Z16" s="35">
+        <f t="shared" ref="Z16:AH16" si="33">Y16</f>
+        <v>378.2</v>
+      </c>
+      <c r="AA16" s="35">
+        <f t="shared" si="33"/>
+        <v>378.2</v>
+      </c>
+      <c r="AB16" s="35">
+        <f t="shared" si="33"/>
+        <v>378.2</v>
+      </c>
+      <c r="AC16" s="35">
+        <f t="shared" si="33"/>
+        <v>378.2</v>
+      </c>
+      <c r="AD16" s="35">
+        <f t="shared" si="33"/>
+        <v>378.2</v>
+      </c>
+      <c r="AE16" s="35">
+        <f t="shared" si="33"/>
+        <v>378.2</v>
+      </c>
+      <c r="AF16" s="35">
+        <f t="shared" si="33"/>
+        <v>378.2</v>
+      </c>
+      <c r="AG16" s="35">
+        <f t="shared" si="33"/>
+        <v>378.2</v>
+      </c>
+      <c r="AH16" s="35">
+        <f t="shared" si="33"/>
+        <v>378.2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:37" s="41" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D18" s="42"/>
       <c r="E18" s="41">
@@ -3048,21 +3820,55 @@
       <c r="N18" s="53"/>
       <c r="P18" s="42"/>
       <c r="U18" s="41">
-        <f t="shared" ref="U18:V18" si="11">U4/T4-1</f>
+        <f t="shared" ref="U18:V18" si="34">U4/T4-1</f>
         <v>0.10529358328515981</v>
       </c>
       <c r="V18" s="41">
-        <f t="shared" si="11"/>
+        <f t="shared" si="34"/>
         <v>-1.5092647937836268E-2</v>
       </c>
       <c r="W18" s="41">
         <f>W4/V4-1</f>
         <v>0.15710817781823683</v>
       </c>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="X18" s="53">
+        <f>X4/W4-1</f>
+        <v>0.22258899888546524</v>
+      </c>
+      <c r="Y18" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="Z18" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="AA18" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="AB18" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="AC18" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="AD18" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="AE18" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="AF18" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="AG18" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="AH18" s="41">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J19" s="40">
         <f>J4/I4-1</f>
@@ -3081,28 +3887,27 @@
         <v>0.11089963202639264</v>
       </c>
       <c r="N19" s="54">
-        <f>N4/M4-1</f>
-        <v>-1</v>
+        <v>0.13</v>
       </c>
       <c r="S19" s="57" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="T19" s="57" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="U19" s="57" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="V19" s="57" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="W19" s="57" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="2:23" s="39" customFormat="1" x14ac:dyDescent="0.15">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="2:37" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B21" s="39" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C21" s="39">
         <f>C5/C4</f>
@@ -3142,25 +3947,75 @@
       <c r="N21" s="54"/>
       <c r="P21" s="40"/>
       <c r="T21" s="39">
-        <f t="shared" ref="T21" si="12">T5/T4</f>
+        <f t="shared" ref="T21" si="35">T5/T4</f>
         <v>0.17986621521182591</v>
       </c>
       <c r="U21" s="39">
-        <f t="shared" ref="U21:V21" si="13">U5/U4</f>
+        <f t="shared" ref="U21" si="36">U5/U4</f>
         <v>0.17438732815301852</v>
       </c>
       <c r="V21" s="39">
-        <f t="shared" ref="V21:W21" si="14">V5/V4</f>
+        <f t="shared" ref="V21:W21" si="37">V5/V4</f>
         <v>0.18267334243665606</v>
       </c>
       <c r="W21" s="39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="37"/>
         <v>0.18284927555235034</v>
       </c>
-    </row>
-    <row r="22" spans="2:23" s="39" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X21" s="54">
+        <f t="shared" ref="X21:AH21" si="38">X5/X4</f>
+        <v>0.1768415097476157</v>
+      </c>
+      <c r="Y21" s="39">
+        <f t="shared" si="38"/>
+        <v>0.18</v>
+      </c>
+      <c r="Z21" s="39">
+        <f t="shared" si="38"/>
+        <v>0.18</v>
+      </c>
+      <c r="AA21" s="39">
+        <f t="shared" si="38"/>
+        <v>0.18</v>
+      </c>
+      <c r="AB21" s="39">
+        <f t="shared" si="38"/>
+        <v>0.18</v>
+      </c>
+      <c r="AC21" s="39">
+        <f t="shared" si="38"/>
+        <v>0.18</v>
+      </c>
+      <c r="AD21" s="39">
+        <f t="shared" si="38"/>
+        <v>0.18</v>
+      </c>
+      <c r="AE21" s="39">
+        <f t="shared" si="38"/>
+        <v>0.17999999999999997</v>
+      </c>
+      <c r="AF21" s="39">
+        <f t="shared" si="38"/>
+        <v>0.18</v>
+      </c>
+      <c r="AG21" s="39">
+        <f t="shared" si="38"/>
+        <v>0.18</v>
+      </c>
+      <c r="AH21" s="39">
+        <f t="shared" si="38"/>
+        <v>0.18</v>
+      </c>
+      <c r="AJ21" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK21" s="78">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="2:37" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C22" s="39">
         <f>C12/C4</f>
@@ -3200,25 +4055,75 @@
       <c r="N22" s="54"/>
       <c r="P22" s="40"/>
       <c r="T22" s="39">
-        <f t="shared" ref="T22" si="15">T12/T4</f>
+        <f t="shared" ref="T22" si="39">T12/T4</f>
         <v>0.14022627797505988</v>
       </c>
       <c r="U22" s="39">
-        <f t="shared" ref="U22:V22" si="16">U12/U4</f>
+        <f t="shared" ref="U22" si="40">U12/U4</f>
         <v>0.13777644949193069</v>
       </c>
       <c r="V22" s="39">
-        <f t="shared" ref="V22:W22" si="17">V12/V4</f>
+        <f t="shared" ref="V22:W22" si="41">V12/V4</f>
         <v>0.1542254589591868</v>
       </c>
       <c r="W22" s="39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="41"/>
         <v>0.16009965252737166</v>
       </c>
-    </row>
-    <row r="23" spans="2:23" s="39" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X22" s="54">
+        <f t="shared" ref="X22:AH22" si="42">X12/X4</f>
+        <v>0.13493881502097169</v>
+      </c>
+      <c r="Y22" s="39">
+        <f t="shared" si="42"/>
+        <v>0.13867370139203813</v>
+      </c>
+      <c r="Z22" s="39">
+        <f t="shared" si="42"/>
+        <v>0.13922964084330744</v>
+      </c>
+      <c r="AA22" s="39">
+        <f t="shared" si="42"/>
+        <v>0.13956560569635687</v>
+      </c>
+      <c r="AB22" s="39">
+        <f t="shared" si="42"/>
+        <v>0.14002932751943725</v>
+      </c>
+      <c r="AC22" s="39">
+        <f t="shared" si="42"/>
+        <v>0.14035353793131092</v>
+      </c>
+      <c r="AD22" s="39">
+        <f t="shared" si="42"/>
+        <v>0.14062429491834813</v>
+      </c>
+      <c r="AE22" s="39">
+        <f t="shared" si="42"/>
+        <v>0.14087247270548028</v>
+      </c>
+      <c r="AF22" s="39">
+        <f t="shared" si="42"/>
+        <v>0.14107317206442571</v>
+      </c>
+      <c r="AG22" s="39">
+        <f t="shared" si="42"/>
+        <v>0.14124420962653625</v>
+      </c>
+      <c r="AH22" s="39">
+        <f t="shared" si="42"/>
+        <v>0.14139092126132088</v>
+      </c>
+      <c r="AJ22" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK22" s="79">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="23" spans="2:37" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B23" s="39" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C23" s="39">
         <f>C11/C10</f>
@@ -3255,33 +4160,110 @@
         <f>M11/M10</f>
         <v>0.21099656357388316</v>
       </c>
-      <c r="N23" s="54"/>
+      <c r="N23" s="54">
+        <v>0.21</v>
+      </c>
       <c r="P23" s="40"/>
       <c r="T23" s="39">
-        <f t="shared" ref="T23" si="18">T11/T10</f>
+        <f t="shared" ref="T23" si="43">T11/T10</f>
         <v>0.17851959361393321</v>
       </c>
       <c r="U23" s="39">
-        <f t="shared" ref="U23:V23" si="19">U11/U10</f>
+        <f t="shared" ref="U23" si="44">U11/U10</f>
         <v>0.17715305667112896</v>
       </c>
       <c r="V23" s="39">
-        <f t="shared" ref="V23:W23" si="20">V11/V10</f>
+        <f t="shared" ref="V23:W23" si="45">V11/V10</f>
         <v>0.19612495057334914</v>
       </c>
       <c r="W23" s="39">
-        <f t="shared" si="20"/>
+        <f t="shared" si="45"/>
         <v>0.19776609724047309</v>
       </c>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="X23" s="54">
+        <f t="shared" ref="X23" si="46">X11/X10</f>
+        <v>0.21045495900610178</v>
+      </c>
+      <c r="Y23" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="Z23" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="AA23" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="AB23" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="AC23" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="AD23" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="AE23" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="AF23" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="AG23" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="AH23" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="AJ23" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK23" s="80">
+        <f>NPV(AK22,X12:BU12)</f>
+        <v>10602.370197716416</v>
+      </c>
+    </row>
+    <row r="24" spans="2:37" x14ac:dyDescent="0.15">
+      <c r="AJ24" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK24" s="13">
+        <f>Main!C11</f>
+        <v>-567.6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:37" x14ac:dyDescent="0.15">
+      <c r="AJ25" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="AK25" s="81">
+        <f>AK23+AK24</f>
+        <v>10034.770197716416</v>
+      </c>
+    </row>
+    <row r="26" spans="2:37" x14ac:dyDescent="0.15">
+      <c r="AJ26" s="76" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK26" s="82">
+        <f>AK25/Main!C7</f>
+        <v>26.532972495284021</v>
+      </c>
+    </row>
+    <row r="27" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B27" s="43" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.15">
+        <v>76</v>
+      </c>
+      <c r="AJ27" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK27" s="13">
+        <f>Main!C6</f>
+        <v>22.55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C28" s="1">
         <f>216.4+586.8</f>
@@ -3324,10 +4306,17 @@
         <f>908.7+325.2</f>
         <v>1233.9000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="AJ28" s="77" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK28" s="83">
+        <f>AK26/AK27-1</f>
+        <v>0.17662849203033359</v>
+      </c>
+    </row>
+    <row r="29" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C29" s="1">
         <v>102.6</v>
@@ -3363,9 +4352,9 @@
         <v>194</v>
       </c>
     </row>
-    <row r="30" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:37" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B30" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C30" s="2">
         <v>3.4</v>
@@ -3390,7 +4379,7 @@
         <v>9.9</v>
       </c>
       <c r="L30" s="36">
-        <f t="shared" ref="L30:L37" si="21">W30</f>
+        <f t="shared" ref="L30:L37" si="47">W30</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="M30" s="33">
@@ -3404,10 +4393,11 @@
       <c r="W30" s="33">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="X30" s="56"/>
+    </row>
+    <row r="31" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
@@ -3423,14 +4413,14 @@
         <v>0</v>
       </c>
       <c r="J31" s="36">
-        <f t="shared" ref="J31:J33" si="22">V31</f>
+        <f t="shared" ref="J31:J33" si="48">V31</f>
         <v>0</v>
       </c>
       <c r="K31" s="35">
         <v>4.8</v>
       </c>
       <c r="L31" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="47"/>
         <v>31.1</v>
       </c>
       <c r="M31" s="35">
@@ -3443,9 +4433,9 @@
         <v>31.1</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
@@ -3461,14 +4451,14 @@
         <v>0</v>
       </c>
       <c r="J32" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="48"/>
         <v>13.9</v>
       </c>
       <c r="K32" s="35">
         <v>14.7</v>
       </c>
       <c r="L32" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="47"/>
         <v>14.7</v>
       </c>
       <c r="M32" s="35">
@@ -3481,9 +4471,9 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C33" s="1">
         <v>55.3</v>
@@ -3499,14 +4489,14 @@
         <v>5.6</v>
       </c>
       <c r="J33" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="48"/>
         <v>1.3</v>
       </c>
       <c r="K33" s="35">
         <v>1.9</v>
       </c>
       <c r="L33" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="47"/>
         <v>2.4</v>
       </c>
       <c r="M33" s="35">
@@ -3519,9 +4509,9 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C34" s="35">
         <f>SUM(C28:C33)</f>
@@ -3565,9 +4555,9 @@
         <v>1484.3000000000002</v>
       </c>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C35" s="1">
         <v>124.2</v>
@@ -3583,14 +4573,14 @@
         <v>175.8</v>
       </c>
       <c r="J35" s="36">
-        <f t="shared" ref="J35:J37" si="23">V35</f>
+        <f t="shared" ref="J35:J37" si="49">V35</f>
         <v>167.8</v>
       </c>
       <c r="K35" s="35">
         <v>193.2</v>
       </c>
       <c r="L35" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="47"/>
         <v>228.8</v>
       </c>
       <c r="M35" s="35">
@@ -3603,9 +4593,9 @@
         <v>228.8</v>
       </c>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C36" s="1">
         <v>203.4</v>
@@ -3621,14 +4611,14 @@
         <v>245.3</v>
       </c>
       <c r="J36" s="36">
-        <f t="shared" si="23"/>
+        <f t="shared" si="49"/>
         <v>268</v>
       </c>
       <c r="K36" s="35">
         <v>279.2</v>
       </c>
       <c r="L36" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="47"/>
         <v>325.10000000000002</v>
       </c>
       <c r="M36" s="35">
@@ -3641,9 +4631,9 @@
         <v>325.10000000000002</v>
       </c>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C37" s="1">
         <v>0.4</v>
@@ -3659,14 +4649,14 @@
         <v>6.5</v>
       </c>
       <c r="J37" s="36">
-        <f t="shared" si="23"/>
+        <f t="shared" si="49"/>
         <v>2.5</v>
       </c>
       <c r="K37" s="35">
         <v>4.4000000000000004</v>
       </c>
       <c r="L37" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="47"/>
         <v>0.7</v>
       </c>
       <c r="M37" s="35">
@@ -3679,9 +4669,9 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="38" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B38" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C38" s="2">
         <v>71.7</v>
@@ -3699,7 +4689,7 @@
         <v>125.5</v>
       </c>
       <c r="J38" s="34">
-        <f t="shared" ref="J38:J39" si="24">V38</f>
+        <f t="shared" ref="J38:J39" si="50">V38</f>
         <v>134.1</v>
       </c>
       <c r="K38" s="33">
@@ -3720,10 +4710,11 @@
       <c r="W38" s="33">
         <v>157.4</v>
       </c>
-    </row>
-    <row r="39" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="X38" s="56"/>
+    </row>
+    <row r="39" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B39" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C39" s="2">
         <v>0.6</v>
@@ -3741,7 +4732,7 @@
         <v>0.4</v>
       </c>
       <c r="J39" s="34">
-        <f t="shared" si="24"/>
+        <f t="shared" si="50"/>
         <v>1.7</v>
       </c>
       <c r="K39" s="33">
@@ -3762,10 +4753,11 @@
       <c r="W39" s="33">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="X39" s="56"/>
+    </row>
+    <row r="40" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C40" s="35">
         <f>SUM(C35:C39)+C34</f>
@@ -3809,7 +4801,7 @@
         <v>2197.0000000000005</v>
       </c>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:24" x14ac:dyDescent="0.15">
       <c r="G41" s="35"/>
       <c r="H41" s="36"/>
       <c r="I41" s="35"/>
@@ -3818,9 +4810,9 @@
       <c r="V41" s="35"/>
       <c r="W41" s="35"/>
     </row>
-    <row r="42" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B42" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C42" s="33">
         <v>0.2</v>
@@ -3859,10 +4851,11 @@
       <c r="W42" s="33">
         <v>72.5</v>
       </c>
-    </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="X42" s="56"/>
+    </row>
+    <row r="43" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C43" s="35">
         <v>0</v>
@@ -3887,7 +4880,7 @@
         <v>3</v>
       </c>
       <c r="L43" s="36">
-        <f t="shared" ref="L43:L47" si="25">W43</f>
+        <f t="shared" ref="L43:L47" si="51">W43</f>
         <v>15.5</v>
       </c>
       <c r="M43" s="35">
@@ -3900,9 +4893,9 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C44" s="35">
         <v>0</v>
@@ -3920,14 +4913,14 @@
         <v>0</v>
       </c>
       <c r="J44" s="36">
-        <f t="shared" ref="J44:J47" si="26">V44</f>
+        <f t="shared" ref="J44:J47" si="52">V44</f>
         <v>0</v>
       </c>
       <c r="K44" s="35">
         <v>14.2</v>
       </c>
       <c r="L44" s="36">
-        <f t="shared" si="25"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="M44" s="35">
@@ -3940,9 +4933,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C45" s="35">
         <v>125.7</v>
@@ -3960,14 +4953,14 @@
         <v>158.69999999999999</v>
       </c>
       <c r="J45" s="36">
-        <f t="shared" si="26"/>
+        <f t="shared" si="52"/>
         <v>186.7</v>
       </c>
       <c r="K45" s="35">
         <v>22</v>
       </c>
       <c r="L45" s="36">
-        <f t="shared" si="25"/>
+        <f t="shared" si="51"/>
         <v>242.7</v>
       </c>
       <c r="M45" s="35">
@@ -3980,9 +4973,9 @@
         <v>242.7</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C46" s="35">
         <v>4.7</v>
@@ -4000,14 +4993,14 @@
         <v>30.5</v>
       </c>
       <c r="J46" s="36">
-        <f t="shared" si="26"/>
+        <f t="shared" si="52"/>
         <v>35.4</v>
       </c>
       <c r="K46" s="35">
         <v>13.8</v>
       </c>
       <c r="L46" s="36">
-        <f t="shared" si="25"/>
+        <f t="shared" si="51"/>
         <v>20.7</v>
       </c>
       <c r="M46" s="35">
@@ -4020,9 +5013,9 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C47" s="35">
         <v>14.9</v>
@@ -4040,14 +5033,14 @@
         <v>11.3</v>
       </c>
       <c r="J47" s="36">
-        <f t="shared" si="26"/>
+        <f t="shared" si="52"/>
         <v>8.9</v>
       </c>
       <c r="K47" s="35">
         <v>0.2</v>
       </c>
       <c r="L47" s="36">
-        <f t="shared" si="25"/>
+        <f t="shared" si="51"/>
         <v>11.6</v>
       </c>
       <c r="M47" s="35">
@@ -4060,9 +5053,9 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="48" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B48" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C48" s="33">
         <v>0.4</v>
@@ -4101,10 +5094,11 @@
       <c r="W48" s="33">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="X48" s="56"/>
+    </row>
+    <row r="49" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C49" s="35">
         <f>SUM(C42:C48)</f>
@@ -4142,17 +5136,17 @@
         <v>400.29999999999995</v>
       </c>
       <c r="V49" s="35">
-        <f t="shared" ref="V49:W49" si="27">SUM(V42:V48)</f>
+        <f t="shared" ref="V49:W49" si="53">SUM(V42:V48)</f>
         <v>248</v>
       </c>
       <c r="W49" s="35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="53"/>
         <v>363.9</v>
       </c>
     </row>
-    <row r="50" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B50" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C50" s="33">
         <v>252.5</v>
@@ -4191,10 +5185,11 @@
       <c r="W50" s="33">
         <v>287.60000000000002</v>
       </c>
-    </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="X50" s="56"/>
+    </row>
+    <row r="51" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C51" s="35">
         <v>0</v>
@@ -4212,14 +5207,14 @@
         <v>51.4</v>
       </c>
       <c r="J51" s="36">
-        <f t="shared" ref="J51:J55" si="28">V51</f>
+        <f t="shared" ref="J51:J55" si="54">V51</f>
         <v>51.7</v>
       </c>
       <c r="K51" s="35">
         <v>53.4</v>
       </c>
       <c r="L51" s="36">
-        <f t="shared" ref="L51:L55" si="29">W51</f>
+        <f t="shared" ref="L51:L55" si="55">W51</f>
         <v>56.6</v>
       </c>
       <c r="M51" s="35">
@@ -4232,9 +5227,9 @@
         <v>56.6</v>
       </c>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C52" s="35">
         <v>66.8</v>
@@ -4252,14 +5247,14 @@
         <v>45</v>
       </c>
       <c r="J52" s="36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="54"/>
         <v>22.5</v>
       </c>
       <c r="K52" s="35">
         <v>10.1</v>
       </c>
       <c r="L52" s="36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="55"/>
         <v>0.6</v>
       </c>
       <c r="M52" s="35">
@@ -4272,9 +5267,9 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C53" s="35">
         <v>11.4</v>
@@ -4292,14 +5287,14 @@
         <v>16.3</v>
       </c>
       <c r="J53" s="36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="54"/>
         <v>16.8</v>
       </c>
       <c r="K53" s="35">
         <v>15.2</v>
       </c>
       <c r="L53" s="36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="55"/>
         <v>19</v>
       </c>
       <c r="M53" s="35">
@@ -4312,9 +5307,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C54" s="35">
         <v>16.899999999999999</v>
@@ -4332,14 +5327,14 @@
         <v>14.3</v>
       </c>
       <c r="J54" s="36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="54"/>
         <v>8.4</v>
       </c>
       <c r="K54" s="35">
         <v>6.3</v>
       </c>
       <c r="L54" s="36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="55"/>
         <v>7.7</v>
       </c>
       <c r="M54" s="35">
@@ -4352,9 +5347,9 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B55" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C55" s="35">
         <v>96</v>
@@ -4372,14 +5367,14 @@
         <v>41.7</v>
       </c>
       <c r="J55" s="36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="54"/>
         <v>40.6</v>
       </c>
       <c r="K55" s="35">
         <v>51.1</v>
       </c>
       <c r="L55" s="36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="55"/>
         <v>58.5</v>
       </c>
       <c r="M55" s="35">
@@ -4392,9 +5387,9 @@
         <v>58.5</v>
       </c>
     </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C56" s="35">
         <f>C49+SUM(C50:C55)</f>
@@ -4440,12 +5435,12 @@
         <v>793.90000000000009</v>
       </c>
     </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:24" x14ac:dyDescent="0.15">
       <c r="M57" s="35"/>
     </row>
-    <row r="58" spans="2:23" s="35" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:24" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B58" s="35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C58" s="35">
         <v>775.3</v>
@@ -4484,10 +5479,11 @@
       <c r="W58" s="35">
         <v>1403.1</v>
       </c>
-    </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="X58" s="51"/>
+    </row>
+    <row r="59" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C59" s="35">
         <f>C58+C56</f>
@@ -4530,9 +5526,9 @@
         <v>2197</v>
       </c>
     </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B61" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C61" s="35">
         <f>C40-C56</f>
@@ -4567,17 +5563,17 @@
         <v>1627</v>
       </c>
       <c r="V61" s="35">
-        <f t="shared" ref="V61:W61" si="30">V40-V56</f>
+        <f t="shared" ref="V61:W61" si="56">V40-V56</f>
         <v>1167.6000000000001</v>
       </c>
       <c r="W61" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="56"/>
         <v>1403.1000000000004</v>
       </c>
     </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C62" s="1">
         <f>C61/C16</f>
@@ -4612,15 +5608,15 @@
         <v>4.3019566367001589</v>
       </c>
       <c r="V62" s="1">
-        <f t="shared" ref="V62:W62" si="31">V61/V16</f>
+        <f t="shared" ref="V62:W62" si="57">V61/V16</f>
         <v>3.0791139240506333</v>
       </c>
       <c r="W62" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="57"/>
         <v>3.7050435701082662</v>
       </c>
     </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B64" s="1" t="s">
         <v>7</v>
       </c>
@@ -4665,7 +5661,7 @@
         <v>166.29999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B65" s="1" t="s">
         <v>8</v>
       </c>
@@ -4710,7 +5706,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B66" s="1" t="s">
         <v>9</v>
       </c>
@@ -4755,9 +5751,9 @@
         <v>-194.70000000000002</v>
       </c>
     </row>
-    <row r="68" spans="1:23" s="37" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:24" s="37" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B68" s="37" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C68" s="37">
         <v>10.8497</v>
@@ -4802,8 +5798,9 @@
       <c r="W68" s="37">
         <v>24.9636</v>
       </c>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="X68" s="52"/>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B69" s="1" t="s">
         <v>6</v>
       </c>
@@ -4824,7 +5821,7 @@
         <v>8761.9267890080991</v>
       </c>
       <c r="J69" s="36">
-        <f t="shared" ref="J69:L69" si="32">J68*J16</f>
+        <f t="shared" ref="J69:L69" si="58">J68*J16</f>
         <v>8886.2333699999999</v>
       </c>
       <c r="K69" s="35">
@@ -4832,7 +5829,7 @@
         <v>10690.468360000001</v>
       </c>
       <c r="L69" s="36">
-        <f t="shared" si="32"/>
+        <f t="shared" si="58"/>
         <v>9453.7153199999993</v>
       </c>
       <c r="M69" s="35">
@@ -4840,23 +5837,23 @@
         <v>7734.19</v>
       </c>
       <c r="T69" s="35">
-        <f t="shared" ref="T69:W69" si="33">T68*T16</f>
+        <f t="shared" ref="T69:W69" si="59">T68*T16</f>
         <v>6172.4174835960002</v>
       </c>
       <c r="U69" s="35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="59"/>
         <v>7145.9384367832008</v>
       </c>
       <c r="V69" s="35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="59"/>
         <v>8897.9659199999987</v>
       </c>
       <c r="W69" s="35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="59"/>
         <v>9453.7153199999993</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B70" s="1" t="s">
         <v>10</v>
       </c>
@@ -4877,7 +5874,7 @@
         <v>9008.2267890080984</v>
       </c>
       <c r="J70" s="36">
-        <f t="shared" ref="J70:L70" si="34">J69-J66</f>
+        <f t="shared" ref="J70:L70" si="60">J69-J66</f>
         <v>9067.1333699999996</v>
       </c>
       <c r="K70" s="35">
@@ -4885,7 +5882,7 @@
         <v>11095.668360000001</v>
       </c>
       <c r="L70" s="36">
-        <f t="shared" si="34"/>
+        <f t="shared" si="60"/>
         <v>9648.4153200000001</v>
       </c>
       <c r="M70" s="35">
@@ -4893,25 +5890,25 @@
         <v>8301.7899999999991</v>
       </c>
       <c r="T70" s="35">
-        <f t="shared" ref="T70:W70" si="35">T69-T66</f>
+        <f t="shared" ref="T70:W70" si="61">T69-T66</f>
         <v>6172.4174835960002</v>
       </c>
       <c r="U70" s="35">
-        <f t="shared" si="35"/>
+        <f t="shared" si="61"/>
         <v>7145.9384367832008</v>
       </c>
       <c r="V70" s="35">
-        <f t="shared" si="35"/>
+        <f t="shared" si="61"/>
         <v>9078.8659199999984</v>
       </c>
       <c r="W70" s="35">
-        <f t="shared" si="35"/>
+        <f t="shared" si="61"/>
         <v>9648.4153200000001</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A72" s="47">
-        <f>AVERAGE(C72:BA72)</f>
+        <f>AVERAGE(C72:AX72)</f>
         <v>6.6455994380078121</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -4942,7 +5939,7 @@
         <v>4.7536508912108166</v>
       </c>
       <c r="V72" s="44">
-        <f t="shared" ref="V72:W72" si="36">V68/V62</f>
+        <f t="shared" ref="V72" si="62">V68/V62</f>
         <v>7.620731346351489</v>
       </c>
       <c r="W72" s="44">
@@ -4950,7 +5947,11 @@
         <v>6.7377345306820589</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A73" s="47">
+        <f>AVERAGE(C73:AX73)</f>
+        <v>6.1262344816301137</v>
+      </c>
       <c r="B73" s="1" t="s">
         <v>23</v>
       </c>
@@ -4975,15 +5976,15 @@
         <v>4.6490682856455878</v>
       </c>
       <c r="T73" s="44">
-        <f t="shared" ref="T73:W73" si="37">T69/T4</f>
+        <f t="shared" ref="T73:V73" si="63">T69/T4</f>
         <v>5.0973800343513087</v>
       </c>
       <c r="U73" s="44">
-        <f t="shared" si="37"/>
+        <f t="shared" si="63"/>
         <v>5.3391650005851767</v>
       </c>
       <c r="V73" s="44">
-        <f t="shared" si="37"/>
+        <f t="shared" si="63"/>
         <v>6.7500879380974039</v>
       </c>
       <c r="W73" s="44">
@@ -4991,12 +5992,16 @@
         <v>6.1979383203304268</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B74" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A75" s="47">
+        <f>AVERAGE(C75:AX75)</f>
+        <v>40.569058563096945</v>
+      </c>
       <c r="B75" s="1" t="s">
         <v>25</v>
       </c>
@@ -5027,15 +6032,15 @@
         <v>34.65810517544427</v>
       </c>
       <c r="T75" s="44">
-        <f t="shared" ref="T75:W75" si="38">T68/T15</f>
+        <f t="shared" ref="T75:V75" si="64">T68/T15</f>
         <v>36.35110414367491</v>
       </c>
       <c r="U75" s="44">
-        <f t="shared" si="38"/>
+        <f t="shared" si="64"/>
         <v>38.752377639822122</v>
       </c>
       <c r="V75" s="44">
-        <f t="shared" si="38"/>
+        <f t="shared" si="64"/>
         <v>43.767663157894724</v>
       </c>
       <c r="W75" s="44">
@@ -5043,13 +6048,13 @@
         <v>38.713002948402945</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B76" s="1" t="s">
         <v>26</v>
       </c>
       <c r="M76" s="39"/>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B77" s="1" t="s">
         <v>27</v>
       </c>
@@ -5077,7 +6082,7 @@
         <v>0.12516018795386588</v>
       </c>
       <c r="V77" s="39">
-        <f t="shared" ref="V77:W77" si="39">V5/(V40-V49)</f>
+        <f t="shared" ref="V77" si="65">V5/(V40-V49)</f>
         <v>0.14773912509969936</v>
       </c>
       <c r="W77" s="39">
@@ -5096,7 +6101,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
   <ignoredErrors>
-    <ignoredError sqref="L10 L34 L49 J10 H10:H15 J34 J49" formula="1"/>
+    <ignoredError sqref="L10 L34 L49 J10 H10:H15 J34 J49 X10" formula="1"/>
     <ignoredError sqref="D11:F15 E10" evalError="1"/>
     <ignoredError sqref="F10 D10" evalError="1" formula="1"/>
   </ignoredErrors>

</xml_diff>